<commit_message>
Fix bug features 1
Still need to update the update 2
</commit_message>
<xml_diff>
--- a/train/grostest.xlsx
+++ b/train/grostest.xlsx
@@ -601,10 +601,15 @@
         <v>0.007428041666666667</v>
       </c>
       <c r="T2" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0</v>
+        <v>63.63469866666667</v>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>(0.8344859658431969, array([[2700, 2447],
+       [2788, 1937],
+       [3397, 2042],
+       [3310, 2551]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -668,10 +673,15 @@
         <v>0.01578345833333333</v>
       </c>
       <c r="T3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" t="n">
-        <v>0</v>
+        <v>24.83500533333333</v>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>(0.7962118272802876, array([[2248, 2455],
+       [2364, 1732],
+       [3272, 1877],
+       [3156, 2601]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -735,10 +745,15 @@
         <v>0.02534066666666667</v>
       </c>
       <c r="T4" t="n">
-        <v>0.9590908089813064</v>
-      </c>
-      <c r="U4" t="n">
-        <v>0.9598524141902736</v>
+        <v>35.06335733333334</v>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>(0.9585903115342803, array([[2246, 2169],
+       [2657, 1253],
+       [3537, 1647],
+       [3125, 2564]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -802,10 +817,15 @@
         <v>0.0257145</v>
       </c>
       <c r="T5" t="n">
-        <v>0.7543906155817381</v>
-      </c>
-      <c r="U5" t="n">
-        <v>0.7543906155817381</v>
+        <v>29.05372</v>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>(0.7543906155817381, array([[2247, 1445],
+       [3052, 1077],
+       [3540, 2144],
+       [2735, 2512]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -869,10 +889,15 @@
         <v>0.02665416666666667</v>
       </c>
       <c r="T6" t="n">
-        <v>0.7364616994662463</v>
-      </c>
-      <c r="U6" t="n">
-        <v>0.7364198557790879</v>
+        <v>35.49981866666667</v>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>(0.7359358785151086, array([[2122, 1605],
+       [2668,  922],
+       [3596, 1664],
+       [3049, 2347]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -936,10 +961,15 @@
         <v>0.02822516666666667</v>
       </c>
       <c r="T7" t="n">
-        <v>0.8579038102846333</v>
-      </c>
-      <c r="U7" t="n">
-        <v>0.8579038102846333</v>
+        <v>39.607296</v>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>(0.8579038102846333, array([[2208, 1840],
+       [2928, 1195],
+       [3679, 2035],
+       [2959, 2680]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -1003,10 +1033,15 @@
         <v>0.02492716666666667</v>
       </c>
       <c r="T8" t="n">
-        <v>0.8195326327080484</v>
-      </c>
-      <c r="U8" t="n">
-        <v>0.8190159795172345</v>
+        <v>45.54208</v>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>(0.8187388386661978, array([[2379, 1501],
+       [3445, 1046],
+       [3817, 1920],
+       [2751, 2374]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -1070,10 +1105,15 @@
         <v>0.02371083333333333</v>
       </c>
       <c r="T9" t="n">
-        <v>0.6700973592800732</v>
-      </c>
-      <c r="U9" t="n">
-        <v>0.6691808244643215</v>
+        <v>50.93696</v>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>(0.6691586861224738, array([[2658, 2787],
+       [2695, 1723],
+       [3408, 1748],
+       [3370, 2812]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -1137,10 +1177,15 @@
         <v>0.0315595</v>
       </c>
       <c r="T10" t="n">
-        <v>0.9886064952150878</v>
-      </c>
-      <c r="U10" t="n">
-        <v>0.9890238293208667</v>
+        <v>53.355648</v>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>(0.9882616985197341, array([[2022, 1885],
+       [2501,  816],
+       [3582, 1299],
+       [3104, 2368]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -1204,10 +1249,15 @@
         <v>0.021639</v>
       </c>
       <c r="T11" t="n">
-        <v>0.8964401294498382</v>
-      </c>
-      <c r="U11" t="n">
-        <v>0.8964401294498382</v>
+        <v>47.788832</v>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>(0.8964401294498382, array([[2080,  776],
+       [2911,  776],
+       [2911, 1703],
+       [2080, 1703]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -1271,10 +1321,15 @@
         <v>0.0153065</v>
       </c>
       <c r="T12" t="n">
-        <v>0.7141986575477366</v>
-      </c>
-      <c r="U12" t="n">
-        <v>0.7135785618796932</v>
+        <v>47.75181333333333</v>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>(0.7131949790335453, array([[2431, 1583],
+       [3205, 1169],
+       [3501, 1721],
+       [2727, 2136]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -1338,10 +1393,15 @@
         <v>0.03264966666666667</v>
       </c>
       <c r="T13" t="n">
-        <v>0.9489804286761476</v>
-      </c>
-      <c r="U13" t="n">
-        <v>0.9489804286761476</v>
+        <v>47.82069333333333</v>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>(0.9489804286761476, array([[1681, 2326],
+       [2612, 1217],
+       [3664, 2101],
+       [2733, 3210]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -1405,10 +1465,15 @@
         <v>0.01363091666666667</v>
       </c>
       <c r="T14" t="n">
-        <v>0</v>
-      </c>
-      <c r="U14" t="n">
-        <v>0</v>
+        <v>27.574448</v>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>(0.9287900100947079, array([[2415, 1918],
+       [3132, 1849],
+       [3206, 2621],
+       [2489, 2690]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -1472,10 +1537,15 @@
         <v>0.021689</v>
       </c>
       <c r="T15" t="n">
-        <v>0.9449161534959289</v>
-      </c>
-      <c r="U15" t="n">
-        <v>0.9444586207461122</v>
+        <v>54.15048</v>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>(0.9439346115807731, array([[2352, 1934],
+       [2764, 1204],
+       [3536, 1641],
+       [3124, 2370]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -1539,10 +1609,15 @@
         <v>0.02168833333333333</v>
       </c>
       <c r="T16" t="n">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="U16" t="n">
-        <v>0.3333333333333333</v>
+        <v>51.95069866666667</v>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>(0.796182235782607, array([[2112, 1677],
+       [2577, 1056],
+       [3357, 1640],
+       [2891, 2261]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -1606,10 +1681,15 @@
         <v>0.04435916666666666</v>
       </c>
       <c r="T17" t="n">
-        <v>0.9198465952997077</v>
-      </c>
-      <c r="U17" t="n">
-        <v>0.9198465952997077</v>
+        <v>56.67906666666666</v>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>(0.9198465952997077, array([[1913, 1962],
+       [2453,  918],
+       [3588, 1505],
+       [3048, 2549]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -1673,10 +1753,15 @@
         <v>0.02879733333333333</v>
       </c>
       <c r="T18" t="n">
-        <v>0.681027628871622</v>
-      </c>
-      <c r="U18" t="n">
-        <v>0.6810618777660431</v>
+        <v>42.42048533333333</v>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>(0.6805910718674436, array([[2528, 2124],
+       [3181, 1090],
+       [3885, 1535],
+       [3232, 2568]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -1740,10 +1825,15 @@
         <v>0.01853133333333333</v>
       </c>
       <c r="T19" t="n">
-        <v>0.6785739531725311</v>
-      </c>
-      <c r="U19" t="n">
-        <v>0.678298576004396</v>
+        <v>46.66402666666666</v>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>(0.6778668884670089, array([[2492, 2067],
+       [3273, 1364],
+       [3750, 1894],
+       [2969, 2596]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -1807,10 +1897,15 @@
         <v>0.01457866666666667</v>
       </c>
       <c r="T20" t="n">
-        <v>0.679588135756404</v>
-      </c>
-      <c r="U20" t="n">
-        <v>0.6803630632069665</v>
+        <v>56.62594666666666</v>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>(0.6795648329922541, array([[2062, 1026],
+       [2913, 1009],
+       [2925, 1588],
+       [2073, 1605]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -1874,10 +1969,15 @@
         <v>0.02898766666666667</v>
       </c>
       <c r="T21" t="n">
-        <v>0.6095042273798988</v>
-      </c>
-      <c r="U21" t="n">
-        <v>0.6095042273798988</v>
+        <v>53.948448</v>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>(0.6095042273798988, array([[2327, 2500],
+       [3026, 2098],
+       [3687, 3244],
+       [2988, 3646]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -1941,10 +2041,15 @@
         <v>0.03543516666666666</v>
       </c>
       <c r="T22" t="n">
-        <v>0.7991032830256088</v>
-      </c>
-      <c r="U22" t="n">
-        <v>0.7992332672806171</v>
+        <v>48.83826666666667</v>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>(0.7986778583184102, array([[2759, 2019],
+       [3400,  974],
+       [4236, 1485],
+       [3595, 2531]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -2008,10 +2113,15 @@
         <v>0.037257</v>
       </c>
       <c r="T23" t="n">
-        <v>0.8876174991636221</v>
-      </c>
-      <c r="U23" t="n">
-        <v>0.8876174991636221</v>
+        <v>28.80438666666667</v>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>(0.8876174991636221, array([[1733, 1523],
+       [3022, 1189],
+       [3319, 2333],
+       [2030, 2667]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -2075,10 +2185,15 @@
         <v>0.015522</v>
       </c>
       <c r="T24" t="n">
-        <v>0.8049271675411069</v>
-      </c>
-      <c r="U24" t="n">
-        <v>0.8055590851913615</v>
+        <v>57.002736</v>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>(0.8047515236937101, array([[2753, 2230],
+       [3532, 2093],
+       [3701, 3061],
+       [2922, 3197]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -2142,10 +2257,15 @@
         <v>0.01804008333333334</v>
       </c>
       <c r="T25" t="n">
-        <v>0</v>
-      </c>
-      <c r="U25" t="n">
-        <v>0</v>
+        <v>40.18913066666666</v>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>(0.8900404425281773, array([[2683, 1494],
+       [3620, 1435],
+       [3672, 2270],
+       [2735, 2328]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -2209,10 +2329,15 @@
         <v>0.02839925</v>
       </c>
       <c r="T26" t="n">
-        <v>0</v>
-      </c>
-      <c r="U26" t="n">
-        <v>0</v>
+        <v>35.43315733333333</v>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>(0.9687814205086791, array([[2648, 1460],
+       [3429,  627],
+       [4289, 1432],
+       [3508, 2266]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -2276,10 +2401,15 @@
         <v>0.018408125</v>
       </c>
       <c r="T27" t="n">
-        <v>0.7942868759010137</v>
-      </c>
-      <c r="U27" t="n">
-        <v>0.7945892684728506</v>
+        <v>48.37641066666666</v>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>(0.7938710379644698, array([[2623, 2226],
+       [3043, 1314],
+       [3768, 1647],
+       [3348, 2560]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -2343,10 +2473,15 @@
         <v>0.02715133333333333</v>
       </c>
       <c r="T28" t="n">
-        <v>0.2822213575695513</v>
-      </c>
-      <c r="U28" t="n">
-        <v>0.2602810012341217</v>
+        <v>50.55494933333333</v>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>(0.5742954118031572, array([[1682, 2115],
+       [2012, 1041],
+       [3882, 1615],
+       [3552, 2690]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -2410,10 +2545,15 @@
         <v>0.0302785</v>
       </c>
       <c r="T29" t="n">
-        <v>0.1785714285714286</v>
-      </c>
-      <c r="U29" t="n">
-        <v>0.1785714285714286</v>
+        <v>54.63698133333333</v>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>(0.6339194275415118, array([[1969, 1484],
+       [2552,  801],
+       [3630, 1720],
+       [3047, 2403]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -2477,10 +2617,15 @@
         <v>0.032656375</v>
       </c>
       <c r="T30" t="n">
-        <v>0.8903778770112327</v>
-      </c>
-      <c r="U30" t="n">
-        <v>0.889703735099161</v>
+        <v>61.323536</v>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>(0.8896099088705697, array([[1621, 1893],
+       [1777,  756],
+       [3055,  931],
+       [2899, 2069]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -2544,10 +2689,15 @@
         <v>0.03888220833333333</v>
       </c>
       <c r="T31" t="n">
-        <v>0.6886305479596794</v>
-      </c>
-      <c r="U31" t="n">
-        <v>0.6886305479596794</v>
+        <v>67.054672</v>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>(0.6886305479596794, array([[2051, 2075],
+       [2849, 1316],
+       [3951, 2475],
+       [3153, 3234]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="32">
@@ -2611,10 +2761,15 @@
         <v>0.04084775</v>
       </c>
       <c r="T32" t="n">
-        <v>0.5651454184219896</v>
-      </c>
-      <c r="U32" t="n">
-        <v>0.5646007947405126</v>
+        <v>44.267016</v>
+      </c>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>(0.5645831581319437, array([[2375, 1221],
+       [3377, 1165],
+       [3475, 2938],
+       [2474, 2994]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -2678,10 +2833,15 @@
         <v>0.03217033333333334</v>
       </c>
       <c r="T33" t="n">
-        <v>0.8248345964703522</v>
-      </c>
-      <c r="U33" t="n">
-        <v>0.8241600053958096</v>
+        <v>48.584672</v>
+      </c>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>(0.824042154848583, array([[1487, 1416],
+       [2709, 1196],
+       [2891, 2203],
+       [1669, 2424]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="34">
@@ -2745,10 +2905,15 @@
         <v>0.04239645833333333</v>
       </c>
       <c r="T34" t="n">
-        <v>0.3993373901604954</v>
-      </c>
-      <c r="U34" t="n">
-        <v>0.3692384584576923</v>
+        <v>35.999768</v>
+      </c>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>(0.8455350003865124, array([[1486, 2949],
+       [1600, 1532],
+       [2799, 1628],
+       [2685, 3046]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="35">
@@ -2812,10 +2977,15 @@
         <v>0.030271125</v>
       </c>
       <c r="T35" t="n">
-        <v>0</v>
-      </c>
-      <c r="U35" t="n">
-        <v>0</v>
+        <v>46.44088</v>
+      </c>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>(0.8927349572241833, array([[2308, 2033],
+       [3239, 1241],
+       [4126, 2284],
+       [3195, 3076]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -2879,10 +3049,15 @@
         <v>0.01632</v>
       </c>
       <c r="T36" t="n">
-        <v>0</v>
-      </c>
-      <c r="U36" t="n">
-        <v>0</v>
+        <v>68.24492266666667</v>
+      </c>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>(0.47103566706641864, array([[2086, 1708],
+       [3278, 1636],
+       [3312, 2198],
+       [2119, 2270]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="37">
@@ -2946,10 +3121,15 @@
         <v>0.02017875</v>
       </c>
       <c r="T37" t="n">
-        <v>0.8841342656366967</v>
-      </c>
-      <c r="U37" t="n">
-        <v>0.883578182954165</v>
+        <v>60.16693866666667</v>
+      </c>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>(0.8832695484166903, array([[2322, 1787],
+       [3201, 1432],
+       [3602, 2426],
+       [2724, 2781]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="38">
@@ -3013,10 +3193,15 @@
         <v>0.03304125</v>
       </c>
       <c r="T38" t="n">
-        <v>0.896326365911809</v>
-      </c>
-      <c r="U38" t="n">
-        <v>0.896326365911809</v>
+        <v>43.29832266666666</v>
+      </c>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>(0.896326365911809, array([[2324,  901],
+       [3379,  782],
+       [3512, 1959],
+       [2457, 2078]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="39">
@@ -3080,10 +3265,15 @@
         <v>0.030832875</v>
       </c>
       <c r="T39" t="n">
-        <v>0.9430742709467377</v>
-      </c>
-      <c r="U39" t="n">
-        <v>0.9430742709467377</v>
+        <v>33.94951733333333</v>
+      </c>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>(0.9430742709467377, array([[1114, 1898],
+       [2257, 1781],
+       [2381, 2993],
+       [1238, 3110]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="40">
@@ -3147,10 +3337,15 @@
         <v>0.03890025</v>
       </c>
       <c r="T40" t="n">
-        <v>0.3636363636363636</v>
-      </c>
-      <c r="U40" t="n">
-        <v>0.3636363636363636</v>
+        <v>60.54719466666667</v>
+      </c>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>(0.8424126996394752, array([[1562,  844],
+       [3192,  687],
+       [3325, 2061],
+       [1694, 2218]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="41">
@@ -3214,10 +3409,15 @@
         <v>0.03878133333333333</v>
       </c>
       <c r="T41" t="n">
-        <v>0.6954470097682223</v>
-      </c>
-      <c r="U41" t="n">
-        <v>0.6955950799618094</v>
+        <v>49.88592533333333</v>
+      </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>(0.6951771644631741, array([[2398,  878],
+       [3783,  256],
+       [4215, 1219],
+       [2831, 1841]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="42">
@@ -3281,10 +3481,15 @@
         <v>0.020028</v>
       </c>
       <c r="T42" t="n">
-        <v>0.6050094184836338</v>
-      </c>
-      <c r="U42" t="n">
-        <v>0.6052485013710623</v>
+        <v>40.67521333333333</v>
+      </c>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>(0.6048151956254484, array([[2533, 2496],
+       [2747, 1709],
+       [4047, 2062],
+       [3834, 2849]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="43">
@@ -3348,10 +3553,15 @@
         <v>0.035679375</v>
       </c>
       <c r="T43" t="n">
-        <v>0.7265064609383657</v>
-      </c>
-      <c r="U43" t="n">
-        <v>0.7265064609383657</v>
+        <v>54.71797333333333</v>
+      </c>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>(0.7265064609383657, array([[2174, 2049],
+       [3333, 1515],
+       [3721, 2357],
+       [2562, 2891]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="44">
@@ -3415,10 +3625,15 @@
         <v>0.0216115</v>
       </c>
       <c r="T44" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="U44" t="n">
-        <v>0.5</v>
+        <v>29.76685333333333</v>
+      </c>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>(0.7969775714298685, array([[2309, 2178],
+       [2769, 1519],
+       [3596, 2096],
+       [3136, 2755]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="45">
@@ -3482,10 +3697,15 @@
         <v>0.029323125</v>
       </c>
       <c r="T45" t="n">
-        <v>0.892474934017691</v>
-      </c>
-      <c r="U45" t="n">
-        <v>0.892474934017691</v>
+        <v>49.221568</v>
+      </c>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>(0.892474934017691, array([[2143, 2162],
+       [3081, 1472],
+       [3697, 2309],
+       [2759, 2999]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="46">
@@ -3549,10 +3769,15 @@
         <v>0.024273375</v>
       </c>
       <c r="T46" t="n">
-        <v>0.6703385073664702</v>
-      </c>
-      <c r="U46" t="n">
-        <v>0.6703385073664702</v>
+        <v>50.51412266666667</v>
+      </c>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>(0.6703385073664702, array([[2237, 2604],
+       [2646, 1348],
+       [3488, 1622],
+       [3079, 2878]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="47">
@@ -3616,10 +3841,15 @@
         <v>0.01099604166666667</v>
       </c>
       <c r="T47" t="n">
-        <v>0</v>
-      </c>
-      <c r="U47" t="n">
-        <v>0</v>
+        <v>50.40916266666667</v>
+      </c>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>(0.8140854685014837, array([[2324, 2137],
+       [2639, 1607],
+       [3290, 1994],
+       [2974, 2525]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="48">
@@ -3683,10 +3913,15 @@
         <v>0.021783875</v>
       </c>
       <c r="T48" t="n">
-        <v>0.8141485856822432</v>
-      </c>
-      <c r="U48" t="n">
-        <v>0.8141485856822432</v>
+        <v>41.737776</v>
+      </c>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>(0.8141485856822432, array([[1854, 2161],
+       [2087, 1307],
+       [3136, 1593],
+       [2903, 2447]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="49">
@@ -3750,10 +3985,15 @@
         <v>0.02043954166666667</v>
       </c>
       <c r="T49" t="n">
-        <v>0.8062894171951291</v>
-      </c>
-      <c r="U49" t="n">
-        <v>0.8062894171951291</v>
+        <v>63.58593066666667</v>
+      </c>
+      <c r="U49" t="inlineStr">
+        <is>
+          <t>(0.8062894171951291, array([[2095, 1646],
+       [2480,  877],
+       [3434, 1354],
+       [3049, 2123]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="50">
@@ -3817,10 +4057,15 @@
         <v>0.0185875</v>
       </c>
       <c r="T50" t="n">
-        <v>0.8138026520937193</v>
-      </c>
-      <c r="U50" t="n">
-        <v>0.8130894052049265</v>
+        <v>35.66297333333333</v>
+      </c>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>(0.812941788428894, array([[3216, 1631],
+       [3407,  727],
+       [4519,  961],
+       [4328, 1866]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="51">
@@ -3884,10 +4129,15 @@
         <v>0.008538125000000001</v>
       </c>
       <c r="T51" t="n">
-        <v>0.8653808156713433</v>
-      </c>
-      <c r="U51" t="n">
-        <v>0.8653808156713433</v>
+        <v>26.510832</v>
+      </c>
+      <c r="U51" t="inlineStr">
+        <is>
+          <t>(0.8653808156713433, array([[2417, 1840],
+       [2988, 1644],
+       [3158, 2138],
+       [2587, 2334]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="52">
@@ -3951,10 +4201,15 @@
         <v>0.00873025</v>
       </c>
       <c r="T52" t="n">
-        <v>0.7148933774933853</v>
-      </c>
-      <c r="U52" t="n">
-        <v>0.7134948692869031</v>
+        <v>29.66302666666667</v>
+      </c>
+      <c r="U52" t="inlineStr">
+        <is>
+          <t>(0.7134754969926915, array([[2398, 1619],
+       [2901, 1609],
+       [2915, 2314],
+       [2411, 2324]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="53">
@@ -4018,10 +4273,15 @@
         <v>0.007945208333333334</v>
       </c>
       <c r="T53" t="n">
-        <v>0.2773500981126146</v>
-      </c>
-      <c r="U53" t="n">
-        <v>0</v>
+        <v>25.95370666666667</v>
+      </c>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>(0.6846142572468186, array([[3053, 1998],
+       [3316, 1406],
+       [3722, 1586],
+       [3459, 2179]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="54">
@@ -4085,10 +4345,15 @@
         <v>0.02707825</v>
       </c>
       <c r="T54" t="n">
-        <v>0.8454417756599041</v>
-      </c>
-      <c r="U54" t="n">
-        <v>0.8454417756599041</v>
+        <v>25.58365333333333</v>
+      </c>
+      <c r="U54" t="inlineStr">
+        <is>
+          <t>(0.8454417756599041, array([[2347, 2758],
+       [2444, 1817],
+       [3557, 1932],
+       [3460, 2873]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="55">
@@ -4152,10 +4417,15 @@
         <v>0.02157225</v>
       </c>
       <c r="T55" t="n">
-        <v>0.6023408678164811</v>
-      </c>
-      <c r="U55" t="n">
-        <v>0.6021183508355402</v>
+        <v>26.324952</v>
+      </c>
+      <c r="U55" t="inlineStr">
+        <is>
+          <t>(0.6017359053993518, array([[2227, 2306],
+       [3053, 1520],
+       [3526, 2017],
+       [2701, 2803]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="56">
@@ -4219,10 +4489,15 @@
         <v>0.028808875</v>
       </c>
       <c r="T56" t="n">
-        <v>0.7694323144104803</v>
-      </c>
-      <c r="U56" t="n">
-        <v>0.7694323144104803</v>
+        <v>24.591304</v>
+      </c>
+      <c r="U56" t="inlineStr">
+        <is>
+          <t>(0.7694323144104803, array([[2250, 2040],
+       [3131, 2040],
+       [3131, 3185],
+       [2250, 3185]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="57">
@@ -4286,10 +4561,15 @@
         <v>0.01523766666666667</v>
       </c>
       <c r="T57" t="n">
-        <v>0.9810271337647909</v>
-      </c>
-      <c r="U57" t="n">
-        <v>0.9813688202049343</v>
+        <v>42.439712</v>
+      </c>
+      <c r="U57" t="inlineStr">
+        <is>
+          <t>(0.9803939018860889, array([[2927, 1823],
+       [3629, 1376],
+       [4085, 2091],
+       [3383, 2539]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="58">
@@ -4353,10 +4633,15 @@
         <v>0.01596066666666667</v>
       </c>
       <c r="T58" t="n">
-        <v>0</v>
-      </c>
-      <c r="U58" t="n">
-        <v>0</v>
+        <v>49.12457066666666</v>
+      </c>
+      <c r="U58" t="inlineStr">
+        <is>
+          <t>(0.8420383113490758, array([[2100, 1622],
+       [3107, 1397],
+       [3297, 2245],
+       [2290, 2471]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="59">
@@ -4420,10 +4705,15 @@
         <v>0.01668425</v>
       </c>
       <c r="T59" t="n">
-        <v>0.7279783069420004</v>
-      </c>
-      <c r="U59" t="n">
-        <v>0.7283024978001152</v>
+        <v>52.86003733333333</v>
+      </c>
+      <c r="U59" t="inlineStr">
+        <is>
+          <t>(0.7273391940960838, array([[1881, 2140],
+       [2789, 1824],
+       [3020, 2485],
+       [2111, 2802]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="60">
@@ -4487,10 +4777,15 @@
         <v>0.01417883333333333</v>
       </c>
       <c r="T60" t="n">
-        <v>0.5020618644176027</v>
-      </c>
-      <c r="U60" t="n">
-        <v>0.5020618644176027</v>
+        <v>24.209096</v>
+      </c>
+      <c r="U60" t="inlineStr">
+        <is>
+          <t>(0.725683382625762, array([[2639, 1559],
+       [3229, 1540],
+       [3256, 2352],
+       [2666, 2372]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="61">
@@ -4554,10 +4849,15 @@
         <v>0.029318</v>
       </c>
       <c r="T61" t="n">
-        <v>0.8380641137030223</v>
-      </c>
-      <c r="U61" t="n">
-        <v>0.8381802350296059</v>
+        <v>35.731032</v>
+      </c>
+      <c r="U61" t="inlineStr">
+        <is>
+          <t>(0.8374243597097225, array([[2585, 1088],
+       [3641,  908],
+       [3856, 2169],
+       [2799, 2348]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="62">
@@ -4621,10 +4921,15 @@
         <v>0.033310875</v>
       </c>
       <c r="T62" t="n">
-        <v>0.6722108441300645</v>
-      </c>
-      <c r="U62" t="n">
-        <v>0.6722108441300645</v>
+        <v>33.9576</v>
+      </c>
+      <c r="U62" t="inlineStr">
+        <is>
+          <t>(0.6722108441300645, array([[1680, 1956],
+       [2451,  540],
+       [3403, 1058],
+       [2632, 2474]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="63">
@@ -4688,10 +4993,15 @@
         <v>0.007896625000000001</v>
       </c>
       <c r="T63" t="n">
-        <v>0.6612549773758402</v>
-      </c>
-      <c r="U63" t="n">
-        <v>0.6612549773758402</v>
+        <v>35.39396</v>
+      </c>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t>(0.6612549773758402, array([[2668, 2309],
+       [2845, 1568],
+       [3335, 1685],
+       [3158, 2426]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="64">
@@ -4755,10 +5065,15 @@
         <v>0.01543379166666667</v>
       </c>
       <c r="T64" t="n">
-        <v>0.6223053360113346</v>
-      </c>
-      <c r="U64" t="n">
-        <v>0.6218724612774554</v>
+        <v>39.04019733333333</v>
+      </c>
+      <c r="U64" t="inlineStr">
+        <is>
+          <t>(0.6215244780800616, array([[2650, 2443],
+       [3257, 1597],
+       [3783, 1974],
+       [3177, 2820]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="65">
@@ -4822,10 +5137,15 @@
         <v>0.03779220833333333</v>
       </c>
       <c r="T65" t="n">
-        <v>0.7336023911317648</v>
-      </c>
-      <c r="U65" t="n">
-        <v>0.7336562677106536</v>
+        <v>27.82893333333333</v>
+      </c>
+      <c r="U65" t="inlineStr">
+        <is>
+          <t>(0.7332616010060513, array([[2058, 1797],
+       [2674,  824],
+       [4001, 1664],
+       [3384, 2637]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="66">
@@ -4889,10 +5209,15 @@
         <v>0.018113875</v>
       </c>
       <c r="T66" t="n">
-        <v>0.9350230099605422</v>
-      </c>
-      <c r="U66" t="n">
-        <v>0.9350230099605422</v>
+        <v>70.53980799999999</v>
+      </c>
+      <c r="U66" t="inlineStr">
+        <is>
+          <t>(0.9350230099605422, array([[2961, 1259],
+       [3731,  567],
+       [4378, 1287],
+       [3608, 1979]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="67">
@@ -4956,10 +5281,15 @@
         <v>0.02211375</v>
       </c>
       <c r="T67" t="n">
-        <v>0.836535321793914</v>
-      </c>
-      <c r="U67" t="n">
-        <v>0.836535321793914</v>
+        <v>71.146272</v>
+      </c>
+      <c r="U67" t="inlineStr">
+        <is>
+          <t>(0.836535321793914, array([[1823, 1197],
+       [2759,  990],
+       [3006, 2109],
+       [2070, 2316]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="68">
@@ -5023,10 +5353,15 @@
         <v>0.01680670833333333</v>
       </c>
       <c r="T68" t="n">
-        <v>0</v>
-      </c>
-      <c r="U68" t="n">
-        <v>0</v>
+        <v>45.54658666666667</v>
+      </c>
+      <c r="U68" t="inlineStr">
+        <is>
+          <t>(0.5950764869850156, array([[1162, 2997],
+       [2271, 2265],
+       [2708, 2925],
+       [1598, 3658]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="69">
@@ -5090,10 +5425,15 @@
         <v>0.032661625</v>
       </c>
       <c r="T69" t="n">
-        <v>0.7329872387574156</v>
-      </c>
-      <c r="U69" t="n">
-        <v>0.7329872387574156</v>
+        <v>35.12685866666666</v>
+      </c>
+      <c r="U69" t="inlineStr">
+        <is>
+          <t>(0.7329872387574156, array([[1304, 2094],
+       [1678, 1106],
+       [3026, 1616],
+       [2652, 2604]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="70">
@@ -5157,10 +5497,15 @@
         <v>0.021076625</v>
       </c>
       <c r="T70" t="n">
-        <v>0.9587094081358429</v>
-      </c>
-      <c r="U70" t="n">
-        <v>0.9578663778737779</v>
+        <v>43.36323466666666</v>
+      </c>
+      <c r="U70" t="inlineStr">
+        <is>
+          <t>(0.9577064137544659, array([[2723, 2554],
+       [2878, 1625],
+       [3848, 1786],
+       [3693, 2716]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="71">
@@ -5224,10 +5569,15 @@
         <v>0.01761625</v>
       </c>
       <c r="T71" t="n">
-        <v>0.322490309931942</v>
-      </c>
-      <c r="U71" t="n">
-        <v>0.322490309931942</v>
+        <v>29.15065866666666</v>
+      </c>
+      <c r="U71" t="inlineStr">
+        <is>
+          <t>(0.8298914784870723, array([[2615, 2348],
+       [2882, 1591],
+       [3793, 1912],
+       [3527, 2669]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="72">
@@ -5291,10 +5641,15 @@
         <v>0.026548125</v>
       </c>
       <c r="T72" t="n">
-        <v>0.1548126033266037</v>
-      </c>
-      <c r="U72" t="n">
-        <v>0.1548126033266037</v>
+        <v>33.30416533333333</v>
+      </c>
+      <c r="U72" t="inlineStr">
+        <is>
+          <t>(0.827313913093154, array([[2586, 1932],
+       [2682,  959],
+       [3858, 1076],
+       [3762, 2049]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="73">
@@ -5358,10 +5713,15 @@
         <v>0.034155375</v>
       </c>
       <c r="T73" t="n">
-        <v>0.7374767589685881</v>
-      </c>
-      <c r="U73" t="n">
-        <v>0.7374767589685881</v>
+        <v>23.89247466666666</v>
+      </c>
+      <c r="U73" t="inlineStr">
+        <is>
+          <t>(0.7374767589685881, array([[2257, 2124],
+       [2434,  961],
+       [4011, 1201],
+       [3834, 2364]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="74">
@@ -5425,10 +5785,15 @@
         <v>0.012401</v>
       </c>
       <c r="T74" t="n">
-        <v>0.7504212420510876</v>
-      </c>
-      <c r="U74" t="n">
-        <v>0.7495304429389414</v>
+        <v>45.93775466666666</v>
+      </c>
+      <c r="U74" t="inlineStr">
+        <is>
+          <t>(0.7493863576057669, array([[2422, 2015],
+       [2552, 1314],
+       [3486, 1488],
+       [3356, 2188]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="75">
@@ -5492,10 +5857,15 @@
         <v>0.01354866666666667</v>
       </c>
       <c r="T75" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="U75" t="n">
-        <v>0.25</v>
+        <v>34.02794933333333</v>
+      </c>
+      <c r="U75" t="inlineStr">
+        <is>
+          <t>(0.8034459947699902, array([[2544, 2745],
+       [2681, 1882],
+       [3754, 2053],
+       [3616, 2915]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="76">
@@ -5559,10 +5929,15 @@
         <v>0.01588145833333333</v>
       </c>
       <c r="T76" t="n">
-        <v>0</v>
-      </c>
-      <c r="U76" t="n">
-        <v>0</v>
+        <v>33.23579733333333</v>
+      </c>
+      <c r="U76" t="inlineStr">
+        <is>
+          <t>(0.974856196622002, array([[2267, 1782],
+       [2982, 1142],
+       [3639, 1875],
+       [2924, 2515]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="77">
@@ -5626,10 +6001,15 @@
         <v>0.01920825</v>
       </c>
       <c r="T77" t="n">
-        <v>0.8221932102687244</v>
-      </c>
-      <c r="U77" t="n">
-        <v>0.8216270961120783</v>
+        <v>35.954048</v>
+      </c>
+      <c r="U77" t="inlineStr">
+        <is>
+          <t>(0.8209783883305874, array([[2480, 1480],
+       [3264, 1314],
+       [3467, 2268],
+       [2682, 2435]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="78">
@@ -5693,10 +6073,15 @@
         <v>0.024756</v>
       </c>
       <c r="T78" t="n">
-        <v>0.6758430482165477</v>
-      </c>
-      <c r="U78" t="n">
-        <v>0.6763229513362352</v>
+        <v>37.41944533333334</v>
+      </c>
+      <c r="U78" t="inlineStr">
+        <is>
+          <t>(0.6758205759890635, array([[2482, 1460],
+       [3391, 1432],
+       [3432, 2777],
+       [2523, 2804]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="79">
@@ -5760,10 +6145,15 @@
         <v>0.01479166666666667</v>
       </c>
       <c r="T79" t="n">
-        <v>0</v>
-      </c>
-      <c r="U79" t="n">
-        <v>0</v>
+        <v>31.012312</v>
+      </c>
+      <c r="U79" t="inlineStr">
+        <is>
+          <t>(0.9454154659690494, array([[2330, 2087],
+       [2828, 1302],
+       [3571, 1774],
+       [3072, 2559]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="80">
@@ -5827,10 +6217,15 @@
         <v>0.01303245833333333</v>
       </c>
       <c r="T80" t="n">
-        <v>0</v>
-      </c>
-      <c r="U80" t="n">
-        <v>0</v>
+        <v>32.899456</v>
+      </c>
+      <c r="U80" t="inlineStr">
+        <is>
+          <t>(0.7158122713042072, array([[2439, 2062],
+       [3071, 1358],
+       [3576, 1810],
+       [2944, 2515]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="81">
@@ -5894,10 +6289,15 @@
         <v>0.02132279166666667</v>
       </c>
       <c r="T81" t="n">
-        <v>0.6872626075631345</v>
-      </c>
-      <c r="U81" t="n">
-        <v>0.6864225963648877</v>
+        <v>37.83626666666667</v>
+      </c>
+      <c r="U81" t="inlineStr">
+        <is>
+          <t>(0.6863498608793892, array([[2810, 2435],
+       [2896, 1692],
+       [3977, 1818],
+       [3891, 2560]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="82">
@@ -5961,10 +6361,15 @@
         <v>0.020887875</v>
       </c>
       <c r="T82" t="n">
-        <v>0.9232478865771004</v>
-      </c>
-      <c r="U82" t="n">
-        <v>0.9232478865771004</v>
+        <v>48.63002666666667</v>
+      </c>
+      <c r="U82" t="inlineStr">
+        <is>
+          <t>(0.9232478865771004, array([[2755, 2141],
+       [3366, 1561],
+       [3994, 2223],
+       [3383, 2803]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="83">
@@ -6028,10 +6433,15 @@
         <v>0.012898375</v>
       </c>
       <c r="T83" t="n">
-        <v>0.7529971463647518</v>
-      </c>
-      <c r="U83" t="n">
-        <v>0.7531857691681176</v>
+        <v>38.44942933333333</v>
+      </c>
+      <c r="U83" t="inlineStr">
+        <is>
+          <t>(0.7524305712643743, array([[2549, 2274],
+       [2976, 1519],
+       [3545, 1840],
+       [3118, 2596]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="84">
@@ -6095,10 +6505,15 @@
         <v>0.022444125</v>
       </c>
       <c r="T84" t="n">
-        <v>0.965431754193505</v>
-      </c>
-      <c r="U84" t="n">
-        <v>0.965431754193505</v>
+        <v>45.055056</v>
+      </c>
+      <c r="U84" t="inlineStr">
+        <is>
+          <t>(0.965431754193505, array([[1975,  670],
+       [3044,  569],
+       [3142, 1601],
+       [2073, 1702]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="85">
@@ -6162,10 +6577,15 @@
         <v>0.030173125</v>
       </c>
       <c r="T85" t="n">
-        <v>0.9839780009245188</v>
-      </c>
-      <c r="U85" t="n">
-        <v>0.9839780009245188</v>
+        <v>51.69056</v>
+      </c>
+      <c r="U85" t="inlineStr">
+        <is>
+          <t>(0.9839780009245188, array([[2035, 2518],
+       [2180, 1327],
+       [3352, 1469],
+       [3207, 2660]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="86">
@@ -6229,10 +6649,15 @@
         <v>0.02764391666666667</v>
       </c>
       <c r="T86" t="n">
-        <v>0.9003468291199492</v>
-      </c>
-      <c r="U86" t="n">
-        <v>0.9005216367493615</v>
+        <v>37.38932533333333</v>
+      </c>
+      <c r="U86" t="inlineStr">
+        <is>
+          <t>(0.8998911719884006, array([[1933, 1788],
+       [2520,  885],
+       [3523, 1538],
+       [2935, 2441]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="87">
@@ -6296,10 +6721,15 @@
         <v>0.02409025</v>
       </c>
       <c r="T87" t="n">
-        <v>0.8015845223593798</v>
-      </c>
-      <c r="U87" t="n">
-        <v>0.8022500333088446</v>
+        <v>25.05626133333333</v>
+      </c>
+      <c r="U87" t="inlineStr">
+        <is>
+          <t>(0.8014854339903609, array([[2188, 1662],
+       [3020, 1576],
+       [3128, 2613],
+       [2296, 2700]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="88">
@@ -6363,10 +6793,15 @@
         <v>0.026822125</v>
       </c>
       <c r="T88" t="n">
-        <v>0.6521791056869546</v>
-      </c>
-      <c r="U88" t="n">
-        <v>0.6516988981287931</v>
+        <v>31.27939466666666</v>
+      </c>
+      <c r="U88" t="inlineStr">
+        <is>
+          <t>(0.651454330632309, array([[2273, 1916],
+       [2640, 1206],
+       [3728, 1770],
+       [3361, 2479]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="89">
@@ -6430,10 +6865,15 @@
         <v>0.01685245833333333</v>
       </c>
       <c r="T89" t="n">
-        <v>0.05590169943749474</v>
-      </c>
-      <c r="U89" t="n">
-        <v>0.0604122093330177</v>
+        <v>56.45187733333334</v>
+      </c>
+      <c r="U89" t="inlineStr">
+        <is>
+          <t>(0.7431258137357967, array([[2521, 1942],
+       [3097, 1549],
+       [3626, 2324],
+       [3050, 2717]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="90">
@@ -6497,10 +6937,15 @@
         <v>0.013739375</v>
       </c>
       <c r="T90" t="n">
-        <v>0</v>
-      </c>
-      <c r="U90" t="n">
-        <v>0</v>
+        <v>29.642512</v>
+      </c>
+      <c r="U90" t="inlineStr">
+        <is>
+          <t>(0.7993329318544752, array([[2262, 2149],
+       [2499, 1296],
+       [3566, 1593],
+       [3329, 2446]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="91">
@@ -6564,10 +7009,15 @@
         <v>0.015003875</v>
       </c>
       <c r="T91" t="n">
-        <v>0</v>
-      </c>
-      <c r="U91" t="n">
-        <v>0</v>
+        <v>27.58088533333333</v>
+      </c>
+      <c r="U91" t="inlineStr">
+        <is>
+          <t>(0.8070766856774393, array([[2260, 2356],
+       [2335, 1118],
+       [3335, 1178],
+       [3260, 2417]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="92">
@@ -6631,10 +7081,15 @@
         <v>0.012524125</v>
       </c>
       <c r="T92" t="n">
-        <v>0.3125</v>
-      </c>
-      <c r="U92" t="n">
-        <v>0.3125</v>
+        <v>38.75453066666667</v>
+      </c>
+      <c r="U92" t="inlineStr">
+        <is>
+          <t>(0.6840510630730532, array([[2247, 1753],
+       [3159, 1387],
+       [3409, 2011],
+       [2497, 2377]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="93">
@@ -6698,10 +7153,15 @@
         <v>0.014082125</v>
       </c>
       <c r="T93" t="n">
-        <v>0.6194371581200879</v>
-      </c>
-      <c r="U93" t="n">
-        <v>0.6194371581200879</v>
+        <v>44.80746133333334</v>
+      </c>
+      <c r="U93" t="inlineStr">
+        <is>
+          <t>(0.6194371581200879, array([[2385, 2234],
+       [2843, 1190],
+       [3490, 1473],
+       [3032, 2517]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="94">
@@ -6765,10 +7225,15 @@
         <v>0.02441508333333333</v>
       </c>
       <c r="T94" t="n">
-        <v>0.8780547250333545</v>
-      </c>
-      <c r="U94" t="n">
-        <v>0.8767481691413811</v>
+        <v>52.94913066666667</v>
+      </c>
+      <c r="U94" t="inlineStr">
+        <is>
+          <t>(0.8767296925006018, array([[2408, 2297],
+       [3175, 1555],
+       [3826, 2227],
+       [3060, 2970]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="95">
@@ -6832,10 +7297,15 @@
         <v>0.02372025</v>
       </c>
       <c r="T95" t="n">
-        <v>0.7057324840764331</v>
-      </c>
-      <c r="U95" t="n">
-        <v>0.7057324840764331</v>
+        <v>42.898008</v>
+      </c>
+      <c r="U95" t="inlineStr">
+        <is>
+          <t>(0.7057324840764331, array([[2067, 1646],
+       [2852,  861],
+       [3406, 1415],
+       [2621, 2200]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="96">
@@ -6899,10 +7369,15 @@
         <v>0.02372025</v>
       </c>
       <c r="T96" t="n">
-        <v>0.7057324840764331</v>
-      </c>
-      <c r="U96" t="n">
-        <v>0.7057324840764331</v>
+        <v>45.40811733333334</v>
+      </c>
+      <c r="U96" t="inlineStr">
+        <is>
+          <t>(0.7057324840764331, array([[2067, 1646],
+       [2852,  861],
+       [3406, 1415],
+       [2621, 2200]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="97">
@@ -6966,10 +7441,15 @@
         <v>0.01897225</v>
       </c>
       <c r="T97" t="n">
-        <v>0.8048042497723854</v>
-      </c>
-      <c r="U97" t="n">
-        <v>0.8048042497723854</v>
+        <v>25.968008</v>
+      </c>
+      <c r="U97" t="inlineStr">
+        <is>
+          <t>(0.8048042497723854, array([[2592, 1256],
+       [3560, 1126],
+       [3665, 1905],
+       [2697, 2035]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="98">
@@ -7033,10 +7513,15 @@
         <v>0.0105845</v>
       </c>
       <c r="T98" t="n">
-        <v>0.5600820533723462</v>
-      </c>
-      <c r="U98" t="n">
-        <v>0.5600820533723462</v>
+        <v>27.814624</v>
+      </c>
+      <c r="U98" t="inlineStr">
+        <is>
+          <t>(0.5600820533723462, array([[2697, 2411],
+       [3219, 2396],
+       [3246, 3328],
+       [2724, 3343]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="99">
@@ -7100,10 +7585,15 @@
         <v>0.037367875</v>
       </c>
       <c r="T99" t="n">
-        <v>0.3954313302576144</v>
-      </c>
-      <c r="U99" t="n">
-        <v>0.3952393846335605</v>
+        <v>53.972512</v>
+      </c>
+      <c r="U99" t="inlineStr">
+        <is>
+          <t>(0.3951233560893895, array([[1578, 1655],
+       [2250, 1014],
+       [3872, 2715],
+       [3199, 3356]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="100">
@@ -7167,10 +7657,15 @@
         <v>0.03958004166666667</v>
       </c>
       <c r="T100" t="n">
-        <v>0.3833673799681843</v>
-      </c>
-      <c r="U100" t="n">
-        <v>0.3830342626646987</v>
+        <v>41.99886933333333</v>
+      </c>
+      <c r="U100" t="inlineStr">
+        <is>
+          <t>(0.3829847227615254, array([[1931, 2225],
+       [2235, 1327],
+       [4580, 2119],
+       [4276, 3018]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="101">
@@ -7234,10 +7729,15 @@
         <v>0.01237495833333333</v>
       </c>
       <c r="T101" t="n">
-        <v>0</v>
-      </c>
-      <c r="U101" t="n">
-        <v>0</v>
+        <v>46.96074666666667</v>
+      </c>
+      <c r="U101" t="inlineStr">
+        <is>
+          <t>(0.8421021183026727, array([[2489, 1704],
+       [3228, 1341],
+       [3535, 1964],
+       [2795, 2327]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="102">
@@ -7301,10 +7801,15 @@
         <v>0.023845125</v>
       </c>
       <c r="T102" t="n">
-        <v>0.8034838129758619</v>
-      </c>
-      <c r="U102" t="n">
-        <v>0.8037981842734963</v>
+        <v>30.273104</v>
+      </c>
+      <c r="U102" t="inlineStr">
+        <is>
+          <t>(0.8027530169078234, array([[2279, 2268],
+       [2536, 1355],
+       [3269, 1561],
+       [3013, 2473]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="103">
@@ -7368,10 +7873,15 @@
         <v>0.011769375</v>
       </c>
       <c r="T103" t="n">
-        <v>0.9461793343444248</v>
-      </c>
-      <c r="U103" t="n">
-        <v>0.9471523105938859</v>
+        <v>48.18122666666667</v>
+      </c>
+      <c r="U103" t="inlineStr">
+        <is>
+          <t>(0.9460952693185568, array([[1935, 2365],
+       [2002, 1475],
+       [2845, 1538],
+       [2778, 2429]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="104">
@@ -7435,10 +7945,15 @@
         <v>0.0324855</v>
       </c>
       <c r="T104" t="n">
-        <v>0.6609280416978599</v>
-      </c>
-      <c r="U104" t="n">
-        <v>0.6610636913358497</v>
+        <v>50.16221333333333</v>
+      </c>
+      <c r="U104" t="inlineStr">
+        <is>
+          <t>(0.6606769774878708, array([[2427, 2018],
+       [3046,  575],
+       [4000,  984],
+       [3381, 2428]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="105">
@@ -7502,10 +8017,15 @@
         <v>0.041817125</v>
       </c>
       <c r="T105" t="n">
-        <v>0.1937656480230451</v>
-      </c>
-      <c r="U105" t="n">
-        <v>0.1844975185250637</v>
+        <v>44.06296533333333</v>
+      </c>
+      <c r="U105" t="inlineStr">
+        <is>
+          <t>(0.6680066550828562, array([[2328, 2814],
+       [2935, 1209],
+       [4008, 1614],
+       [3401, 3220]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="106">
@@ -7569,10 +8089,15 @@
         <v>0.022354625</v>
       </c>
       <c r="T106" t="n">
-        <v>0.9191574907157033</v>
-      </c>
-      <c r="U106" t="n">
-        <v>0.9193502346969963</v>
+        <v>47.2264</v>
+      </c>
+      <c r="U106" t="inlineStr">
+        <is>
+          <t>(0.9186776390395036, array([[2164, 1805],
+       [3042, 1230],
+       [3669, 2184],
+       [2791, 2760]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="107">
@@ -7636,10 +8161,15 @@
         <v>0.024717625</v>
       </c>
       <c r="T107" t="n">
-        <v>0.9382539351851534</v>
-      </c>
-      <c r="U107" t="n">
-        <v>0.9390122050015289</v>
+        <v>41.32511466666666</v>
+      </c>
+      <c r="U107" t="inlineStr">
+        <is>
+          <t>(0.9381340756030845, array([[2546, 1353],
+       [3533, 1227],
+       [3668, 2278],
+       [2681, 2405]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="108">
@@ -7703,10 +8233,15 @@
         <v>0.02660525</v>
       </c>
       <c r="T108" t="n">
-        <v>0.9163021250302159</v>
-      </c>
-      <c r="U108" t="n">
-        <v>0.9156922638918129</v>
+        <v>59.37103466666667</v>
+      </c>
+      <c r="U108" t="inlineStr">
+        <is>
+          <t>(0.9154671334806379, array([[2685, 2245],
+       [2982, 1235],
+       [4084, 1560],
+       [3787, 2569]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="109">
@@ -7770,10 +8305,15 @@
         <v>0.023532875</v>
       </c>
       <c r="T109" t="n">
-        <v>0.958895653698288</v>
-      </c>
-      <c r="U109" t="n">
-        <v>0.958895653698288</v>
+        <v>65.11604266666667</v>
+      </c>
+      <c r="U109" t="inlineStr">
+        <is>
+          <t>(0.958895653698288, array([[2025, 2090],
+       [2919, 1329],
+       [3713, 2261],
+       [2819, 3022]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="110">
@@ -7837,10 +8377,15 @@
         <v>0.02349525</v>
       </c>
       <c r="T110" t="n">
-        <v>0</v>
-      </c>
-      <c r="U110" t="n">
-        <v>0</v>
+        <v>71.24863999999999</v>
+      </c>
+      <c r="U110" t="inlineStr">
+        <is>
+          <t>(0.9221736039376568, array([[2062, 1774],
+       [3090, 1453],
+       [3386, 2401],
+       [2358, 2722]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="111">
@@ -7904,10 +8449,15 @@
         <v>0.03651925</v>
       </c>
       <c r="T111" t="n">
-        <v>0.7541469194681832</v>
-      </c>
-      <c r="U111" t="n">
-        <v>0.7542211236367233</v>
+        <v>31.547192</v>
+      </c>
+      <c r="U111" t="inlineStr">
+        <is>
+          <t>(0.753836825228226, array([[1967, 1838],
+       [2624,  758],
+       [4057, 1629],
+       [3399, 2709]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="112">
@@ -7971,10 +8521,15 @@
         <v>0.008553</v>
       </c>
       <c r="T112" t="n">
-        <v>0</v>
-      </c>
-      <c r="U112" t="n">
-        <v>0</v>
+        <v>58.89546666666666</v>
+      </c>
+      <c r="U112" t="inlineStr">
+        <is>
+          <t>(0.6858984726615991, array([[2572, 1513],
+       [3371, 1385],
+       [3459, 1933],
+       [2660, 2061]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="113">
@@ -8038,10 +8593,15 @@
         <v>0.019336625</v>
       </c>
       <c r="T113" t="n">
-        <v>0</v>
-      </c>
-      <c r="U113" t="n">
-        <v>0</v>
+        <v>59.34085866666667</v>
+      </c>
+      <c r="U113" t="inlineStr">
+        <is>
+          <t>(0.9637714137815512, array([[2104, 1568],
+       [2950,  999],
+       [3539, 1876],
+       [2694, 2444]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="114">
@@ -8105,10 +8665,15 @@
         <v>0.02837670833333333</v>
       </c>
       <c r="T114" t="n">
-        <v>0.7912560822840621</v>
-      </c>
-      <c r="U114" t="n">
-        <v>0.7912560822840621</v>
+        <v>59.76681066666666</v>
+      </c>
+      <c r="U114" t="inlineStr">
+        <is>
+          <t>(0.7912560822840621, array([[2256, 2517],
+       [3015, 1961],
+       [3718, 2920],
+       [2959, 3476]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="115">
@@ -8172,10 +8737,15 @@
         <v>0.020289625</v>
       </c>
       <c r="T115" t="n">
-        <v>0.9011516671518695</v>
-      </c>
-      <c r="U115" t="n">
-        <v>0.9007335880949791</v>
+        <v>35.4024</v>
+      </c>
+      <c r="U115" t="inlineStr">
+        <is>
+          <t>(0.9003383482850029, array([[1733, 2356],
+       [2196, 1499],
+       [3148, 2012],
+       [2685, 2870]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="116">
@@ -8239,10 +8809,15 @@
         <v>0.03662225</v>
       </c>
       <c r="T116" t="n">
-        <v>0.2857142857142858</v>
-      </c>
-      <c r="U116" t="n">
-        <v>0.2857142857142858</v>
+        <v>26.14265866666667</v>
+      </c>
+      <c r="U116" t="inlineStr">
+        <is>
+          <t>(0.8570481054282094, array([[  23, 3909],
+       [  66, 2447],
+       [1319, 2484],
+       [1276, 3946]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="117">
@@ -8306,10 +8881,15 @@
         <v>0.06901879166666666</v>
       </c>
       <c r="T117" t="n">
-        <v>0.1033808516690532</v>
-      </c>
-      <c r="U117" t="n">
-        <v>0.1033808516690532</v>
+        <v>34.11153333333333</v>
+      </c>
+      <c r="U117" t="inlineStr">
+        <is>
+          <t>(0.6730519441570973, array([[1258, 2115],
+       [1760,  690],
+       [3876, 1435],
+       [3375, 2860]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="118">
@@ -8373,10 +8953,15 @@
         <v>0.03745425</v>
       </c>
       <c r="T118" t="n">
-        <v>0.7465704888100302</v>
-      </c>
-      <c r="U118" t="n">
-        <v>0.7465742663190291</v>
+        <v>28.135544</v>
+      </c>
+      <c r="U118" t="inlineStr">
+        <is>
+          <t>(0.7461588758057693, array([[2121, 1886],
+       [2763, 1019],
+       [3924, 1878],
+       [3283, 2745]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="119">
@@ -8440,10 +9025,15 @@
         <v>0.034826875</v>
       </c>
       <c r="T119" t="n">
-        <v>0.8832521759737265</v>
-      </c>
-      <c r="U119" t="n">
-        <v>0.8832521759737265</v>
+        <v>52.18878933333333</v>
+      </c>
+      <c r="U119" t="inlineStr">
+        <is>
+          <t>(0.8832521759737265, array([[1973, 1348],
+       [3037,  838],
+       [3487, 1778],
+       [2423, 2288]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="120">
@@ -8507,10 +9097,15 @@
         <v>0.02162304166666667</v>
       </c>
       <c r="T120" t="n">
-        <v>0.9500274076081913</v>
-      </c>
-      <c r="U120" t="n">
-        <v>0.9500274076081913</v>
+        <v>60.870224</v>
+      </c>
+      <c r="U120" t="inlineStr">
+        <is>
+          <t>(0.9500274076081913, array([[2551, 2486],
+       [3034, 1654],
+       [3910, 2162],
+       [3427, 2994]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="121">
@@ -8574,10 +9169,15 @@
         <v>0.0633095</v>
       </c>
       <c r="T121" t="n">
-        <v>0.8888787697627003</v>
-      </c>
-      <c r="U121" t="n">
-        <v>0.8885890640650879</v>
+        <v>72.40114666666666</v>
+      </c>
+      <c r="U121" t="inlineStr">
+        <is>
+          <t>(0.8884167117185933, array([[1412, 2685],
+       [2098, 1049],
+       [3938, 1822],
+       [3252, 3457]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="122">
@@ -8641,10 +9241,15 @@
         <v>0.02710066666666667</v>
       </c>
       <c r="T122" t="n">
-        <v>0</v>
-      </c>
-      <c r="U122" t="n">
-        <v>0</v>
+        <v>66.99020266666666</v>
+      </c>
+      <c r="U122" t="inlineStr">
+        <is>
+          <t>(0.6950579082297214, array([[2538, 1719],
+       [4240, 1562],
+       [4349, 2745],
+       [2647, 2902]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="123">
@@ -8708,10 +9313,15 @@
         <v>0.010833</v>
       </c>
       <c r="T123" t="n">
-        <v>0.969179462332034</v>
-      </c>
-      <c r="U123" t="n">
-        <v>0.969179462332034</v>
+        <v>35.460672</v>
+      </c>
+      <c r="U123" t="inlineStr">
+        <is>
+          <t>(0.969179462332034, array([[2596, 1640],
+       [3058, 1159],
+       [3554, 1636],
+       [3092, 2117]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="124">
@@ -8775,10 +9385,15 @@
         <v>0.01604379166666667</v>
       </c>
       <c r="T124" t="n">
-        <v>0</v>
-      </c>
-      <c r="U124" t="n">
-        <v>0</v>
+        <v>49.00270933333334</v>
+      </c>
+      <c r="U124" t="inlineStr">
+        <is>
+          <t>(0.6200077396016714, array([[2176, 2257],
+       [2317, 1518],
+       [3509, 1745],
+       [3368, 2484]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="125">
@@ -8842,10 +9457,15 @@
         <v>0.012324125</v>
       </c>
       <c r="T125" t="n">
-        <v>0</v>
-      </c>
-      <c r="U125" t="n">
-        <v>0</v>
+        <v>39.66750133333333</v>
+      </c>
+      <c r="U125" t="inlineStr">
+        <is>
+          <t>(0.8658994907986438, array([[2729, 1767],
+       [3587, 1628],
+       [3707, 2371],
+       [2850, 2510]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="126">
@@ -8909,10 +9529,15 @@
         <v>0.013546875</v>
       </c>
       <c r="T126" t="n">
-        <v>0.9651904387334862</v>
-      </c>
-      <c r="U126" t="n">
-        <v>0.9651904387334862</v>
+        <v>41.34861866666667</v>
+      </c>
+      <c r="U126" t="inlineStr">
+        <is>
+          <t>(0.9651904387334862, array([[2616, 1451],
+       [3257,  770],
+       [3914, 1389],
+       [3273, 2070]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="127">
@@ -8976,10 +9601,15 @@
         <v>0.006400375</v>
       </c>
       <c r="T127" t="n">
-        <v>0.984326639799061</v>
-      </c>
-      <c r="U127" t="n">
-        <v>0.984326639799061</v>
+        <v>52.13469866666667</v>
+      </c>
+      <c r="U127" t="inlineStr">
+        <is>
+          <t>(0.984326639799061, array([[2399, 2553],
+       [2837, 2299],
+       [3095, 2744],
+       [2657, 2998]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="128">
@@ -9043,10 +9673,15 @@
         <v>0.013624</v>
       </c>
       <c r="T128" t="n">
-        <v>0.8101865125590416</v>
-      </c>
-      <c r="U128" t="n">
-        <v>0.8101865125590416</v>
+        <v>26.78416533333333</v>
+      </c>
+      <c r="U128" t="inlineStr">
+        <is>
+          <t>(0.8101865125590416, array([[2635, 1410],
+       [3331, 1358],
+       [3396, 2217],
+       [2700, 2269]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="129">
@@ -9110,10 +9745,15 @@
         <v>0.03511875</v>
       </c>
       <c r="T129" t="n">
-        <v>0.7897920072045305</v>
-      </c>
-      <c r="U129" t="n">
-        <v>0.7892555963012582</v>
+        <v>34.945792</v>
+      </c>
+      <c r="U129" t="inlineStr">
+        <is>
+          <t>(0.7890837939401463, array([[2446, 3015],
+       [2842, 1725],
+       [3861, 2038],
+       [3464, 3328]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="130">
@@ -9177,10 +9817,15 @@
         <v>0.016076375</v>
       </c>
       <c r="T130" t="n">
-        <v>0.9857988165680474</v>
-      </c>
-      <c r="U130" t="n">
-        <v>0.9857988165680474</v>
+        <v>57.03722666666667</v>
+      </c>
+      <c r="U130" t="inlineStr">
+        <is>
+          <t>(0.9857988165680474, array([[2316, 1710],
+       [3161, 1710],
+       [3161, 2543],
+       [2316, 2543]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="131">
@@ -9244,10 +9889,15 @@
         <v>0.0360285</v>
       </c>
       <c r="T131" t="n">
-        <v>0.8442267362743272</v>
-      </c>
-      <c r="U131" t="n">
-        <v>0.8444465067573651</v>
+        <v>41.244312</v>
+      </c>
+      <c r="U131" t="inlineStr">
+        <is>
+          <t>(0.8439169642834791, array([[1904, 2862],
+       [2438, 1780],
+       [3720, 2413],
+       [3185, 3495]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="132">
@@ -9311,10 +9961,15 @@
         <v>0.02317775</v>
       </c>
       <c r="T132" t="n">
-        <v>0.833792982828481</v>
-      </c>
-      <c r="U132" t="n">
-        <v>0.833792982828481</v>
+        <v>42.25391466666667</v>
+      </c>
+      <c r="U132" t="inlineStr">
+        <is>
+          <t>(0.833792982828481, array([[2847, 2608],
+       [2919, 1525],
+       [3822, 1585],
+       [3750, 2668]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="133">
@@ -9378,10 +10033,15 @@
         <v>0.019377375</v>
       </c>
       <c r="T133" t="n">
-        <v>0.7851095020508974</v>
-      </c>
-      <c r="U133" t="n">
-        <v>0.7851095020508974</v>
+        <v>34.364488</v>
+      </c>
+      <c r="U133" t="inlineStr">
+        <is>
+          <t>(0.7851095020508974, array([[2259, 2292],
+       [2529, 1426],
+       [3632, 1770],
+       [3362, 2636]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="134">
@@ -9445,10 +10105,15 @@
         <v>0.04788425</v>
       </c>
       <c r="T134" t="n">
-        <v>0.02352941176470588</v>
-      </c>
-      <c r="U134" t="n">
-        <v>0.02352941176470588</v>
+        <v>40.901712</v>
+      </c>
+      <c r="U134" t="inlineStr">
+        <is>
+          <t>(0.8377579189795478, array([[2361, 2034],
+       [3681, 1223],
+       [4361, 2329],
+       [3041, 3141]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="135">
@@ -9512,10 +10177,15 @@
         <v>0.01381341666666667</v>
       </c>
       <c r="T135" t="n">
-        <v>0</v>
-      </c>
-      <c r="U135" t="n">
-        <v>0</v>
+        <v>50.91778666666666</v>
+      </c>
+      <c r="U135" t="inlineStr">
+        <is>
+          <t>(0.7158113180744468, array([[2691, 1557],
+       [3662, 1331],
+       [3824, 2026],
+       [2853, 2252]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="136">
@@ -9579,10 +10249,15 @@
         <v>0.04341616666666667</v>
       </c>
       <c r="T136" t="n">
-        <v>0.6738931125912325</v>
-      </c>
-      <c r="U136" t="n">
-        <v>0.6738931125912325</v>
+        <v>47.44738133333333</v>
+      </c>
+      <c r="U136" t="inlineStr">
+        <is>
+          <t>(0.6738931125912325, array([[1977, 2345],
+       [3421, 1933],
+       [3699, 2906],
+       [2255, 3318]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="137">
@@ -9646,10 +10321,15 @@
         <v>0.038485875</v>
       </c>
       <c r="T137" t="n">
-        <v>0.8245417586345913</v>
-      </c>
-      <c r="U137" t="n">
-        <v>0.8248651225923652</v>
+        <v>46.09085333333334</v>
+      </c>
+      <c r="U137" t="inlineStr">
+        <is>
+          <t>(0.8241021792545831, array([[2198, 2005],
+       [3270, 1623],
+       [3733, 2924],
+       [2660, 3305]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="138">
@@ -9713,10 +10393,15 @@
         <v>0.0401345</v>
       </c>
       <c r="T138" t="n">
-        <v>0</v>
-      </c>
-      <c r="U138" t="n">
-        <v>0</v>
+        <v>46.59665066666667</v>
+      </c>
+      <c r="U138" t="inlineStr">
+        <is>
+          <t>(0.8882405077984863, array([[2279, 1952],
+       [3503, 1528],
+       [3979, 2905],
+       [2756, 3329]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="139">
@@ -9780,10 +10465,15 @@
         <v>0.007721125</v>
       </c>
       <c r="T139" t="n">
-        <v>0.2857142857142858</v>
-      </c>
-      <c r="U139" t="n">
-        <v>0.2857142857142858</v>
+        <v>64.008912</v>
+      </c>
+      <c r="U139" t="inlineStr">
+        <is>
+          <t>(0.8809670145039596, array([[2307, 2332],
+       [2445, 1882],
+       [2955, 2037],
+       [2818, 2488]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="140">
@@ -9847,10 +10537,15 @@
         <v>0.022474</v>
       </c>
       <c r="T140" t="n">
-        <v>0.7489459828139958</v>
-      </c>
-      <c r="U140" t="n">
-        <v>0.7489459828139958</v>
+        <v>30.77593866666667</v>
+      </c>
+      <c r="U140" t="inlineStr">
+        <is>
+          <t>(0.7489459828139958, array([[1854, 2178],
+       [2151, 1050],
+       [3657, 1447],
+       [3360, 2575]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="141">
@@ -9914,10 +10609,15 @@
         <v>0.032730125</v>
       </c>
       <c r="T141" t="n">
-        <v>0.6318293712569086</v>
-      </c>
-      <c r="U141" t="n">
-        <v>0.6318293712569086</v>
+        <v>43.42771466666667</v>
+      </c>
+      <c r="U141" t="inlineStr">
+        <is>
+          <t>(0.6318293712569086, array([[2761, 2477],
+       [4442, 1667],
+       [4954, 2729],
+       [3273, 3539]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="142">
@@ -9981,10 +10681,15 @@
         <v>0.02533125</v>
       </c>
       <c r="T142" t="n">
-        <v>0.2317736142542175</v>
-      </c>
-      <c r="U142" t="n">
-        <v>0.2317736142542175</v>
+        <v>44.43474133333333</v>
+      </c>
+      <c r="U142" t="inlineStr">
+        <is>
+          <t>(0.8377066935147247, array([[2822, 1637],
+       [3899, 1178],
+       [4284, 2080],
+       [3207, 2539]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="143">
@@ -10048,10 +10753,15 @@
         <v>0.029271</v>
       </c>
       <c r="T143" t="n">
-        <v>0.8331038403154448</v>
-      </c>
-      <c r="U143" t="n">
-        <v>0.8331038403154448</v>
+        <v>46.012032</v>
+      </c>
+      <c r="U143" t="inlineStr">
+        <is>
+          <t>(0.8331038403154448, array([[2017, 1916],
+       [2512,  963],
+       [3656, 1557],
+       [3161, 2510]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="144">
@@ -10115,10 +10825,15 @@
         <v>0.0130305</v>
       </c>
       <c r="T144" t="n">
-        <v>0.6237636228179618</v>
-      </c>
-      <c r="U144" t="n">
-        <v>0.6240376183941498</v>
+        <v>43.71890933333334</v>
+      </c>
+      <c r="U144" t="inlineStr">
+        <is>
+          <t>(0.6234405607903093, array([[2652, 1617],
+       [3590, 1300],
+       [3787, 1885],
+       [2850, 2202]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="145">
@@ -10182,10 +10897,15 @@
         <v>0.026777</v>
       </c>
       <c r="T145" t="n">
-        <v>0.9202824572296485</v>
-      </c>
-      <c r="U145" t="n">
-        <v>0.9196127625331444</v>
+        <v>51.56782933333334</v>
+      </c>
+      <c r="U145" t="inlineStr">
+        <is>
+          <t>(0.9194253201681456, array([[2182, 2448],
+       [2444, 1344],
+       [3460, 1586],
+       [3197, 2690]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="146">
@@ -10249,10 +10969,15 @@
         <v>0.01677391666666667</v>
       </c>
       <c r="T146" t="n">
-        <v>0</v>
-      </c>
-      <c r="U146" t="n">
-        <v>0</v>
+        <v>49.76656</v>
+      </c>
+      <c r="U146" t="inlineStr">
+        <is>
+          <t>(0.41505850167974323, array([[1667, 1589],
+       [1907, 1097],
+       [3092, 1676],
+       [2851, 2168]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="147">
@@ -10316,10 +11041,15 @@
         <v>0.026699625</v>
       </c>
       <c r="T147" t="n">
-        <v>0.5152806090169156</v>
-      </c>
-      <c r="U147" t="n">
-        <v>0.5152806090169156</v>
+        <v>68.44891200000001</v>
+      </c>
+      <c r="U147" t="inlineStr">
+        <is>
+          <t>(0.5152806090169156, array([[2414, 1642],
+       [3990, 1418],
+       [4106, 2230],
+       [2530, 2454]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="148">
@@ -10383,10 +11113,15 @@
         <v>0.01730241666666667</v>
       </c>
       <c r="T148" t="n">
-        <v>0.6542946751968977</v>
-      </c>
-      <c r="U148" t="n">
-        <v>0.6542946751968977</v>
+        <v>38.92284</v>
+      </c>
+      <c r="U148" t="inlineStr">
+        <is>
+          <t>(0.6542946751968977, array([[2329, 1522],
+       [2914, 1265],
+       [3307, 2159],
+       [2722, 2416]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="149">
@@ -10450,10 +11185,15 @@
         <v>0.008178208333333332</v>
       </c>
       <c r="T149" t="n">
-        <v>0.712482240190723</v>
-      </c>
-      <c r="U149" t="n">
-        <v>0.712482240190723</v>
+        <v>42.766216</v>
+      </c>
+      <c r="U149" t="inlineStr">
+        <is>
+          <t>(0.712482240190723, array([[2793, 2285],
+       [2814, 1652],
+       [3265, 1667],
+       [3244, 2300]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="150">
@@ -10517,10 +11257,15 @@
         <v>0.0129755</v>
       </c>
       <c r="T150" t="n">
-        <v>0.7738993253501172</v>
-      </c>
-      <c r="U150" t="n">
-        <v>0.7738993253501172</v>
+        <v>25.47427466666667</v>
+      </c>
+      <c r="U150" t="inlineStr">
+        <is>
+          <t>(0.7738993253501172, array([[3718, 1998],
+       [4357, 1381],
+       [4834, 1876],
+       [4195, 2493]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="151">
@@ -10584,10 +11329,15 @@
         <v>0.03939170833333333</v>
       </c>
       <c r="T151" t="n">
-        <v>0.9142440586137702</v>
-      </c>
-      <c r="U151" t="n">
-        <v>0.9142255057134479</v>
+        <v>27.856768</v>
+      </c>
+      <c r="U151" t="inlineStr">
+        <is>
+          <t>(0.9138271008846776, array([[2575, 1296],
+       [3670,  248],
+       [4816, 1446],
+       [3721, 2493]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="152">
@@ -10651,10 +11401,15 @@
         <v>0.007349916666666667</v>
       </c>
       <c r="T152" t="n">
-        <v>0</v>
-      </c>
-      <c r="U152" t="n">
-        <v>0</v>
+        <v>27.19453333333333</v>
+      </c>
+      <c r="U152" t="inlineStr">
+        <is>
+          <t>(0.6941425774048618, array([[2684, 1744],
+       [2921, 1226],
+       [3666, 1567],
+       [3429, 2084]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="153">
@@ -10718,10 +11473,15 @@
         <v>0.1181235</v>
       </c>
       <c r="T153" t="n">
-        <v>0.9518004837020029</v>
-      </c>
-      <c r="U153" t="n">
-        <v>0.9518004837020029</v>
+        <v>57.44512533333333</v>
+      </c>
+      <c r="U153" t="inlineStr">
+        <is>
+          <t>(0.9518004837020029, array([[1293, 1013],
+       [3406,  441],
+       [3951, 2452],
+       [1838, 3024]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="154">
@@ -10785,10 +11545,15 @@
         <v>0.0686645</v>
       </c>
       <c r="T154" t="n">
-        <v>0.4429407957906277</v>
-      </c>
-      <c r="U154" t="n">
-        <v>0.4429407957906277</v>
+        <v>86.539536</v>
+      </c>
+      <c r="U154" t="inlineStr">
+        <is>
+          <t>(0.4429407957906277, array([[2190,  867],
+       [3386,  696],
+       [3773, 3396],
+       [2577, 3567]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="155">
@@ -10852,10 +11617,15 @@
         <v>0.07400491666666667</v>
       </c>
       <c r="T155" t="n">
-        <v>0.5007451229336447</v>
-      </c>
-      <c r="U155" t="n">
-        <v>0.5007117191972243</v>
+        <v>68.219168</v>
+      </c>
+      <c r="U155" t="inlineStr">
+        <is>
+          <t>(0.5005852361946254, array([[2041, 2580],
+       [3830, -245],
+       [5245,  650],
+       [3456, 3476]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="156">
@@ -10919,10 +11689,15 @@
         <v>0.022765875</v>
       </c>
       <c r="T156" t="n">
-        <v>0</v>
-      </c>
-      <c r="U156" t="n">
-        <v>0</v>
+        <v>54.56769066666666</v>
+      </c>
+      <c r="U156" t="inlineStr">
+        <is>
+          <t>(0.6255612752874432, array([[2357, 2343],
+       [2458,  981],
+       [3311, 1045],
+       [3209, 2407]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="157">
@@ -10986,10 +11761,15 @@
         <v>0.02250479166666667</v>
       </c>
       <c r="T157" t="n">
-        <v>0</v>
-      </c>
-      <c r="U157" t="n">
-        <v>0</v>
+        <v>52.26304</v>
+      </c>
+      <c r="U157" t="inlineStr">
+        <is>
+          <t>(0.9583789139810158, array([[2263, 2684],
+       [2419, 1697],
+       [3365, 1846],
+       [3209, 2833]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="158">
@@ -11053,10 +11833,15 @@
         <v>0.02347975</v>
       </c>
       <c r="T158" t="n">
-        <v>0.8842448086589791</v>
-      </c>
-      <c r="U158" t="n">
-        <v>0.8842448086589791</v>
+        <v>60.53091733333333</v>
+      </c>
+      <c r="U158" t="inlineStr">
+        <is>
+          <t>(0.8842448086589791, array([[2332,  926],
+       [3432,  735],
+       [3648, 1979],
+       [2548, 2170]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="159">
@@ -11120,10 +11905,15 @@
         <v>0.02035591666666667</v>
       </c>
       <c r="T159" t="n">
-        <v>0.7943055594319675</v>
-      </c>
-      <c r="U159" t="n">
-        <v>0.7943055594319675</v>
+        <v>48.30657066666667</v>
+      </c>
+      <c r="U159" t="inlineStr">
+        <is>
+          <t>(0.7943055594319675, array([[2371, 1482],
+       [3645, 1255],
+       [3825, 2267],
+       [2551, 2494]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="160">
@@ -11187,10 +11977,15 @@
         <v>0.02675120833333333</v>
       </c>
       <c r="T160" t="n">
-        <v>0.8764027528892024</v>
-      </c>
-      <c r="U160" t="n">
-        <v>0.8764027528892024</v>
+        <v>40.06544</v>
+      </c>
+      <c r="U160" t="inlineStr">
+        <is>
+          <t>(0.8764027528892024, array([[2401, 1478],
+       [3695, 1104],
+       [4023, 2238],
+       [2729, 2612]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="161">
@@ -11254,10 +12049,15 @@
         <v>0.024148125</v>
       </c>
       <c r="T161" t="n">
-        <v>0.8309308389745385</v>
-      </c>
-      <c r="U161" t="n">
-        <v>0.8314445792673752</v>
+        <v>46.52319466666667</v>
+      </c>
+      <c r="U161" t="inlineStr">
+        <is>
+          <t>(0.8304540805794198, array([[2524, 1283],
+       [3366,  923],
+       [3799, 1935],
+       [2958, 2296]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="162">
@@ -11321,10 +12121,15 @@
         <v>0.006230625</v>
       </c>
       <c r="T162" t="n">
-        <v>0.6860175382333676</v>
-      </c>
-      <c r="U162" t="n">
-        <v>0.6852036400470782</v>
+        <v>71.22851733333333</v>
+      </c>
+      <c r="U162" t="inlineStr">
+        <is>
+          <t>(0.6847912262994035, array([[2511, 2660],
+       [2833, 2003],
+       [3284, 2224],
+       [2961, 2881]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="163">
@@ -11388,10 +12193,15 @@
         <v>0.007295375</v>
       </c>
       <c r="T163" t="n">
-        <v>0.6549766339356375</v>
-      </c>
-      <c r="U163" t="n">
-        <v>0.6549766339356375</v>
+        <v>41.84029066666667</v>
+      </c>
+      <c r="U163" t="inlineStr">
+        <is>
+          <t>(0.6549766339356375, array([[1786, 3342],
+       [1926, 2760],
+       [2815, 2972],
+       [2675, 3554]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="164">
@@ -11455,10 +12265,15 @@
         <v>0.00625025</v>
       </c>
       <c r="T164" t="n">
-        <v>0.9848032652034218</v>
-      </c>
-      <c r="U164" t="n">
-        <v>0.9848032652034218</v>
+        <v>85.18154133333333</v>
+      </c>
+      <c r="U164" t="inlineStr">
+        <is>
+          <t>(0.9848032652034218, array([[2731, 2299],
+       [2965, 1824],
+       [3433, 2054],
+       [3199, 2529]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="165">
@@ -11522,10 +12337,15 @@
         <v>0.020050375</v>
       </c>
       <c r="T165" t="n">
-        <v>0.7144848867483449</v>
-      </c>
-      <c r="U165" t="n">
-        <v>0.7149815258267617</v>
+        <v>37.164144</v>
+      </c>
+      <c r="U165" t="inlineStr">
+        <is>
+          <t>(0.714390386402238, array([[2420, 1313],
+       [3273, 1216],
+       [3409, 2409],
+       [2556, 2507]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="166">
@@ -11589,10 +12409,15 @@
         <v>0.0070325</v>
       </c>
       <c r="T166" t="n">
-        <v>0.773535702346509</v>
-      </c>
-      <c r="U166" t="n">
-        <v>0.773535702346509</v>
+        <v>23.17853866666667</v>
+      </c>
+      <c r="U166" t="inlineStr">
+        <is>
+          <t>(0.773535702346509, array([[2440, 1555],
+       [3116, 1371],
+       [3258, 1894],
+       [2582, 2078]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="167">
@@ -11656,10 +12481,15 @@
         <v>0.01195925</v>
       </c>
       <c r="T167" t="n">
-        <v>0.9441263227228803</v>
-      </c>
-      <c r="U167" t="n">
-        <v>0.9441263227228803</v>
+        <v>39.646144</v>
+      </c>
+      <c r="U167" t="inlineStr">
+        <is>
+          <t>(0.9441263227228803, array([[2216, 1894],
+       [2570, 1194],
+       [3231, 1528],
+       [2877, 2228]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="168">
@@ -11723,10 +12553,15 @@
         <v>0.01148145833333333</v>
       </c>
       <c r="T168" t="n">
-        <v>0</v>
-      </c>
-      <c r="U168" t="n">
-        <v>0</v>
+        <v>30.24366666666667</v>
+      </c>
+      <c r="U168" t="inlineStr">
+        <is>
+          <t>(0.5444398519567942, array([[2277, 1630],
+       [2384,  982],
+       [3573, 1178],
+       [3467, 1826]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="169">
@@ -11790,10 +12625,15 @@
         <v>0.02336666666666667</v>
       </c>
       <c r="T169" t="n">
-        <v>0.7063828565149519</v>
-      </c>
-      <c r="U169" t="n">
-        <v>0.7060641371707909</v>
+        <v>70.681504</v>
+      </c>
+      <c r="U169" t="inlineStr">
+        <is>
+          <t>(0.7057316737201017, array([[1758, 1668],
+       [2766,  940],
+       [3281, 1651],
+       [2273, 2380]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="170">
@@ -11857,10 +12697,15 @@
         <v>0.01638866666666667</v>
       </c>
       <c r="T170" t="n">
-        <v>0</v>
-      </c>
-      <c r="U170" t="n">
-        <v>0</v>
+        <v>24.110872</v>
+      </c>
+      <c r="U170" t="inlineStr">
+        <is>
+          <t>(0.9167652684028362, array([[2261,  697],
+       [3098,  342],
+       [3484, 1254],
+       [2648, 1609]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="171">
@@ -11924,10 +12769,15 @@
         <v>0.003765041666666667</v>
       </c>
       <c r="T171" t="n">
-        <v>0</v>
-      </c>
-      <c r="U171" t="n">
-        <v>0</v>
+        <v>52.28736</v>
+      </c>
+      <c r="U171" t="inlineStr">
+        <is>
+          <t>(0.7260908657670215, array([[3087, 1681],
+       [3406, 1631],
+       [3475, 2068],
+       [3157, 2119]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="172">
@@ -11991,10 +12841,15 @@
         <v>0.0075635</v>
       </c>
       <c r="T172" t="n">
-        <v>0</v>
-      </c>
-      <c r="U172" t="n">
-        <v>0</v>
+        <v>43.55556</v>
+      </c>
+      <c r="U172" t="inlineStr">
+        <is>
+          <t>(0.8630946107646352, array([[2608, 2000],
+       [3207, 1887],
+       [3338, 2581],
+       [2739, 2694]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="173">
@@ -12058,10 +12913,15 @@
         <v>0.01492520833333333</v>
       </c>
       <c r="T173" t="n">
-        <v>0</v>
-      </c>
-      <c r="U173" t="n">
-        <v>0</v>
+        <v>29.25066933333333</v>
+      </c>
+      <c r="U173" t="inlineStr">
+        <is>
+          <t>(0.7441840548535965, array([[2758, 2148],
+       [2784, 1476],
+       [3687, 1511],
+       [3660, 2183]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="174">
@@ -12125,10 +12985,15 @@
         <v>0.022093125</v>
       </c>
       <c r="T174" t="n">
-        <v>0</v>
-      </c>
-      <c r="U174" t="n">
-        <v>0</v>
+        <v>68.85675733333333</v>
+      </c>
+      <c r="U174" t="inlineStr">
+        <is>
+          <t>(0.8072356692661349, array([[1974,  918],
+       [3116,  578],
+       [3390, 1500],
+       [2248, 1840]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="175">
@@ -12192,10 +13057,15 @@
         <v>0.01785545833333333</v>
       </c>
       <c r="T175" t="n">
-        <v>0</v>
-      </c>
-      <c r="U175" t="n">
-        <v>0</v>
+        <v>33.77013066666667</v>
+      </c>
+      <c r="U175" t="inlineStr">
+        <is>
+          <t>(0.9173938526295233, array([[2044, 2115],
+       [2929, 1755],
+       [3259, 2567],
+       [2374, 2927]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="176">
@@ -12259,10 +13129,15 @@
         <v>0.011362125</v>
       </c>
       <c r="T176" t="n">
-        <v>0</v>
-      </c>
-      <c r="U176" t="n">
-        <v>0</v>
+        <v>37.67774133333333</v>
+      </c>
+      <c r="U176" t="inlineStr">
+        <is>
+          <t>(0.9473722018580473, array([[2611, 2372],
+       [2818, 1739],
+       [3486, 1958],
+       [3278, 2591]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="177">
@@ -12326,10 +13201,15 @@
         <v>0.009864166666666667</v>
       </c>
       <c r="T177" t="n">
-        <v>0.7780096022807969</v>
-      </c>
-      <c r="U177" t="n">
-        <v>0.7780096022807969</v>
+        <v>38.171568</v>
+      </c>
+      <c r="U177" t="inlineStr">
+        <is>
+          <t>(0.7780096022807969, array([[2733, 1923],
+       [2809, 1324],
+       [3579, 1421],
+       [3503, 2020]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="178">
@@ -12393,10 +13273,15 @@
         <v>0.008155916666666667</v>
       </c>
       <c r="T178" t="n">
-        <v>0.7861154046316396</v>
-      </c>
-      <c r="U178" t="n">
-        <v>0.7855060660539027</v>
+        <v>41.965352</v>
+      </c>
+      <c r="U178" t="inlineStr">
+        <is>
+          <t>(0.7850522946858017, array([[3039, 2174],
+       [3434, 1448],
+       [4004, 1758],
+       [3610, 2484]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="179">
@@ -12460,10 +13345,15 @@
         <v>0.0080445</v>
       </c>
       <c r="T179" t="n">
-        <v>0.4072513456534986</v>
-      </c>
-      <c r="U179" t="n">
-        <v>0.4072513456534986</v>
+        <v>48.27762666666667</v>
+      </c>
+      <c r="U179" t="inlineStr">
+        <is>
+          <t>(0.826074585224947, array([[2586, 1567],
+       [3328, 1454],
+       [3421, 2068],
+       [2679, 2180]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="180">
@@ -12527,10 +13417,15 @@
         <v>0.00541725</v>
       </c>
       <c r="T180" t="n">
-        <v>0.5832182886765894</v>
-      </c>
-      <c r="U180" t="n">
-        <v>0.5832182886765894</v>
+        <v>62.02737066666667</v>
+      </c>
+      <c r="U180" t="inlineStr">
+        <is>
+          <t>(0.5832182886765894, array([[2556, 1834],
+       [2885, 1802],
+       [2941, 2366],
+       [2612, 2398]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="181">
@@ -12594,10 +13489,15 @@
         <v>0.009457333333333333</v>
       </c>
       <c r="T181" t="n">
-        <v>0.9266836902543422</v>
-      </c>
-      <c r="U181" t="n">
-        <v>0.9259806437496146</v>
+        <v>31.31382933333333</v>
+      </c>
+      <c r="U181" t="inlineStr">
+        <is>
+          <t>(0.925026554254775, array([[2348, 2022],
+       [2513, 1317],
+       [3166, 1469],
+       [3002, 2175]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="182">
@@ -12661,10 +13561,15 @@
         <v>0.0104475</v>
       </c>
       <c r="T182" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="U182" t="n">
-        <v>0.25</v>
+        <v>48.81990933333334</v>
+      </c>
+      <c r="U182" t="inlineStr">
+        <is>
+          <t>(0.9875964546357379, array([[2747, 1683],
+       [3258, 1158],
+       [3790, 1675],
+       [3279, 2200]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="183">
@@ -12728,10 +13633,15 @@
         <v>0.01157</v>
       </c>
       <c r="T183" t="n">
-        <v>0.8092699503871142</v>
-      </c>
-      <c r="U183" t="n">
-        <v>0.8092699503871142</v>
+        <v>57.62716266666666</v>
+      </c>
+      <c r="U183" t="inlineStr">
+        <is>
+          <t>(0.8092699503871142, array([[1888, 2547],
+       [2452, 2334],
+       [2715, 3031],
+       [2151, 3244]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="184">
@@ -12795,10 +13705,15 @@
         <v>0.01658483333333333</v>
       </c>
       <c r="T184" t="n">
-        <v>0.8446601941747572</v>
-      </c>
-      <c r="U184" t="n">
-        <v>0.8446601941747572</v>
+        <v>37.43929333333333</v>
+      </c>
+      <c r="U184" t="inlineStr">
+        <is>
+          <t>(0.8446601941747572, array([[2704, 1944],
+       [3487, 1944],
+       [3487, 2871],
+       [2704, 2871]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="185">
@@ -12862,10 +13777,15 @@
         <v>0.013187375</v>
       </c>
       <c r="T185" t="n">
-        <v>0</v>
-      </c>
-      <c r="U185" t="n">
-        <v>0</v>
+        <v>56.48178666666666</v>
+      </c>
+      <c r="U185" t="inlineStr">
+        <is>
+          <t>(0.7123814922785041, array([[2937, 2083],
+       [3830, 1772],
+       [4052, 2408],
+       [3159, 2719]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="186">
@@ -12929,10 +13849,15 @@
         <v>0.01470125</v>
       </c>
       <c r="T186" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="U186" t="n">
-        <v>0.5</v>
+        <v>29.07110133333333</v>
+      </c>
+      <c r="U186" t="inlineStr">
+        <is>
+          <t>(0.8891428571428571, array([[2766, 2629],
+       [2766, 1851],
+       [3641, 1851],
+       [3641, 2629]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="187">
@@ -12996,10 +13921,15 @@
         <v>0.0093895</v>
       </c>
       <c r="T187" t="n">
-        <v>0.4408138780545868</v>
-      </c>
-      <c r="U187" t="n">
-        <v>0.4399767462665262</v>
+        <v>52.09096</v>
+      </c>
+      <c r="U187" t="inlineStr">
+        <is>
+          <t>(0.43957043342297414, array([[2600, 1444],
+       [2998, 1385],
+       [3131, 2288],
+       [2734, 2346]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="188">
@@ -13063,10 +13993,15 @@
         <v>0.013253875</v>
       </c>
       <c r="T188" t="n">
-        <v>0.9313053112992989</v>
-      </c>
-      <c r="U188" t="n">
-        <v>0.9310418108280122</v>
+        <v>58.010464</v>
+      </c>
+      <c r="U188" t="inlineStr">
+        <is>
+          <t>(0.9302709416562868, array([[2167, 2115],
+       [2756, 1643],
+       [3195, 2192],
+       [2606, 2663]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="189">
@@ -13130,10 +14065,15 @@
         <v>0.01939133333333333</v>
       </c>
       <c r="T189" t="n">
-        <v>0.6031764488452556</v>
-      </c>
-      <c r="U189" t="n">
-        <v>0.6031764488452556</v>
+        <v>35.38577066666667</v>
+      </c>
+      <c r="U189" t="inlineStr">
+        <is>
+          <t>(0.6031764488452556, array([[2660, 2458],
+       [3296, 1380],
+       [3946, 1764],
+       [3310, 2842]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="190">
@@ -13197,10 +14137,15 @@
         <v>0.01255433333333333</v>
       </c>
       <c r="T190" t="n">
-        <v>0.9537002821510464</v>
-      </c>
-      <c r="U190" t="n">
-        <v>0.9529006526703171</v>
+        <v>54.20159466666667</v>
+      </c>
+      <c r="U190" t="inlineStr">
+        <is>
+          <t>(0.9525636972960276, array([[2634, 1814],
+       [3436, 1565],
+       [3674, 2329],
+       [2872, 2579]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="191">
@@ -13264,10 +14209,15 @@
         <v>0.01361541666666667</v>
       </c>
       <c r="T191" t="n">
-        <v>0.9114084686987906</v>
-      </c>
-      <c r="U191" t="n">
-        <v>0.9114084686987906</v>
+        <v>28.12924</v>
+      </c>
+      <c r="U191" t="inlineStr">
+        <is>
+          <t>(0.9114084686987906, array([[2630, 2360],
+       [2706, 1547],
+       [3447, 1616],
+       [3371, 2429]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="192">
@@ -13331,10 +14281,15 @@
         <v>0.02093445833333333</v>
       </c>
       <c r="T192" t="n">
-        <v>0.9456297119162951</v>
-      </c>
-      <c r="U192" t="n">
-        <v>0.9456297119162951</v>
+        <v>30.16310666666667</v>
+      </c>
+      <c r="U192" t="inlineStr">
+        <is>
+          <t>(0.9456297119162951, array([[2405, 2203],
+       [2424, 1265],
+       [3311, 1283],
+       [3292, 2221]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="193">
@@ -13398,10 +14353,15 @@
         <v>0.012116</v>
       </c>
       <c r="T193" t="n">
-        <v>0.9712538023889895</v>
-      </c>
-      <c r="U193" t="n">
-        <v>0.9700559139768462</v>
+        <v>47.546496</v>
+      </c>
+      <c r="U193" t="inlineStr">
+        <is>
+          <t>(0.9699565174047596, array([[3016, 2423],
+       [3077, 1657],
+       [3820, 1716],
+       [3760, 2482]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="194">
@@ -13465,10 +14425,15 @@
         <v>0.009546374999999999</v>
       </c>
       <c r="T194" t="n">
-        <v>0.6566659103480385</v>
-      </c>
-      <c r="U194" t="n">
-        <v>0.6566659103480385</v>
+        <v>46.636784</v>
+      </c>
+      <c r="U194" t="inlineStr">
+        <is>
+          <t>(0.6566659103480385, array([[2834, 1698],
+       [3343, 1594],
+       [3502, 2369],
+       [2993, 2473]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="195">
@@ -13532,10 +14497,15 @@
         <v>0.01780525</v>
       </c>
       <c r="T195" t="n">
-        <v>0.68600219257073</v>
-      </c>
-      <c r="U195" t="n">
-        <v>0.6859835254948921</v>
+        <v>50.02877866666667</v>
+      </c>
+      <c r="U195" t="inlineStr">
+        <is>
+          <t>(0.6853988690210843, array([[2348, 2398],
+       [2901, 1616],
+       [3437, 1996],
+       [2884, 2777]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="196">
@@ -13599,10 +14569,15 @@
         <v>0.009164624999999999</v>
       </c>
       <c r="T196" t="n">
-        <v>0</v>
-      </c>
-      <c r="U196" t="n">
-        <v>0</v>
+        <v>75.35854933333333</v>
+      </c>
+      <c r="U196" t="inlineStr">
+        <is>
+          <t>(0.7485529746548677, array([[2423, 1957],
+       [3199, 1732],
+       [3367, 2313],
+       [2592, 2538]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="197">
@@ -13666,10 +14641,15 @@
         <v>0.01984966666666667</v>
       </c>
       <c r="T197" t="n">
-        <v>0.7581588205752515</v>
-      </c>
-      <c r="U197" t="n">
-        <v>0.7582180933981779</v>
+        <v>35.9966</v>
+      </c>
+      <c r="U197" t="inlineStr">
+        <is>
+          <t>(0.7576549661376324, array([[2086, 2531],
+       [2711, 1609],
+       [3410, 2083],
+       [2785, 3006]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="198">
@@ -13733,10 +14713,15 @@
         <v>0.02193633333333333</v>
       </c>
       <c r="T198" t="n">
-        <v>0.9572619587969877</v>
-      </c>
-      <c r="U198" t="n">
-        <v>0.9572619587969877</v>
+        <v>45.155856</v>
+      </c>
+      <c r="U198" t="inlineStr">
+        <is>
+          <t>(0.9572619587969877, array([[2473, 1243],
+       [3366,  664],
+       [3920, 1519],
+       [3027, 2098]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="199">
@@ -13800,10 +14785,15 @@
         <v>0.020392</v>
       </c>
       <c r="T199" t="n">
-        <v>0.8960848695914926</v>
-      </c>
-      <c r="U199" t="n">
-        <v>0.8960848695914926</v>
+        <v>36.771824</v>
+      </c>
+      <c r="U199" t="inlineStr">
+        <is>
+          <t>(0.8960848695914926, array([[2471, 2060],
+       [2680, 1049],
+       [3586, 1236],
+       [3377, 2247]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="200">
@@ -13867,10 +14857,15 @@
         <v>0.0164825</v>
       </c>
       <c r="T200" t="n">
-        <v>0.7368952052268563</v>
-      </c>
-      <c r="U200" t="n">
-        <v>0.7375020567354351</v>
+        <v>32.858576</v>
+      </c>
+      <c r="U200" t="inlineStr">
+        <is>
+          <t>(0.7367579989400834, array([[2144, 2834],
+       [2277, 1861],
+       [2994, 1959],
+       [2861, 2931]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="201">
@@ -13934,10 +14929,15 @@
         <v>0.01179075</v>
       </c>
       <c r="T201" t="n">
-        <v>0.951931112670104</v>
-      </c>
-      <c r="U201" t="n">
-        <v>0.951931112670104</v>
+        <v>91.003136</v>
+      </c>
+      <c r="U201" t="inlineStr">
+        <is>
+          <t>(0.951931112670104, array([[2755, 1432],
+       [3281,  816],
+       [3868, 1316],
+       [3342, 1932]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="202">
@@ -14001,10 +15001,15 @@
         <v>0.01345133333333333</v>
       </c>
       <c r="T202" t="n">
-        <v>0.813548790364547</v>
-      </c>
-      <c r="U202" t="n">
-        <v>0.8132031779593987</v>
+        <v>44.71149333333334</v>
+      </c>
+      <c r="U202" t="inlineStr">
+        <is>
+          <t>(0.8125979905151278, array([[2473, 2407],
+       [3125, 1896],
+       [3540, 2427],
+       [2888, 2937]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="203">
@@ -14068,10 +15073,15 @@
         <v>0.008527833333333333</v>
       </c>
       <c r="T203" t="n">
-        <v>0.7288493511700294</v>
-      </c>
-      <c r="U203" t="n">
-        <v>0.7294535392558241</v>
+        <v>55.48130133333333</v>
+      </c>
+      <c r="U203" t="inlineStr">
+        <is>
+          <t>(0.7284767528434594, array([[2504, 2409],
+       [2645, 1904],
+       [3337, 2097],
+       [3197, 2602]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="204">
@@ -14135,10 +15145,15 @@
         <v>0.007866333333333333</v>
       </c>
       <c r="T204" t="n">
-        <v>0.7335446670513783</v>
-      </c>
-      <c r="U204" t="n">
-        <v>0.7337233367338828</v>
+        <v>58.03114666666666</v>
+      </c>
+      <c r="U204" t="inlineStr">
+        <is>
+          <t>(0.7324973534983009, array([[2351, 2173],
+       [2469, 1661],
+       [3167, 1821],
+       [3050, 2334]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="205">
@@ -14202,10 +15217,15 @@
         <v>0.01040366666666667</v>
       </c>
       <c r="T205" t="n">
-        <v>0.8199067084661141</v>
-      </c>
-      <c r="U205" t="n">
-        <v>0.8199067084661141</v>
+        <v>55.16712</v>
+      </c>
+      <c r="U205" t="inlineStr">
+        <is>
+          <t>(0.8199067084661141, array([[2812, 2209],
+       [3595, 2132],
+       [3658, 2774],
+       [2875, 2851]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="206">
@@ -14269,10 +15289,15 @@
         <v>0.0114715</v>
       </c>
       <c r="T206" t="n">
-        <v>0.944152701260937</v>
-      </c>
-      <c r="U206" t="n">
-        <v>0.9432833756285637</v>
+        <v>53.950112</v>
+      </c>
+      <c r="U206" t="inlineStr">
+        <is>
+          <t>(0.942993739943042, array([[2850, 2165],
+       [3656, 1951],
+       [3858, 2712],
+       [3052, 2925]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="207">
@@ -14336,10 +15361,15 @@
         <v>0.005916833333333333</v>
       </c>
       <c r="T207" t="n">
-        <v>0</v>
-      </c>
-      <c r="U207" t="n">
-        <v>0</v>
+        <v>70.958544</v>
+      </c>
+      <c r="U207" t="inlineStr">
+        <is>
+          <t>(0.9456322704215387, array([[2292, 1835],
+       [2769, 1557],
+       [3032, 2009],
+       [2555, 2286]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="208">
@@ -14403,10 +15433,15 @@
         <v>0.007962833333333334</v>
       </c>
       <c r="T208" t="n">
-        <v>0.9325383615555682</v>
-      </c>
-      <c r="U208" t="n">
-        <v>0.9325383615555682</v>
+        <v>48.02062933333333</v>
+      </c>
+      <c r="U208" t="inlineStr">
+        <is>
+          <t>(0.9325383615555682, array([[2490, 2262],
+       [2681, 1722],
+       [3260, 1927],
+       [3069, 2467]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="209">
@@ -14470,10 +15505,15 @@
         <v>0.01699683333333333</v>
       </c>
       <c r="T209" t="n">
-        <v>0.7379563731652221</v>
-      </c>
-      <c r="U209" t="n">
-        <v>0.7379563731652221</v>
+        <v>45.95682133333333</v>
+      </c>
+      <c r="U209" t="inlineStr">
+        <is>
+          <t>(0.7379563731652221, array([[2920, 2604],
+       [3169, 1784],
+       [4280, 2122],
+       [4031, 2942]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="210">
@@ -14537,10 +15577,15 @@
         <v>0.0200545</v>
       </c>
       <c r="T210" t="n">
-        <v>0.8110073983357659</v>
-      </c>
-      <c r="U210" t="n">
-        <v>0.8100044670323809</v>
+        <v>34.39473066666667</v>
+      </c>
+      <c r="U210" t="inlineStr">
+        <is>
+          <t>(0.8097869185447385, array([[1633, 1755],
+       [2127,  983],
+       [3081, 1592],
+       [2586, 2365]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="211">
@@ -14604,10 +15649,15 @@
         <v>0.01318483333333333</v>
       </c>
       <c r="T211" t="n">
-        <v>0.5044500656436298</v>
-      </c>
-      <c r="U211" t="n">
-        <v>0.50489281484977</v>
+        <v>30.97504</v>
+      </c>
+      <c r="U211" t="inlineStr">
+        <is>
+          <t>(0.5041880900003409, array([[2242, 1640],
+       [2525, 1225],
+       [3347, 1787],
+       [3063, 2201]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="212">
@@ -14671,10 +15721,15 @@
         <v>0.02632075</v>
       </c>
       <c r="T212" t="n">
-        <v>0.7880457523379308</v>
-      </c>
-      <c r="U212" t="n">
-        <v>0.7880457523379308</v>
+        <v>29.485512</v>
+      </c>
+      <c r="U212" t="inlineStr">
+        <is>
+          <t>(0.7880457523379308, array([[1847, 2209],
+       [2588, 1541],
+       [3436, 2481],
+       [2695, 3149]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="213">
@@ -14738,10 +15793,15 @@
         <v>0.02441283333333333</v>
       </c>
       <c r="T213" t="n">
-        <v>0.7603952973716022</v>
-      </c>
-      <c r="U213" t="n">
-        <v>0.7603952973716022</v>
+        <v>29.324936</v>
+      </c>
+      <c r="U213" t="inlineStr">
+        <is>
+          <t>(0.7603952973716022, array([[2897, 2352],
+       [2991, 1129],
+       [3921, 1200],
+       [3827, 2423]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="214">
@@ -14805,10 +15865,15 @@
         <v>0.02465666666666667</v>
       </c>
       <c r="T214" t="n">
-        <v>0.667525517947171</v>
-      </c>
-      <c r="U214" t="n">
-        <v>0.6668775532938958</v>
+        <v>29.151352</v>
+      </c>
+      <c r="U214" t="inlineStr">
+        <is>
+          <t>(0.6668461665024835, array([[1928, 2385],
+       [1995, 1408],
+       [3460, 1509],
+       [3393, 2487]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="215">
@@ -14872,10 +15937,15 @@
         <v>0.01751033333333333</v>
       </c>
       <c r="T215" t="n">
-        <v>0.5560107741914831</v>
-      </c>
-      <c r="U215" t="n">
-        <v>0.5553348102272287</v>
+        <v>39.71856</v>
+      </c>
+      <c r="U215" t="inlineStr">
+        <is>
+          <t>(0.5553279462851484, array([[1921, 2205],
+       [1936, 1391],
+       [3400, 1418],
+       [3385, 2231]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="216">
@@ -14939,10 +16009,15 @@
         <v>0.0161465</v>
       </c>
       <c r="T216" t="n">
-        <v>0.7792861932483168</v>
-      </c>
-      <c r="U216" t="n">
-        <v>0.7794627317747885</v>
+        <v>34.41254933333333</v>
+      </c>
+      <c r="U216" t="inlineStr">
+        <is>
+          <t>(0.7788116008994862, array([[3336, 2210],
+       [4240, 1696],
+       [4641, 2401],
+       [3736, 2915]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="217">
@@ -15006,10 +16081,15 @@
         <v>0.017729</v>
       </c>
       <c r="T217" t="n">
-        <v>0.6815088379977062</v>
-      </c>
-      <c r="U217" t="n">
-        <v>0.6808633170661057</v>
+        <v>58.01289066666666</v>
+      </c>
+      <c r="U217" t="inlineStr">
+        <is>
+          <t>(0.6806373964371867, array([[2208, 1924],
+       [2890, 1664],
+       [3272, 2666],
+       [2589, 2926]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="218">
@@ -15073,10 +16153,15 @@
         <v>0.00565875</v>
       </c>
       <c r="T218" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="U218" t="n">
-        <v>0.2</v>
+        <v>58.71042133333334</v>
+      </c>
+      <c r="U218" t="inlineStr">
+        <is>
+          <t>(0.46034994430642273, array([[3334, 2498],
+       [3570, 1849],
+       [3869, 1957],
+       [3633, 2606]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="219">
@@ -15140,10 +16225,15 @@
         <v>0.01526616666666667</v>
       </c>
       <c r="T219" t="n">
-        <v>0.5630585898709036</v>
-      </c>
-      <c r="U219" t="n">
-        <v>0.5630585898709036</v>
+        <v>50.23104</v>
+      </c>
+      <c r="U219" t="inlineStr">
+        <is>
+          <t>(0.5630585898709036, array([[2592, 1880],
+       [3159, 1880],
+       [3159, 2887],
+       [2592, 2887]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="220">
@@ -15207,10 +16297,15 @@
         <v>0.006874666666666667</v>
       </c>
       <c r="T220" t="n">
-        <v>0.5329124822428983</v>
-      </c>
-      <c r="U220" t="n">
-        <v>0.53180059351749</v>
+        <v>39.15983733333334</v>
+      </c>
+      <c r="U220" t="inlineStr">
+        <is>
+          <t>(0.5315922763799609, array([[2978, 1727],
+       [3088, 1356],
+       [3784, 1563],
+       [3674, 1933]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="221">
@@ -15274,10 +16369,15 @@
         <v>0.0073725</v>
       </c>
       <c r="T221" t="n">
-        <v>0.3095634919571715</v>
-      </c>
-      <c r="U221" t="n">
-        <v>0.3095634919571715</v>
+        <v>30.98941866666667</v>
+      </c>
+      <c r="U221" t="inlineStr">
+        <is>
+          <t>(0.30956349195717153, array([[3330,  858],
+       [3672,  755],
+       [4004, 1860],
+       [3662, 1963]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="222">
@@ -15341,10 +16441,15 @@
         <v>0.01831016666666667</v>
       </c>
       <c r="T222" t="n">
-        <v>0.8979031180182171</v>
-      </c>
-      <c r="U222" t="n">
-        <v>0.8979031180182171</v>
+        <v>32.23806133333333</v>
+      </c>
+      <c r="U222" t="inlineStr">
+        <is>
+          <t>(0.8979031180182171, array([[2968, 2100],
+       [3412, 1355],
+       [4242, 1849],
+       [3798, 2594]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="223">
@@ -15408,10 +16513,15 @@
         <v>0.01696533333333333</v>
       </c>
       <c r="T223" t="n">
-        <v>0.9090791868361587</v>
-      </c>
-      <c r="U223" t="n">
-        <v>0.9090791868361587</v>
+        <v>31.89033066666667</v>
+      </c>
+      <c r="U223" t="inlineStr">
+        <is>
+          <t>(0.9090791868361587, array([[2775, 2160],
+       [2884, 1290],
+       [3841, 1410],
+       [3732, 2280]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="224">
@@ -15475,10 +16585,15 @@
         <v>0.00476125</v>
       </c>
       <c r="T224" t="n">
-        <v>0.553048345425141</v>
-      </c>
-      <c r="U224" t="n">
-        <v>0.553048345425141</v>
+        <v>43.03270133333334</v>
+      </c>
+      <c r="U224" t="inlineStr">
+        <is>
+          <t>(0.553048345425141, array([[2607, 2261],
+       [2793, 1994],
+       [3276, 2330],
+       [3090, 2597]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="225">
@@ -15542,10 +16657,15 @@
         <v>0.013378</v>
       </c>
       <c r="T225" t="n">
-        <v>0.4678089794754949</v>
-      </c>
-      <c r="U225" t="n">
-        <v>0.4681087731168927</v>
+        <v>33.92915466666667</v>
+      </c>
+      <c r="U225" t="inlineStr">
+        <is>
+          <t>(0.4676848444784646, array([[2860, 1718],
+       [3367, 1648],
+       [3515, 2732],
+       [3008, 2801]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="226">
@@ -15609,10 +16729,15 @@
         <v>0.007123375</v>
       </c>
       <c r="T226" t="n">
-        <v>0.8270045363200609</v>
-      </c>
-      <c r="U226" t="n">
-        <v>0.8272432859722905</v>
+        <v>46.395168</v>
+      </c>
+      <c r="U226" t="inlineStr">
+        <is>
+          <t>(0.8262506207517989, array([[2681, 1759],
+       [2992, 1265],
+       [3589, 1640],
+       [3279, 2134]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="227">
@@ -15676,10 +16801,15 @@
         <v>0.01938683333333333</v>
       </c>
       <c r="T227" t="n">
-        <v>0.9322789803668677</v>
-      </c>
-      <c r="U227" t="n">
-        <v>0.9322789803668677</v>
+        <v>73.214032</v>
+      </c>
+      <c r="U227" t="inlineStr">
+        <is>
+          <t>(0.9322789803668677, array([[2199, 2064],
+       [2948, 1101],
+       [3846, 1799],
+       [3097, 2762]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="228">
@@ -15743,10 +16873,15 @@
         <v>0.01279033333333333</v>
       </c>
       <c r="T228" t="n">
-        <v>0.4581294773671222</v>
-      </c>
-      <c r="U228" t="n">
-        <v>0.4573506742381376</v>
+        <v>42.71416</v>
+      </c>
+      <c r="U228" t="inlineStr">
+        <is>
+          <t>(0.4572781122886502, array([[1767, 2167],
+       [1864, 1647],
+       [2999, 1859],
+       [2902, 2378]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="229">
@@ -15810,10 +16945,15 @@
         <v>0.007454083333333333</v>
       </c>
       <c r="T229" t="n">
-        <v>0</v>
-      </c>
-      <c r="U229" t="n">
-        <v>0</v>
+        <v>74.78309333333333</v>
+      </c>
+      <c r="U229" t="inlineStr">
+        <is>
+          <t>(0.5970262565193875, array([[1600, 2036],
+       [1856, 1658],
+       [2488, 2086],
+       [2232, 2463]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="230">
@@ -15877,10 +17017,15 @@
         <v>0.012707</v>
       </c>
       <c r="T230" t="n">
-        <v>0.4178268296914196</v>
-      </c>
-      <c r="U230" t="n">
-        <v>0.4179487925954684</v>
+        <v>61.71795733333333</v>
+      </c>
+      <c r="U230" t="inlineStr">
+        <is>
+          <t>(0.41760943776586446, array([[2239, 1918],
+       [2367, 1438],
+       [3516, 1746],
+       [3387, 2226]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="231">
@@ -15944,10 +17089,15 @@
         <v>0.01563616666666667</v>
       </c>
       <c r="T231" t="n">
-        <v>0</v>
-      </c>
-      <c r="U231" t="n">
-        <v>0</v>
+        <v>60.57999466666666</v>
+      </c>
+      <c r="U231" t="inlineStr">
+        <is>
+          <t>(0.48234703813057295, array([[2028, 2019],
+       [2202, 1440],
+       [3402, 1802],
+       [3227, 2381]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="232">
@@ -16011,10 +17161,15 @@
         <v>0.04024433333333333</v>
       </c>
       <c r="T232" t="n">
-        <v>0.5436884599184507</v>
-      </c>
-      <c r="U232" t="n">
-        <v>0.5438218995496763</v>
+        <v>48.22080533333333</v>
+      </c>
+      <c r="U232" t="inlineStr">
+        <is>
+          <t>(0.54363429041721, array([[1561, 2754],
+       [1803, 1216],
+       [4631, 1660],
+       [4390, 3198]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="233">
@@ -16078,10 +17233,15 @@
         <v>0.1874578333333333</v>
       </c>
       <c r="T233" t="n">
-        <v>0.7929777781925607</v>
-      </c>
-      <c r="U233" t="n">
-        <v>0.7929479705141201</v>
+        <v>49.7144</v>
+      </c>
+      <c r="U233" t="inlineStr">
+        <is>
+          <t>(0.7927664542342664, array([[1204, 2442],
+       [3562,  265],
+       [5289, 2135],
+       [2930, 4312]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="234">
@@ -16145,10 +17305,15 @@
         <v>0.015821865720477</v>
       </c>
       <c r="T234" t="n">
-        <v>0.6175815311872718</v>
-      </c>
-      <c r="U234" t="n">
-        <v>0.6168306088384395</v>
+        <v>36.58720059998172</v>
+      </c>
+      <c r="U234" t="inlineStr">
+        <is>
+          <t>(0.6164190614013437, array([[2111,  843],
+       [2511,  614],
+       [2882, 1261],
+       [2483, 1490]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="235">
@@ -16212,10 +17377,15 @@
         <v>0.05283633333333333</v>
       </c>
       <c r="T235" t="n">
-        <v>0.2868756090167074</v>
-      </c>
-      <c r="U235" t="n">
-        <v>0.2757485386402535</v>
+        <v>85.77860800000001</v>
+      </c>
+      <c r="U235" t="inlineStr">
+        <is>
+          <t>(0.7884718711488758, array([[1828, 2364],
+       [3351, 1647],
+       [3916, 2848],
+       [2393, 3565]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="236">
@@ -16279,10 +17449,15 @@
         <v>0.0253965</v>
       </c>
       <c r="T236" t="n">
-        <v>0.6370612206189764</v>
-      </c>
-      <c r="U236" t="n">
-        <v>0.6370612206189764</v>
+        <v>41.569992</v>
+      </c>
+      <c r="U236" t="inlineStr">
+        <is>
+          <t>(0.6370612206189764, array([[2141, 1210],
+       [2622,  615],
+       [3556, 1370],
+       [3075, 1965]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="237">
@@ -16346,10 +17521,15 @@
         <v>0.02543833333333333</v>
       </c>
       <c r="T237" t="n">
-        <v>0.5224742523173281</v>
-      </c>
-      <c r="U237" t="n">
-        <v>0.5224742523173281</v>
+        <v>69.109792</v>
+      </c>
+      <c r="U237" t="inlineStr">
+        <is>
+          <t>(0.5224742523173281, array([[2468, 2525],
+       [2489, 1886],
+       [3712, 1927],
+       [3691, 2566]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="238">
@@ -16413,10 +17593,15 @@
         <v>0.0432945</v>
       </c>
       <c r="T238" t="n">
-        <v>0.9900737702402014</v>
-      </c>
-      <c r="U238" t="n">
-        <v>0.9900737702402014</v>
+        <v>45.32157866666667</v>
+      </c>
+      <c r="U238" t="inlineStr">
+        <is>
+          <t>(0.9900737702402014, array([[2117, 2682],
+       [2655, 1503],
+       [3846, 2046],
+       [3308, 3225]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="239">
@@ -16480,10 +17665,15 @@
         <v>0.01983816666666667</v>
       </c>
       <c r="T239" t="n">
-        <v>0.9175162109416977</v>
-      </c>
-      <c r="U239" t="n">
-        <v>0.9177634354937267</v>
+        <v>23.66088266666667</v>
+      </c>
+      <c r="U239" t="inlineStr">
+        <is>
+          <t>(0.9169483807664355, array([[2612, 1898],
+       [3345, 1429],
+       [3856, 2228],
+       [3123, 2696]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="240">
@@ -16547,10 +17737,15 @@
         <v>0.007199416666666666</v>
       </c>
       <c r="T240" t="n">
-        <v>0</v>
-      </c>
-      <c r="U240" t="n">
-        <v>0</v>
+        <v>22.210764</v>
+      </c>
+      <c r="U240" t="inlineStr">
+        <is>
+          <t>(0.9473559954612275, array([[2768, 1697],
+       [3292, 1413],
+       [3592, 1965],
+       [3068, 2250]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="241">
@@ -16614,10 +17809,15 @@
         <v>0.0197255</v>
       </c>
       <c r="T241" t="n">
-        <v>0.9820335505064731</v>
-      </c>
-      <c r="U241" t="n">
-        <v>0.9831098702787999</v>
+        <v>52.74612266666666</v>
+      </c>
+      <c r="U241" t="inlineStr">
+        <is>
+          <t>(0.9820059273730166, array([[2476, 2670],
+       [2497, 1796],
+       [3387, 1818],
+       [3365, 2692]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="242">
@@ -16681,10 +17881,15 @@
         <v>0.03945316666666666</v>
       </c>
       <c r="T242" t="n">
-        <v>0.565078772909978</v>
-      </c>
-      <c r="U242" t="n">
-        <v>0.5649047264810314</v>
+        <v>38.15652266666667</v>
+      </c>
+      <c r="U242" t="inlineStr">
+        <is>
+          <t>(0.5646371958117212, array([[1411,  913],
+       [2049,  318],
+       [3102, 1447],
+       [2464, 2041]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="243">
@@ -16748,10 +17953,15 @@
         <v>0.03404291666666667</v>
       </c>
       <c r="T243" t="n">
-        <v>0.9187294639285984</v>
-      </c>
-      <c r="U243" t="n">
-        <v>0.9185540494712814</v>
+        <v>48.133952</v>
+      </c>
+      <c r="U243" t="inlineStr">
+        <is>
+          <t>(0.9181202316439604, array([[1690, 1651],
+       [2485,  626],
+       [3426, 1356],
+       [2632, 2381]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="244">
@@ -16815,10 +18025,15 @@
         <v>0.03879566666666667</v>
       </c>
       <c r="T244" t="n">
-        <v>0.8172874921962638</v>
-      </c>
-      <c r="U244" t="n">
-        <v>0.8172874921962638</v>
+        <v>44.373016</v>
+      </c>
+      <c r="U244" t="inlineStr">
+        <is>
+          <t>(0.8172874921962638, array([[2435, 1592],
+       [3419, 1225],
+       [3868, 2429],
+       [2884, 2796]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="245">
@@ -16882,10 +18097,15 @@
         <v>0.0403435</v>
       </c>
       <c r="T245" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="U245" t="n">
-        <v>0.1</v>
+        <v>70.29410133333333</v>
+      </c>
+      <c r="U245" t="inlineStr">
+        <is>
+          <t>(0.8346311082716826, array([[1601, 2962],
+       [2531, 1807],
+       [3496, 2583],
+       [2566, 3739]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="246">
@@ -16949,10 +18169,15 @@
         <v>0.02890683333333333</v>
       </c>
       <c r="T246" t="n">
-        <v>0.7725426482534524</v>
-      </c>
-      <c r="U246" t="n">
-        <v>0.7725426482534524</v>
+        <v>60.22644266666666</v>
+      </c>
+      <c r="U246" t="inlineStr">
+        <is>
+          <t>(0.7725426482534524, array([[1224, 1720],
+       [2455, 1720],
+       [2455, 2671],
+       [1224, 2671]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="247">
@@ -17016,10 +18241,15 @@
         <v>0.0365135</v>
       </c>
       <c r="T247" t="n">
-        <v>0.9309140140134954</v>
-      </c>
-      <c r="U247" t="n">
-        <v>0.9309140140134954</v>
+        <v>58.68736</v>
+      </c>
+      <c r="U247" t="inlineStr">
+        <is>
+          <t>(0.9309140140134954, array([[2004, 1678],
+       [2850,  947],
+       [3635, 1856],
+       [2789, 2587]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="248">
@@ -17083,10 +18313,15 @@
         <v>0.038646</v>
       </c>
       <c r="T248" t="n">
-        <v>0.6097637200121846</v>
-      </c>
-      <c r="U248" t="n">
-        <v>0.6097637200121846</v>
+        <v>45.04216533333334</v>
+      </c>
+      <c r="U248" t="inlineStr">
+        <is>
+          <t>(0.6097637200121846, array([[2120, 2329],
+       [2206, 1426],
+       [3687, 1566],
+       [3601, 2469]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="249">
@@ -17150,10 +18385,15 @@
         <v>0.02642116666666667</v>
       </c>
       <c r="T249" t="n">
-        <v>0.7998331943286072</v>
-      </c>
-      <c r="U249" t="n">
-        <v>0.7998331943286072</v>
+        <v>42.05477866666666</v>
+      </c>
+      <c r="U249" t="inlineStr">
+        <is>
+          <t>(0.7998331943286072, array([[2024,  792],
+       [3223,  792],
+       [3223, 1751],
+       [2024, 1751]], dtype=int64))</t>
+        </is>
       </c>
     </row>
     <row r="250">
@@ -17217,10 +18457,15 @@
         <v>0.0363615</v>
       </c>
       <c r="T250" t="n">
-        <v>0.6355576903352136</v>
-      </c>
-      <c r="U250" t="n">
-        <v>0.6354861331063454</v>
+        <v>56.77508266666667</v>
+      </c>
+      <c r="U250" t="inlineStr">
+        <is>
+          <t>(0.6349674006940695, array([[2717, 1718],
+       [3598, 1577],
+       [3820, 2962],
+       [2940, 3104]], dtype=int64))</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Essai updated with working features
Features 2 qui donne un résultat probable et Features 6 à faire encore
</commit_message>
<xml_diff>
--- a/train/grostest.xlsx
+++ b/train/grostest.xlsx
@@ -603,13 +603,8 @@
       <c r="T2" t="n">
         <v>63.63469866666667</v>
       </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>(0.8344859658431969, array([[2700, 2447],
-       [2788, 1937],
-       [3397, 2042],
-       [3310, 2551]], dtype=int64))</t>
-        </is>
+      <c r="U2" t="n">
+        <v>0.8355886904891203</v>
       </c>
     </row>
     <row r="3">
@@ -675,13 +670,8 @@
       <c r="T3" t="n">
         <v>24.83500533333333</v>
       </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>(0.7962118272802876, array([[2248, 2455],
-       [2364, 1732],
-       [3272, 1877],
-       [3156, 2601]], dtype=int64))</t>
-        </is>
+      <c r="U3" t="n">
+        <v>0.7993205968713839</v>
       </c>
     </row>
     <row r="4">
@@ -747,13 +737,8 @@
       <c r="T4" t="n">
         <v>35.06335733333334</v>
       </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>(0.9585903115342803, array([[2246, 2169],
-       [2657, 1253],
-       [3537, 1647],
-       [3125, 2564]], dtype=int64))</t>
-        </is>
+      <c r="U4" t="n">
+        <v>0.9598524141902736</v>
       </c>
     </row>
     <row r="5">
@@ -819,13 +804,8 @@
       <c r="T5" t="n">
         <v>29.05372</v>
       </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>(0.7543906155817381, array([[2247, 1445],
-       [3052, 1077],
-       [3540, 2144],
-       [2735, 2512]], dtype=int64))</t>
-        </is>
+      <c r="U5" t="n">
+        <v>0.7543906155817381</v>
       </c>
     </row>
     <row r="6">
@@ -891,13 +871,8 @@
       <c r="T6" t="n">
         <v>35.49981866666667</v>
       </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>(0.7359358785151086, array([[2122, 1605],
-       [2668,  922],
-       [3596, 1664],
-       [3049, 2347]], dtype=int64))</t>
-        </is>
+      <c r="U6" t="n">
+        <v>0.7364198557790879</v>
       </c>
     </row>
     <row r="7">
@@ -963,13 +938,8 @@
       <c r="T7" t="n">
         <v>39.607296</v>
       </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>(0.8579038102846333, array([[2208, 1840],
-       [2928, 1195],
-       [3679, 2035],
-       [2959, 2680]], dtype=int64))</t>
-        </is>
+      <c r="U7" t="n">
+        <v>0.8579038102846333</v>
       </c>
     </row>
     <row r="8">
@@ -1035,13 +1005,8 @@
       <c r="T8" t="n">
         <v>45.54208</v>
       </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>(0.8187388386661978, array([[2379, 1501],
-       [3445, 1046],
-       [3817, 1920],
-       [2751, 2374]], dtype=int64))</t>
-        </is>
+      <c r="U8" t="n">
+        <v>0.8190159795172345</v>
       </c>
     </row>
     <row r="9">
@@ -1107,13 +1072,8 @@
       <c r="T9" t="n">
         <v>50.93696</v>
       </c>
-      <c r="U9" t="inlineStr">
-        <is>
-          <t>(0.6691586861224738, array([[2658, 2787],
-       [2695, 1723],
-       [3408, 1748],
-       [3370, 2812]], dtype=int64))</t>
-        </is>
+      <c r="U9" t="n">
+        <v>0.6691808244643215</v>
       </c>
     </row>
     <row r="10">
@@ -1179,13 +1139,8 @@
       <c r="T10" t="n">
         <v>53.355648</v>
       </c>
-      <c r="U10" t="inlineStr">
-        <is>
-          <t>(0.9882616985197341, array([[2022, 1885],
-       [2501,  816],
-       [3582, 1299],
-       [3104, 2368]], dtype=int64))</t>
-        </is>
+      <c r="U10" t="n">
+        <v>0.9890238293208667</v>
       </c>
     </row>
     <row r="11">
@@ -1251,13 +1206,8 @@
       <c r="T11" t="n">
         <v>47.788832</v>
       </c>
-      <c r="U11" t="inlineStr">
-        <is>
-          <t>(0.8964401294498382, array([[2080,  776],
-       [2911,  776],
-       [2911, 1703],
-       [2080, 1703]], dtype=int64))</t>
-        </is>
+      <c r="U11" t="n">
+        <v>0.8964401294498382</v>
       </c>
     </row>
     <row r="12">
@@ -1323,13 +1273,8 @@
       <c r="T12" t="n">
         <v>47.75181333333333</v>
       </c>
-      <c r="U12" t="inlineStr">
-        <is>
-          <t>(0.7131949790335453, array([[2431, 1583],
-       [3205, 1169],
-       [3501, 1721],
-       [2727, 2136]], dtype=int64))</t>
-        </is>
+      <c r="U12" t="n">
+        <v>0.7135785618796932</v>
       </c>
     </row>
     <row r="13">
@@ -1395,13 +1340,8 @@
       <c r="T13" t="n">
         <v>47.82069333333333</v>
       </c>
-      <c r="U13" t="inlineStr">
-        <is>
-          <t>(0.9489804286761476, array([[1681, 2326],
-       [2612, 1217],
-       [3664, 2101],
-       [2733, 3210]], dtype=int64))</t>
-        </is>
+      <c r="U13" t="n">
+        <v>0.9489804286761476</v>
       </c>
     </row>
     <row r="14">
@@ -1467,13 +1407,8 @@
       <c r="T14" t="n">
         <v>27.574448</v>
       </c>
-      <c r="U14" t="inlineStr">
-        <is>
-          <t>(0.9287900100947079, array([[2415, 1918],
-       [3132, 1849],
-       [3206, 2621],
-       [2489, 2690]], dtype=int64))</t>
-        </is>
+      <c r="U14" t="n">
+        <v>0.9301190801726968</v>
       </c>
     </row>
     <row r="15">
@@ -1539,13 +1474,8 @@
       <c r="T15" t="n">
         <v>54.15048</v>
       </c>
-      <c r="U15" t="inlineStr">
-        <is>
-          <t>(0.9439346115807731, array([[2352, 1934],
-       [2764, 1204],
-       [3536, 1641],
-       [3124, 2370]], dtype=int64))</t>
-        </is>
+      <c r="U15" t="n">
+        <v>0.9444586207461122</v>
       </c>
     </row>
     <row r="16">
@@ -1611,13 +1541,8 @@
       <c r="T16" t="n">
         <v>51.95069866666667</v>
       </c>
-      <c r="U16" t="inlineStr">
-        <is>
-          <t>(0.796182235782607, array([[2112, 1677],
-       [2577, 1056],
-       [3357, 1640],
-       [2891, 2261]], dtype=int64))</t>
-        </is>
+      <c r="U16" t="n">
+        <v>0.7968367046524801</v>
       </c>
     </row>
     <row r="17">
@@ -1683,13 +1608,8 @@
       <c r="T17" t="n">
         <v>56.67906666666666</v>
       </c>
-      <c r="U17" t="inlineStr">
-        <is>
-          <t>(0.9198465952997077, array([[1913, 1962],
-       [2453,  918],
-       [3588, 1505],
-       [3048, 2549]], dtype=int64))</t>
-        </is>
+      <c r="U17" t="n">
+        <v>0.9198465952997077</v>
       </c>
     </row>
     <row r="18">
@@ -1755,13 +1675,8 @@
       <c r="T18" t="n">
         <v>42.42048533333333</v>
       </c>
-      <c r="U18" t="inlineStr">
-        <is>
-          <t>(0.6805910718674436, array([[2528, 2124],
-       [3181, 1090],
-       [3885, 1535],
-       [3232, 2568]], dtype=int64))</t>
-        </is>
+      <c r="U18" t="n">
+        <v>0.6810618777660431</v>
       </c>
     </row>
     <row r="19">
@@ -1827,13 +1742,8 @@
       <c r="T19" t="n">
         <v>46.66402666666666</v>
       </c>
-      <c r="U19" t="inlineStr">
-        <is>
-          <t>(0.6778668884670089, array([[2492, 2067],
-       [3273, 1364],
-       [3750, 1894],
-       [2969, 2596]], dtype=int64))</t>
-        </is>
+      <c r="U19" t="n">
+        <v>0.678298576004396</v>
       </c>
     </row>
     <row r="20">
@@ -1899,13 +1809,8 @@
       <c r="T20" t="n">
         <v>56.62594666666666</v>
       </c>
-      <c r="U20" t="inlineStr">
-        <is>
-          <t>(0.6795648329922541, array([[2062, 1026],
-       [2913, 1009],
-       [2925, 1588],
-       [2073, 1605]], dtype=int64))</t>
-        </is>
+      <c r="U20" t="n">
+        <v>0.6803630632069665</v>
       </c>
     </row>
     <row r="21">
@@ -1971,13 +1876,8 @@
       <c r="T21" t="n">
         <v>53.948448</v>
       </c>
-      <c r="U21" t="inlineStr">
-        <is>
-          <t>(0.6095042273798988, array([[2327, 2500],
-       [3026, 2098],
-       [3687, 3244],
-       [2988, 3646]], dtype=int64))</t>
-        </is>
+      <c r="U21" t="n">
+        <v>0.6095042273798988</v>
       </c>
     </row>
     <row r="22">
@@ -2043,13 +1943,8 @@
       <c r="T22" t="n">
         <v>48.83826666666667</v>
       </c>
-      <c r="U22" t="inlineStr">
-        <is>
-          <t>(0.7986778583184102, array([[2759, 2019],
-       [3400,  974],
-       [4236, 1485],
-       [3595, 2531]], dtype=int64))</t>
-        </is>
+      <c r="U22" t="n">
+        <v>0.7992332672806171</v>
       </c>
     </row>
     <row r="23">
@@ -2115,13 +2010,8 @@
       <c r="T23" t="n">
         <v>28.80438666666667</v>
       </c>
-      <c r="U23" t="inlineStr">
-        <is>
-          <t>(0.8876174991636221, array([[1733, 1523],
-       [3022, 1189],
-       [3319, 2333],
-       [2030, 2667]], dtype=int64))</t>
-        </is>
+      <c r="U23" t="n">
+        <v>0.8876174991636221</v>
       </c>
     </row>
     <row r="24">
@@ -2187,13 +2077,8 @@
       <c r="T24" t="n">
         <v>57.002736</v>
       </c>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>(0.8047515236937101, array([[2753, 2230],
-       [3532, 2093],
-       [3701, 3061],
-       [2922, 3197]], dtype=int64))</t>
-        </is>
+      <c r="U24" t="n">
+        <v>0.8055590851913615</v>
       </c>
     </row>
     <row r="25">
@@ -2259,13 +2144,8 @@
       <c r="T25" t="n">
         <v>40.18913066666666</v>
       </c>
-      <c r="U25" t="inlineStr">
-        <is>
-          <t>(0.8900404425281773, array([[2683, 1494],
-       [3620, 1435],
-       [3672, 2270],
-       [2735, 2328]], dtype=int64))</t>
-        </is>
+      <c r="U25" t="n">
+        <v>0.8900995185391424</v>
       </c>
     </row>
     <row r="26">
@@ -2331,13 +2211,8 @@
       <c r="T26" t="n">
         <v>35.43315733333333</v>
       </c>
-      <c r="U26" t="inlineStr">
-        <is>
-          <t>(0.9687814205086791, array([[2648, 1460],
-       [3429,  627],
-       [4289, 1432],
-       [3508, 2266]], dtype=int64))</t>
-        </is>
+      <c r="U26" t="n">
+        <v>0.8920037623857388</v>
       </c>
     </row>
     <row r="27">
@@ -2403,13 +2278,8 @@
       <c r="T27" t="n">
         <v>48.37641066666666</v>
       </c>
-      <c r="U27" t="inlineStr">
-        <is>
-          <t>(0.7938710379644698, array([[2623, 2226],
-       [3043, 1314],
-       [3768, 1647],
-       [3348, 2560]], dtype=int64))</t>
-        </is>
+      <c r="U27" t="n">
+        <v>0.7945892684728506</v>
       </c>
     </row>
     <row r="28">
@@ -2475,13 +2345,8 @@
       <c r="T28" t="n">
         <v>50.55494933333333</v>
       </c>
-      <c r="U28" t="inlineStr">
-        <is>
-          <t>(0.5742954118031572, array([[1682, 2115],
-       [2012, 1041],
-       [3882, 1615],
-       [3552, 2690]], dtype=int64))</t>
-        </is>
+      <c r="U28" t="n">
+        <v>0.5743816312309943</v>
       </c>
     </row>
     <row r="29">
@@ -2547,13 +2412,8 @@
       <c r="T29" t="n">
         <v>54.63698133333333</v>
       </c>
-      <c r="U29" t="inlineStr">
-        <is>
-          <t>(0.6339194275415118, array([[1969, 1484],
-       [2552,  801],
-       [3630, 1720],
-       [3047, 2403]], dtype=int64))</t>
-        </is>
+      <c r="U29" t="n">
+        <v>0.6339194275415118</v>
       </c>
     </row>
     <row r="30">
@@ -2619,13 +2479,8 @@
       <c r="T30" t="n">
         <v>61.323536</v>
       </c>
-      <c r="U30" t="inlineStr">
-        <is>
-          <t>(0.8896099088705697, array([[1621, 1893],
-       [1777,  756],
-       [3055,  931],
-       [2899, 2069]], dtype=int64))</t>
-        </is>
+      <c r="U30" t="n">
+        <v>0.889703735099161</v>
       </c>
     </row>
     <row r="31">
@@ -2691,13 +2546,8 @@
       <c r="T31" t="n">
         <v>67.054672</v>
       </c>
-      <c r="U31" t="inlineStr">
-        <is>
-          <t>(0.6886305479596794, array([[2051, 2075],
-       [2849, 1316],
-       [3951, 2475],
-       [3153, 3234]], dtype=int64))</t>
-        </is>
+      <c r="U31" t="n">
+        <v>0.6886305479596794</v>
       </c>
     </row>
     <row r="32">
@@ -2763,13 +2613,8 @@
       <c r="T32" t="n">
         <v>44.267016</v>
       </c>
-      <c r="U32" t="inlineStr">
-        <is>
-          <t>(0.5645831581319437, array([[2375, 1221],
-       [3377, 1165],
-       [3475, 2938],
-       [2474, 2994]], dtype=int64))</t>
-        </is>
+      <c r="U32" t="n">
+        <v>0.5646007947405126</v>
       </c>
     </row>
     <row r="33">
@@ -2835,13 +2680,8 @@
       <c r="T33" t="n">
         <v>48.584672</v>
       </c>
-      <c r="U33" t="inlineStr">
-        <is>
-          <t>(0.824042154848583, array([[1487, 1416],
-       [2709, 1196],
-       [2891, 2203],
-       [1669, 2424]], dtype=int64))</t>
-        </is>
+      <c r="U33" t="n">
+        <v>0.8241600053958096</v>
       </c>
     </row>
     <row r="34">
@@ -2907,13 +2747,8 @@
       <c r="T34" t="n">
         <v>35.999768</v>
       </c>
-      <c r="U34" t="inlineStr">
-        <is>
-          <t>(0.8455350003865124, array([[1486, 2949],
-       [1600, 1532],
-       [2799, 1628],
-       [2685, 3046]], dtype=int64))</t>
-        </is>
+      <c r="U34" t="n">
+        <v>0.8461278722285002</v>
       </c>
     </row>
     <row r="35">
@@ -2979,13 +2814,8 @@
       <c r="T35" t="n">
         <v>46.44088</v>
       </c>
-      <c r="U35" t="inlineStr">
-        <is>
-          <t>(0.8927349572241833, array([[2308, 2033],
-       [3239, 1241],
-       [4126, 2284],
-       [3195, 3076]], dtype=int64))</t>
-        </is>
+      <c r="U35" t="n">
+        <v>0.8899860924917873</v>
       </c>
     </row>
     <row r="36">
@@ -3051,13 +2881,8 @@
       <c r="T36" t="n">
         <v>68.24492266666667</v>
       </c>
-      <c r="U36" t="inlineStr">
-        <is>
-          <t>(0.47103566706641864, array([[2086, 1708],
-       [3278, 1636],
-       [3312, 2198],
-       [2119, 2270]], dtype=int64))</t>
-        </is>
+      <c r="U36" t="n">
+        <v>0.4722910868456565</v>
       </c>
     </row>
     <row r="37">
@@ -3123,13 +2948,8 @@
       <c r="T37" t="n">
         <v>60.16693866666667</v>
       </c>
-      <c r="U37" t="inlineStr">
-        <is>
-          <t>(0.8832695484166903, array([[2322, 1787],
-       [3201, 1432],
-       [3602, 2426],
-       [2724, 2781]], dtype=int64))</t>
-        </is>
+      <c r="U37" t="n">
+        <v>0.883578182954165</v>
       </c>
     </row>
     <row r="38">
@@ -3195,13 +3015,8 @@
       <c r="T38" t="n">
         <v>43.29832266666666</v>
       </c>
-      <c r="U38" t="inlineStr">
-        <is>
-          <t>(0.896326365911809, array([[2324,  901],
-       [3379,  782],
-       [3512, 1959],
-       [2457, 2078]], dtype=int64))</t>
-        </is>
+      <c r="U38" t="n">
+        <v>0.896326365911809</v>
       </c>
     </row>
     <row r="39">
@@ -3267,13 +3082,8 @@
       <c r="T39" t="n">
         <v>33.94951733333333</v>
       </c>
-      <c r="U39" t="inlineStr">
-        <is>
-          <t>(0.9430742709467377, array([[1114, 1898],
-       [2257, 1781],
-       [2381, 2993],
-       [1238, 3110]], dtype=int64))</t>
-        </is>
+      <c r="U39" t="n">
+        <v>0.9430742709467377</v>
       </c>
     </row>
     <row r="40">
@@ -3339,13 +3149,8 @@
       <c r="T40" t="n">
         <v>60.54719466666667</v>
       </c>
-      <c r="U40" t="inlineStr">
-        <is>
-          <t>(0.8424126996394752, array([[1562,  844],
-       [3192,  687],
-       [3325, 2061],
-       [1694, 2218]], dtype=int64))</t>
-        </is>
+      <c r="U40" t="n">
+        <v>0.8288804590287229</v>
       </c>
     </row>
     <row r="41">
@@ -3411,13 +3216,8 @@
       <c r="T41" t="n">
         <v>49.88592533333333</v>
       </c>
-      <c r="U41" t="inlineStr">
-        <is>
-          <t>(0.6951771644631741, array([[2398,  878],
-       [3783,  256],
-       [4215, 1219],
-       [2831, 1841]], dtype=int64))</t>
-        </is>
+      <c r="U41" t="n">
+        <v>0.6955950799618094</v>
       </c>
     </row>
     <row r="42">
@@ -3483,13 +3283,8 @@
       <c r="T42" t="n">
         <v>40.67521333333333</v>
       </c>
-      <c r="U42" t="inlineStr">
-        <is>
-          <t>(0.6048151956254484, array([[2533, 2496],
-       [2747, 1709],
-       [4047, 2062],
-       [3834, 2849]], dtype=int64))</t>
-        </is>
+      <c r="U42" t="n">
+        <v>0.6052485013710623</v>
       </c>
     </row>
     <row r="43">
@@ -3555,13 +3350,8 @@
       <c r="T43" t="n">
         <v>54.71797333333333</v>
       </c>
-      <c r="U43" t="inlineStr">
-        <is>
-          <t>(0.7265064609383657, array([[2174, 2049],
-       [3333, 1515],
-       [3721, 2357],
-       [2562, 2891]], dtype=int64))</t>
-        </is>
+      <c r="U43" t="n">
+        <v>0.7265064609383657</v>
       </c>
     </row>
     <row r="44">
@@ -3627,13 +3417,8 @@
       <c r="T44" t="n">
         <v>29.76685333333333</v>
       </c>
-      <c r="U44" t="inlineStr">
-        <is>
-          <t>(0.7969775714298685, array([[2309, 2178],
-       [2769, 1519],
-       [3596, 2096],
-       [3136, 2755]], dtype=int64))</t>
-        </is>
+      <c r="U44" t="n">
+        <v>0.7940669954810665</v>
       </c>
     </row>
     <row r="45">
@@ -3699,13 +3484,8 @@
       <c r="T45" t="n">
         <v>49.221568</v>
       </c>
-      <c r="U45" t="inlineStr">
-        <is>
-          <t>(0.892474934017691, array([[2143, 2162],
-       [3081, 1472],
-       [3697, 2309],
-       [2759, 2999]], dtype=int64))</t>
-        </is>
+      <c r="U45" t="n">
+        <v>0.892474934017691</v>
       </c>
     </row>
     <row r="46">
@@ -3771,13 +3551,8 @@
       <c r="T46" t="n">
         <v>50.51412266666667</v>
       </c>
-      <c r="U46" t="inlineStr">
-        <is>
-          <t>(0.6703385073664702, array([[2237, 2604],
-       [2646, 1348],
-       [3488, 1622],
-       [3079, 2878]], dtype=int64))</t>
-        </is>
+      <c r="U46" t="n">
+        <v>0.6703385073664702</v>
       </c>
     </row>
     <row r="47">
@@ -3843,13 +3618,8 @@
       <c r="T47" t="n">
         <v>50.40916266666667</v>
       </c>
-      <c r="U47" t="inlineStr">
-        <is>
-          <t>(0.8140854685014837, array([[2324, 2137],
-       [2639, 1607],
-       [3290, 1994],
-       [2974, 2525]], dtype=int64))</t>
-        </is>
+      <c r="U47" t="n">
+        <v>0.8159378969700728</v>
       </c>
     </row>
     <row r="48">
@@ -3915,13 +3685,8 @@
       <c r="T48" t="n">
         <v>41.737776</v>
       </c>
-      <c r="U48" t="inlineStr">
-        <is>
-          <t>(0.8141485856822432, array([[1854, 2161],
-       [2087, 1307],
-       [3136, 1593],
-       [2903, 2447]], dtype=int64))</t>
-        </is>
+      <c r="U48" t="n">
+        <v>0.8141485856822432</v>
       </c>
     </row>
     <row r="49">
@@ -3987,13 +3752,8 @@
       <c r="T49" t="n">
         <v>63.58593066666667</v>
       </c>
-      <c r="U49" t="inlineStr">
-        <is>
-          <t>(0.8062894171951291, array([[2095, 1646],
-       [2480,  877],
-       [3434, 1354],
-       [3049, 2123]], dtype=int64))</t>
-        </is>
+      <c r="U49" t="n">
+        <v>0.8062894171951291</v>
       </c>
     </row>
     <row r="50">
@@ -4059,13 +3819,8 @@
       <c r="T50" t="n">
         <v>35.66297333333333</v>
       </c>
-      <c r="U50" t="inlineStr">
-        <is>
-          <t>(0.812941788428894, array([[3216, 1631],
-       [3407,  727],
-       [4519,  961],
-       [4328, 1866]], dtype=int64))</t>
-        </is>
+      <c r="U50" t="n">
+        <v>0.8130894052049265</v>
       </c>
     </row>
     <row r="51">
@@ -4131,13 +3886,8 @@
       <c r="T51" t="n">
         <v>26.510832</v>
       </c>
-      <c r="U51" t="inlineStr">
-        <is>
-          <t>(0.8653808156713433, array([[2417, 1840],
-       [2988, 1644],
-       [3158, 2138],
-       [2587, 2334]], dtype=int64))</t>
-        </is>
+      <c r="U51" t="n">
+        <v>0.8653808156713433</v>
       </c>
     </row>
     <row r="52">
@@ -4203,13 +3953,8 @@
       <c r="T52" t="n">
         <v>29.66302666666667</v>
       </c>
-      <c r="U52" t="inlineStr">
-        <is>
-          <t>(0.7134754969926915, array([[2398, 1619],
-       [2901, 1609],
-       [2915, 2314],
-       [2411, 2324]], dtype=int64))</t>
-        </is>
+      <c r="U52" t="n">
+        <v>0.7134948692869031</v>
       </c>
     </row>
     <row r="53">
@@ -4275,13 +4020,8 @@
       <c r="T53" t="n">
         <v>25.95370666666667</v>
       </c>
-      <c r="U53" t="inlineStr">
-        <is>
-          <t>(0.6846142572468186, array([[3053, 1998],
-       [3316, 1406],
-       [3722, 1586],
-       [3459, 2179]], dtype=int64))</t>
-        </is>
+      <c r="U53" t="n">
+        <v>0.6855802155580321</v>
       </c>
     </row>
     <row r="54">
@@ -4347,13 +4087,8 @@
       <c r="T54" t="n">
         <v>25.58365333333333</v>
       </c>
-      <c r="U54" t="inlineStr">
-        <is>
-          <t>(0.8454417756599041, array([[2347, 2758],
-       [2444, 1817],
-       [3557, 1932],
-       [3460, 2873]], dtype=int64))</t>
-        </is>
+      <c r="U54" t="n">
+        <v>0.8454417756599041</v>
       </c>
     </row>
     <row r="55">
@@ -4419,13 +4154,8 @@
       <c r="T55" t="n">
         <v>26.324952</v>
       </c>
-      <c r="U55" t="inlineStr">
-        <is>
-          <t>(0.6017359053993518, array([[2227, 2306],
-       [3053, 1520],
-       [3526, 2017],
-       [2701, 2803]], dtype=int64))</t>
-        </is>
+      <c r="U55" t="n">
+        <v>0.6021183508355402</v>
       </c>
     </row>
     <row r="56">
@@ -4491,13 +4221,8 @@
       <c r="T56" t="n">
         <v>24.591304</v>
       </c>
-      <c r="U56" t="inlineStr">
-        <is>
-          <t>(0.7694323144104803, array([[2250, 2040],
-       [3131, 2040],
-       [3131, 3185],
-       [2250, 3185]], dtype=int64))</t>
-        </is>
+      <c r="U56" t="n">
+        <v>0.7694323144104803</v>
       </c>
     </row>
     <row r="57">
@@ -4563,13 +4288,8 @@
       <c r="T57" t="n">
         <v>42.439712</v>
       </c>
-      <c r="U57" t="inlineStr">
-        <is>
-          <t>(0.9803939018860889, array([[2927, 1823],
-       [3629, 1376],
-       [4085, 2091],
-       [3383, 2539]], dtype=int64))</t>
-        </is>
+      <c r="U57" t="n">
+        <v>0.9813688202049343</v>
       </c>
     </row>
     <row r="58">
@@ -4635,13 +4355,8 @@
       <c r="T58" t="n">
         <v>49.12457066666666</v>
       </c>
-      <c r="U58" t="inlineStr">
-        <is>
-          <t>(0.8420383113490758, array([[2100, 1622],
-       [3107, 1397],
-       [3297, 2245],
-       [2290, 2471]], dtype=int64))</t>
-        </is>
+      <c r="U58" t="n">
+        <v>0.8422166377992671</v>
       </c>
     </row>
     <row r="59">
@@ -4707,13 +4422,8 @@
       <c r="T59" t="n">
         <v>52.86003733333333</v>
       </c>
-      <c r="U59" t="inlineStr">
-        <is>
-          <t>(0.7273391940960838, array([[1881, 2140],
-       [2789, 1824],
-       [3020, 2485],
-       [2111, 2802]], dtype=int64))</t>
-        </is>
+      <c r="U59" t="n">
+        <v>0.7283024978001152</v>
       </c>
     </row>
     <row r="60">
@@ -4779,13 +4489,8 @@
       <c r="T60" t="n">
         <v>24.209096</v>
       </c>
-      <c r="U60" t="inlineStr">
-        <is>
-          <t>(0.725683382625762, array([[2639, 1559],
-       [3229, 1540],
-       [3256, 2352],
-       [2666, 2372]], dtype=int64))</t>
-        </is>
+      <c r="U60" t="n">
+        <v>0.7265760949574748</v>
       </c>
     </row>
     <row r="61">
@@ -4851,13 +4556,8 @@
       <c r="T61" t="n">
         <v>35.731032</v>
       </c>
-      <c r="U61" t="inlineStr">
-        <is>
-          <t>(0.8374243597097225, array([[2585, 1088],
-       [3641,  908],
-       [3856, 2169],
-       [2799, 2348]], dtype=int64))</t>
-        </is>
+      <c r="U61" t="n">
+        <v>0.8381802350296059</v>
       </c>
     </row>
     <row r="62">
@@ -4923,13 +4623,8 @@
       <c r="T62" t="n">
         <v>33.9576</v>
       </c>
-      <c r="U62" t="inlineStr">
-        <is>
-          <t>(0.6722108441300645, array([[1680, 1956],
-       [2451,  540],
-       [3403, 1058],
-       [2632, 2474]], dtype=int64))</t>
-        </is>
+      <c r="U62" t="n">
+        <v>0.6722108441300645</v>
       </c>
     </row>
     <row r="63">
@@ -4995,13 +4690,8 @@
       <c r="T63" t="n">
         <v>35.39396</v>
       </c>
-      <c r="U63" t="inlineStr">
-        <is>
-          <t>(0.6612549773758402, array([[2668, 2309],
-       [2845, 1568],
-       [3335, 1685],
-       [3158, 2426]], dtype=int64))</t>
-        </is>
+      <c r="U63" t="n">
+        <v>0.6612549773758402</v>
       </c>
     </row>
     <row r="64">
@@ -5067,13 +4757,8 @@
       <c r="T64" t="n">
         <v>39.04019733333333</v>
       </c>
-      <c r="U64" t="inlineStr">
-        <is>
-          <t>(0.6215244780800616, array([[2650, 2443],
-       [3257, 1597],
-       [3783, 1974],
-       [3177, 2820]], dtype=int64))</t>
-        </is>
+      <c r="U64" t="n">
+        <v>0.6218724612774554</v>
       </c>
     </row>
     <row r="65">
@@ -5139,13 +4824,8 @@
       <c r="T65" t="n">
         <v>27.82893333333333</v>
       </c>
-      <c r="U65" t="inlineStr">
-        <is>
-          <t>(0.7332616010060513, array([[2058, 1797],
-       [2674,  824],
-       [4001, 1664],
-       [3384, 2637]], dtype=int64))</t>
-        </is>
+      <c r="U65" t="n">
+        <v>0.7336562677106536</v>
       </c>
     </row>
     <row r="66">
@@ -5211,13 +4891,8 @@
       <c r="T66" t="n">
         <v>70.53980799999999</v>
       </c>
-      <c r="U66" t="inlineStr">
-        <is>
-          <t>(0.9350230099605422, array([[2961, 1259],
-       [3731,  567],
-       [4378, 1287],
-       [3608, 1979]], dtype=int64))</t>
-        </is>
+      <c r="U66" t="n">
+        <v>0.9350230099605422</v>
       </c>
     </row>
     <row r="67">
@@ -5283,13 +4958,8 @@
       <c r="T67" t="n">
         <v>71.146272</v>
       </c>
-      <c r="U67" t="inlineStr">
-        <is>
-          <t>(0.836535321793914, array([[1823, 1197],
-       [2759,  990],
-       [3006, 2109],
-       [2070, 2316]], dtype=int64))</t>
-        </is>
+      <c r="U67" t="n">
+        <v>0.836535321793914</v>
       </c>
     </row>
     <row r="68">
@@ -5355,13 +5025,8 @@
       <c r="T68" t="n">
         <v>45.54658666666667</v>
       </c>
-      <c r="U68" t="inlineStr">
-        <is>
-          <t>(0.5950764869850156, array([[1162, 2997],
-       [2271, 2265],
-       [2708, 2925],
-       [1598, 3658]], dtype=int64))</t>
-        </is>
+      <c r="U68" t="n">
+        <v>0.594288912460719</v>
       </c>
     </row>
     <row r="69">
@@ -5427,13 +5092,8 @@
       <c r="T69" t="n">
         <v>35.12685866666666</v>
       </c>
-      <c r="U69" t="inlineStr">
-        <is>
-          <t>(0.7329872387574156, array([[1304, 2094],
-       [1678, 1106],
-       [3026, 1616],
-       [2652, 2604]], dtype=int64))</t>
-        </is>
+      <c r="U69" t="n">
+        <v>0.7329872387574156</v>
       </c>
     </row>
     <row r="70">
@@ -5499,13 +5159,8 @@
       <c r="T70" t="n">
         <v>43.36323466666666</v>
       </c>
-      <c r="U70" t="inlineStr">
-        <is>
-          <t>(0.9577064137544659, array([[2723, 2554],
-       [2878, 1625],
-       [3848, 1786],
-       [3693, 2716]], dtype=int64))</t>
-        </is>
+      <c r="U70" t="n">
+        <v>0.9578663778737779</v>
       </c>
     </row>
     <row r="71">
@@ -5571,13 +5226,8 @@
       <c r="T71" t="n">
         <v>29.15065866666666</v>
       </c>
-      <c r="U71" t="inlineStr">
-        <is>
-          <t>(0.8298914784870723, array([[2615, 2348],
-       [2882, 1591],
-       [3793, 1912],
-       [3527, 2669]], dtype=int64))</t>
-        </is>
+      <c r="U71" t="n">
+        <v>0.8307018833276572</v>
       </c>
     </row>
     <row r="72">
@@ -5643,13 +5293,8 @@
       <c r="T72" t="n">
         <v>33.30416533333333</v>
       </c>
-      <c r="U72" t="inlineStr">
-        <is>
-          <t>(0.827313913093154, array([[2586, 1932],
-       [2682,  959],
-       [3858, 1076],
-       [3762, 2049]], dtype=int64))</t>
-        </is>
+      <c r="U72" t="n">
+        <v>0.8273139130931541</v>
       </c>
     </row>
     <row r="73">
@@ -5715,13 +5360,8 @@
       <c r="T73" t="n">
         <v>23.89247466666666</v>
       </c>
-      <c r="U73" t="inlineStr">
-        <is>
-          <t>(0.7374767589685881, array([[2257, 2124],
-       [2434,  961],
-       [4011, 1201],
-       [3834, 2364]], dtype=int64))</t>
-        </is>
+      <c r="U73" t="n">
+        <v>0.7374767589685881</v>
       </c>
     </row>
     <row r="74">
@@ -5787,13 +5427,8 @@
       <c r="T74" t="n">
         <v>45.93775466666666</v>
       </c>
-      <c r="U74" t="inlineStr">
-        <is>
-          <t>(0.7493863576057669, array([[2422, 2015],
-       [2552, 1314],
-       [3486, 1488],
-       [3356, 2188]], dtype=int64))</t>
-        </is>
+      <c r="U74" t="n">
+        <v>0.7495304429389414</v>
       </c>
     </row>
     <row r="75">
@@ -5859,13 +5494,8 @@
       <c r="T75" t="n">
         <v>34.02794933333333</v>
       </c>
-      <c r="U75" t="inlineStr">
-        <is>
-          <t>(0.8034459947699902, array([[2544, 2745],
-       [2681, 1882],
-       [3754, 2053],
-       [3616, 2915]], dtype=int64))</t>
-        </is>
+      <c r="U75" t="n">
+        <v>0.8042932663310409</v>
       </c>
     </row>
     <row r="76">
@@ -5931,13 +5561,8 @@
       <c r="T76" t="n">
         <v>33.23579733333333</v>
       </c>
-      <c r="U76" t="inlineStr">
-        <is>
-          <t>(0.974856196622002, array([[2267, 1782],
-       [2982, 1142],
-       [3639, 1875],
-       [2924, 2515]], dtype=int64))</t>
-        </is>
+      <c r="U76" t="n">
+        <v>0.974856196622002</v>
       </c>
     </row>
     <row r="77">
@@ -6003,13 +5628,8 @@
       <c r="T77" t="n">
         <v>35.954048</v>
       </c>
-      <c r="U77" t="inlineStr">
-        <is>
-          <t>(0.8209783883305874, array([[2480, 1480],
-       [3264, 1314],
-       [3467, 2268],
-       [2682, 2435]], dtype=int64))</t>
-        </is>
+      <c r="U77" t="n">
+        <v>0.8216270961120783</v>
       </c>
     </row>
     <row r="78">
@@ -6075,13 +5695,8 @@
       <c r="T78" t="n">
         <v>37.41944533333334</v>
       </c>
-      <c r="U78" t="inlineStr">
-        <is>
-          <t>(0.6758205759890635, array([[2482, 1460],
-       [3391, 1432],
-       [3432, 2777],
-       [2523, 2804]], dtype=int64))</t>
-        </is>
+      <c r="U78" t="n">
+        <v>0.6763229513362352</v>
       </c>
     </row>
     <row r="79">
@@ -6147,13 +5762,8 @@
       <c r="T79" t="n">
         <v>31.012312</v>
       </c>
-      <c r="U79" t="inlineStr">
-        <is>
-          <t>(0.9454154659690494, array([[2330, 2087],
-       [2828, 1302],
-       [3571, 1774],
-       [3072, 2559]], dtype=int64))</t>
-        </is>
+      <c r="U79" t="n">
+        <v>0.9463899239927138</v>
       </c>
     </row>
     <row r="80">
@@ -6219,13 +5829,8 @@
       <c r="T80" t="n">
         <v>32.899456</v>
       </c>
-      <c r="U80" t="inlineStr">
-        <is>
-          <t>(0.7158122713042072, array([[2439, 2062],
-       [3071, 1358],
-       [3576, 1810],
-       [2944, 2515]], dtype=int64))</t>
-        </is>
+      <c r="U80" t="n">
+        <v>0.716375476785548</v>
       </c>
     </row>
     <row r="81">
@@ -6291,13 +5896,8 @@
       <c r="T81" t="n">
         <v>37.83626666666667</v>
       </c>
-      <c r="U81" t="inlineStr">
-        <is>
-          <t>(0.6863498608793892, array([[2810, 2435],
-       [2896, 1692],
-       [3977, 1818],
-       [3891, 2560]], dtype=int64))</t>
-        </is>
+      <c r="U81" t="n">
+        <v>0.6864225963648877</v>
       </c>
     </row>
     <row r="82">
@@ -6363,13 +5963,8 @@
       <c r="T82" t="n">
         <v>48.63002666666667</v>
       </c>
-      <c r="U82" t="inlineStr">
-        <is>
-          <t>(0.9232478865771004, array([[2755, 2141],
-       [3366, 1561],
-       [3994, 2223],
-       [3383, 2803]], dtype=int64))</t>
-        </is>
+      <c r="U82" t="n">
+        <v>0.9232478865771004</v>
       </c>
     </row>
     <row r="83">
@@ -6435,13 +6030,8 @@
       <c r="T83" t="n">
         <v>38.44942933333333</v>
       </c>
-      <c r="U83" t="inlineStr">
-        <is>
-          <t>(0.7524305712643743, array([[2549, 2274],
-       [2976, 1519],
-       [3545, 1840],
-       [3118, 2596]], dtype=int64))</t>
-        </is>
+      <c r="U83" t="n">
+        <v>0.7531857691681176</v>
       </c>
     </row>
     <row r="84">
@@ -6507,13 +6097,8 @@
       <c r="T84" t="n">
         <v>45.055056</v>
       </c>
-      <c r="U84" t="inlineStr">
-        <is>
-          <t>(0.965431754193505, array([[1975,  670],
-       [3044,  569],
-       [3142, 1601],
-       [2073, 1702]], dtype=int64))</t>
-        </is>
+      <c r="U84" t="n">
+        <v>0.965431754193505</v>
       </c>
     </row>
     <row r="85">
@@ -6579,13 +6164,8 @@
       <c r="T85" t="n">
         <v>51.69056</v>
       </c>
-      <c r="U85" t="inlineStr">
-        <is>
-          <t>(0.9839780009245188, array([[2035, 2518],
-       [2180, 1327],
-       [3352, 1469],
-       [3207, 2660]], dtype=int64))</t>
-        </is>
+      <c r="U85" t="n">
+        <v>0.9839780009245188</v>
       </c>
     </row>
     <row r="86">
@@ -6651,13 +6231,8 @@
       <c r="T86" t="n">
         <v>37.38932533333333</v>
       </c>
-      <c r="U86" t="inlineStr">
-        <is>
-          <t>(0.8998911719884006, array([[1933, 1788],
-       [2520,  885],
-       [3523, 1538],
-       [2935, 2441]], dtype=int64))</t>
-        </is>
+      <c r="U86" t="n">
+        <v>0.8933065994418085</v>
       </c>
     </row>
     <row r="87">
@@ -6723,13 +6298,8 @@
       <c r="T87" t="n">
         <v>25.05626133333333</v>
       </c>
-      <c r="U87" t="inlineStr">
-        <is>
-          <t>(0.8014854339903609, array([[2188, 1662],
-       [3020, 1576],
-       [3128, 2613],
-       [2296, 2700]], dtype=int64))</t>
-        </is>
+      <c r="U87" t="n">
+        <v>0.8022500333088446</v>
       </c>
     </row>
     <row r="88">
@@ -6795,13 +6365,8 @@
       <c r="T88" t="n">
         <v>31.27939466666666</v>
       </c>
-      <c r="U88" t="inlineStr">
-        <is>
-          <t>(0.651454330632309, array([[2273, 1916],
-       [2640, 1206],
-       [3728, 1770],
-       [3361, 2479]], dtype=int64))</t>
-        </is>
+      <c r="U88" t="n">
+        <v>0.6516988981287931</v>
       </c>
     </row>
     <row r="89">
@@ -6867,13 +6432,8 @@
       <c r="T89" t="n">
         <v>56.45187733333334</v>
       </c>
-      <c r="U89" t="inlineStr">
-        <is>
-          <t>(0.7431258137357967, array([[2521, 1942],
-       [3097, 1549],
-       [3626, 2324],
-       [3050, 2717]], dtype=int64))</t>
-        </is>
+      <c r="U89" t="n">
+        <v>0.7431258137357967</v>
       </c>
     </row>
     <row r="90">
@@ -6939,13 +6499,8 @@
       <c r="T90" t="n">
         <v>29.642512</v>
       </c>
-      <c r="U90" t="inlineStr">
-        <is>
-          <t>(0.7993329318544752, array([[2262, 2149],
-       [2499, 1296],
-       [3566, 1593],
-       [3329, 2446]], dtype=int64))</t>
-        </is>
+      <c r="U90" t="n">
+        <v>0.8006181731041928</v>
       </c>
     </row>
     <row r="91">
@@ -7011,13 +6566,8 @@
       <c r="T91" t="n">
         <v>27.58088533333333</v>
       </c>
-      <c r="U91" t="inlineStr">
-        <is>
-          <t>(0.8070766856774393, array([[2260, 2356],
-       [2335, 1118],
-       [3335, 1178],
-       [3260, 2417]], dtype=int64))</t>
-        </is>
+      <c r="U91" t="n">
+        <v>0.8077262225343242</v>
       </c>
     </row>
     <row r="92">
@@ -7083,13 +6633,8 @@
       <c r="T92" t="n">
         <v>38.75453066666667</v>
       </c>
-      <c r="U92" t="inlineStr">
-        <is>
-          <t>(0.6840510630730532, array([[2247, 1753],
-       [3159, 1387],
-       [3409, 2011],
-       [2497, 2377]], dtype=int64))</t>
-        </is>
+      <c r="U92" t="n">
+        <v>0.6840510630730532</v>
       </c>
     </row>
     <row r="93">
@@ -7155,13 +6700,8 @@
       <c r="T93" t="n">
         <v>44.80746133333334</v>
       </c>
-      <c r="U93" t="inlineStr">
-        <is>
-          <t>(0.6194371581200879, array([[2385, 2234],
-       [2843, 1190],
-       [3490, 1473],
-       [3032, 2517]], dtype=int64))</t>
-        </is>
+      <c r="U93" t="n">
+        <v>0.6194371581200879</v>
       </c>
     </row>
     <row r="94">
@@ -7227,13 +6767,8 @@
       <c r="T94" t="n">
         <v>52.94913066666667</v>
       </c>
-      <c r="U94" t="inlineStr">
-        <is>
-          <t>(0.8767296925006018, array([[2408, 2297],
-       [3175, 1555],
-       [3826, 2227],
-       [3060, 2970]], dtype=int64))</t>
-        </is>
+      <c r="U94" t="n">
+        <v>0.8767481691413811</v>
       </c>
     </row>
     <row r="95">
@@ -7299,13 +6834,8 @@
       <c r="T95" t="n">
         <v>42.898008</v>
       </c>
-      <c r="U95" t="inlineStr">
-        <is>
-          <t>(0.7057324840764331, array([[2067, 1646],
-       [2852,  861],
-       [3406, 1415],
-       [2621, 2200]], dtype=int64))</t>
-        </is>
+      <c r="U95" t="n">
+        <v>0.7057324840764331</v>
       </c>
     </row>
     <row r="96">
@@ -7371,13 +6901,8 @@
       <c r="T96" t="n">
         <v>45.40811733333334</v>
       </c>
-      <c r="U96" t="inlineStr">
-        <is>
-          <t>(0.7057324840764331, array([[2067, 1646],
-       [2852,  861],
-       [3406, 1415],
-       [2621, 2200]], dtype=int64))</t>
-        </is>
+      <c r="U96" t="n">
+        <v>0.7057324840764331</v>
       </c>
     </row>
     <row r="97">
@@ -7443,13 +6968,8 @@
       <c r="T97" t="n">
         <v>25.968008</v>
       </c>
-      <c r="U97" t="inlineStr">
-        <is>
-          <t>(0.8048042497723854, array([[2592, 1256],
-       [3560, 1126],
-       [3665, 1905],
-       [2697, 2035]], dtype=int64))</t>
-        </is>
+      <c r="U97" t="n">
+        <v>0.8048042497723854</v>
       </c>
     </row>
     <row r="98">
@@ -7515,13 +7035,8 @@
       <c r="T98" t="n">
         <v>27.814624</v>
       </c>
-      <c r="U98" t="inlineStr">
-        <is>
-          <t>(0.5600820533723462, array([[2697, 2411],
-       [3219, 2396],
-       [3246, 3328],
-       [2724, 3343]], dtype=int64))</t>
-        </is>
+      <c r="U98" t="n">
+        <v>0.5600820533723462</v>
       </c>
     </row>
     <row r="99">
@@ -7587,13 +7102,8 @@
       <c r="T99" t="n">
         <v>53.972512</v>
       </c>
-      <c r="U99" t="inlineStr">
-        <is>
-          <t>(0.3951233560893895, array([[1578, 1655],
-       [2250, 1014],
-       [3872, 2715],
-       [3199, 3356]], dtype=int64))</t>
-        </is>
+      <c r="U99" t="n">
+        <v>0.3952393846335605</v>
       </c>
     </row>
     <row r="100">
@@ -7659,13 +7169,8 @@
       <c r="T100" t="n">
         <v>41.99886933333333</v>
       </c>
-      <c r="U100" t="inlineStr">
-        <is>
-          <t>(0.3829847227615254, array([[1931, 2225],
-       [2235, 1327],
-       [4580, 2119],
-       [4276, 3018]], dtype=int64))</t>
-        </is>
+      <c r="U100" t="n">
+        <v>0.3830342626646987</v>
       </c>
     </row>
     <row r="101">
@@ -7731,13 +7236,8 @@
       <c r="T101" t="n">
         <v>46.96074666666667</v>
       </c>
-      <c r="U101" t="inlineStr">
-        <is>
-          <t>(0.8421021183026727, array([[2489, 1704],
-       [3228, 1341],
-       [3535, 1964],
-       [2795, 2327]], dtype=int64))</t>
-        </is>
+      <c r="U101" t="n">
+        <v>0.8416519083800509</v>
       </c>
     </row>
     <row r="102">
@@ -7803,13 +7303,8 @@
       <c r="T102" t="n">
         <v>30.273104</v>
       </c>
-      <c r="U102" t="inlineStr">
-        <is>
-          <t>(0.8027530169078234, array([[2279, 2268],
-       [2536, 1355],
-       [3269, 1561],
-       [3013, 2473]], dtype=int64))</t>
-        </is>
+      <c r="U102" t="n">
+        <v>0.8037981842734963</v>
       </c>
     </row>
     <row r="103">
@@ -7875,13 +7370,8 @@
       <c r="T103" t="n">
         <v>48.18122666666667</v>
       </c>
-      <c r="U103" t="inlineStr">
-        <is>
-          <t>(0.9460952693185568, array([[1935, 2365],
-       [2002, 1475],
-       [2845, 1538],
-       [2778, 2429]], dtype=int64))</t>
-        </is>
+      <c r="U103" t="n">
+        <v>0.9471523105938859</v>
       </c>
     </row>
     <row r="104">
@@ -7947,13 +7437,8 @@
       <c r="T104" t="n">
         <v>50.16221333333333</v>
       </c>
-      <c r="U104" t="inlineStr">
-        <is>
-          <t>(0.6606769774878708, array([[2427, 2018],
-       [3046,  575],
-       [4000,  984],
-       [3381, 2428]], dtype=int64))</t>
-        </is>
+      <c r="U104" t="n">
+        <v>0.6610636913358497</v>
       </c>
     </row>
     <row r="105">
@@ -8019,13 +7504,8 @@
       <c r="T105" t="n">
         <v>44.06296533333333</v>
       </c>
-      <c r="U105" t="inlineStr">
-        <is>
-          <t>(0.6680066550828562, array([[2328, 2814],
-       [2935, 1209],
-       [4008, 1614],
-       [3401, 3220]], dtype=int64))</t>
-        </is>
+      <c r="U105" t="n">
+        <v>0.6683707922609278</v>
       </c>
     </row>
     <row r="106">
@@ -8091,13 +7571,8 @@
       <c r="T106" t="n">
         <v>47.2264</v>
       </c>
-      <c r="U106" t="inlineStr">
-        <is>
-          <t>(0.9186776390395036, array([[2164, 1805],
-       [3042, 1230],
-       [3669, 2184],
-       [2791, 2760]], dtype=int64))</t>
-        </is>
+      <c r="U106" t="n">
+        <v>0.9193502346969963</v>
       </c>
     </row>
     <row r="107">
@@ -8163,13 +7638,8 @@
       <c r="T107" t="n">
         <v>41.32511466666666</v>
       </c>
-      <c r="U107" t="inlineStr">
-        <is>
-          <t>(0.9381340756030845, array([[2546, 1353],
-       [3533, 1227],
-       [3668, 2278],
-       [2681, 2405]], dtype=int64))</t>
-        </is>
+      <c r="U107" t="n">
+        <v>0.9390122050015289</v>
       </c>
     </row>
     <row r="108">
@@ -8235,13 +7705,8 @@
       <c r="T108" t="n">
         <v>59.37103466666667</v>
       </c>
-      <c r="U108" t="inlineStr">
-        <is>
-          <t>(0.9154671334806379, array([[2685, 2245],
-       [2982, 1235],
-       [4084, 1560],
-       [3787, 2569]], dtype=int64))</t>
-        </is>
+      <c r="U108" t="n">
+        <v>0.9156922638918129</v>
       </c>
     </row>
     <row r="109">
@@ -8307,13 +7772,8 @@
       <c r="T109" t="n">
         <v>65.11604266666667</v>
       </c>
-      <c r="U109" t="inlineStr">
-        <is>
-          <t>(0.958895653698288, array([[2025, 2090],
-       [2919, 1329],
-       [3713, 2261],
-       [2819, 3022]], dtype=int64))</t>
-        </is>
+      <c r="U109" t="n">
+        <v>0.958895653698288</v>
       </c>
     </row>
     <row r="110">
@@ -8379,13 +7839,8 @@
       <c r="T110" t="n">
         <v>71.24863999999999</v>
       </c>
-      <c r="U110" t="inlineStr">
-        <is>
-          <t>(0.9221736039376568, array([[2062, 1774],
-       [3090, 1453],
-       [3386, 2401],
-       [2358, 2722]], dtype=int64))</t>
-        </is>
+      <c r="U110" t="n">
+        <v>0.9221736039376568</v>
       </c>
     </row>
     <row r="111">
@@ -8451,13 +7906,8 @@
       <c r="T111" t="n">
         <v>31.547192</v>
       </c>
-      <c r="U111" t="inlineStr">
-        <is>
-          <t>(0.753836825228226, array([[1967, 1838],
-       [2624,  758],
-       [4057, 1629],
-       [3399, 2709]], dtype=int64))</t>
-        </is>
+      <c r="U111" t="n">
+        <v>0.7542211236367233</v>
       </c>
     </row>
     <row r="112">
@@ -8523,13 +7973,8 @@
       <c r="T112" t="n">
         <v>58.89546666666666</v>
       </c>
-      <c r="U112" t="inlineStr">
-        <is>
-          <t>(0.6858984726615991, array([[2572, 1513],
-       [3371, 1385],
-       [3459, 1933],
-       [2660, 2061]], dtype=int64))</t>
-        </is>
+      <c r="U112" t="n">
+        <v>0.684423382004901</v>
       </c>
     </row>
     <row r="113">
@@ -8595,13 +8040,8 @@
       <c r="T113" t="n">
         <v>59.34085866666667</v>
       </c>
-      <c r="U113" t="inlineStr">
-        <is>
-          <t>(0.9637714137815512, array([[2104, 1568],
-       [2950,  999],
-       [3539, 1876],
-       [2694, 2444]], dtype=int64))</t>
-        </is>
+      <c r="U113" t="n">
+        <v>0.9640193499285361</v>
       </c>
     </row>
     <row r="114">
@@ -8667,13 +8107,8 @@
       <c r="T114" t="n">
         <v>59.76681066666666</v>
       </c>
-      <c r="U114" t="inlineStr">
-        <is>
-          <t>(0.7912560822840621, array([[2256, 2517],
-       [3015, 1961],
-       [3718, 2920],
-       [2959, 3476]], dtype=int64))</t>
-        </is>
+      <c r="U114" t="n">
+        <v>0.7912560822840621</v>
       </c>
     </row>
     <row r="115">
@@ -8739,13 +8174,8 @@
       <c r="T115" t="n">
         <v>35.4024</v>
       </c>
-      <c r="U115" t="inlineStr">
-        <is>
-          <t>(0.9003383482850029, array([[1733, 2356],
-       [2196, 1499],
-       [3148, 2012],
-       [2685, 2870]], dtype=int64))</t>
-        </is>
+      <c r="U115" t="n">
+        <v>0.9007335880949791</v>
       </c>
     </row>
     <row r="116">
@@ -8811,13 +8241,8 @@
       <c r="T116" t="n">
         <v>26.14265866666667</v>
       </c>
-      <c r="U116" t="inlineStr">
-        <is>
-          <t>(0.8570481054282094, array([[  23, 3909],
-       [  66, 2447],
-       [1319, 2484],
-       [1276, 3946]], dtype=int64))</t>
-        </is>
+      <c r="U116" t="n">
+        <v>0.8570481054282094</v>
       </c>
     </row>
     <row r="117">
@@ -8883,13 +8308,8 @@
       <c r="T117" t="n">
         <v>34.11153333333333</v>
       </c>
-      <c r="U117" t="inlineStr">
-        <is>
-          <t>(0.6730519441570973, array([[1258, 2115],
-       [1760,  690],
-       [3876, 1435],
-       [3375, 2860]], dtype=int64))</t>
-        </is>
+      <c r="U117" t="n">
+        <v>0.6686223890721767</v>
       </c>
     </row>
     <row r="118">
@@ -8955,13 +8375,8 @@
       <c r="T118" t="n">
         <v>28.135544</v>
       </c>
-      <c r="U118" t="inlineStr">
-        <is>
-          <t>(0.7461588758057693, array([[2121, 1886],
-       [2763, 1019],
-       [3924, 1878],
-       [3283, 2745]], dtype=int64))</t>
-        </is>
+      <c r="U118" t="n">
+        <v>0.7465742663190291</v>
       </c>
     </row>
     <row r="119">
@@ -9027,13 +8442,8 @@
       <c r="T119" t="n">
         <v>52.18878933333333</v>
       </c>
-      <c r="U119" t="inlineStr">
-        <is>
-          <t>(0.8832521759737265, array([[1973, 1348],
-       [3037,  838],
-       [3487, 1778],
-       [2423, 2288]], dtype=int64))</t>
-        </is>
+      <c r="U119" t="n">
+        <v>0.8832521759737265</v>
       </c>
     </row>
     <row r="120">
@@ -9099,13 +8509,8 @@
       <c r="T120" t="n">
         <v>60.870224</v>
       </c>
-      <c r="U120" t="inlineStr">
-        <is>
-          <t>(0.9500274076081913, array([[2551, 2486],
-       [3034, 1654],
-       [3910, 2162],
-       [3427, 2994]], dtype=int64))</t>
-        </is>
+      <c r="U120" t="n">
+        <v>0.9500274076081913</v>
       </c>
     </row>
     <row r="121">
@@ -9171,13 +8576,8 @@
       <c r="T121" t="n">
         <v>72.40114666666666</v>
       </c>
-      <c r="U121" t="inlineStr">
-        <is>
-          <t>(0.8884167117185933, array([[1412, 2685],
-       [2098, 1049],
-       [3938, 1822],
-       [3252, 3457]], dtype=int64))</t>
-        </is>
+      <c r="U121" t="n">
+        <v>0.8885890640650879</v>
       </c>
     </row>
     <row r="122">
@@ -9243,13 +8643,8 @@
       <c r="T122" t="n">
         <v>66.99020266666666</v>
       </c>
-      <c r="U122" t="inlineStr">
-        <is>
-          <t>(0.6950579082297214, array([[2538, 1719],
-       [4240, 1562],
-       [4349, 2745],
-       [2647, 2902]], dtype=int64))</t>
-        </is>
+      <c r="U122" t="n">
+        <v>0.7857214063443816</v>
       </c>
     </row>
     <row r="123">
@@ -9315,13 +8710,8 @@
       <c r="T123" t="n">
         <v>35.460672</v>
       </c>
-      <c r="U123" t="inlineStr">
-        <is>
-          <t>(0.969179462332034, array([[2596, 1640],
-       [3058, 1159],
-       [3554, 1636],
-       [3092, 2117]], dtype=int64))</t>
-        </is>
+      <c r="U123" t="n">
+        <v>0.969179462332034</v>
       </c>
     </row>
     <row r="124">
@@ -9387,13 +8777,8 @@
       <c r="T124" t="n">
         <v>49.00270933333334</v>
       </c>
-      <c r="U124" t="inlineStr">
-        <is>
-          <t>(0.6200077396016714, array([[2176, 2257],
-       [2317, 1518],
-       [3509, 1745],
-       [3368, 2484]], dtype=int64))</t>
-        </is>
+      <c r="U124" t="n">
+        <v>0.6184104285885537</v>
       </c>
     </row>
     <row r="125">
@@ -9459,13 +8844,8 @@
       <c r="T125" t="n">
         <v>39.66750133333333</v>
       </c>
-      <c r="U125" t="inlineStr">
-        <is>
-          <t>(0.8658994907986438, array([[2729, 1767],
-       [3587, 1628],
-       [3707, 2371],
-       [2850, 2510]], dtype=int64))</t>
-        </is>
+      <c r="U125" t="n">
+        <v>0.8668839913075392</v>
       </c>
     </row>
     <row r="126">
@@ -9531,13 +8911,8 @@
       <c r="T126" t="n">
         <v>41.34861866666667</v>
       </c>
-      <c r="U126" t="inlineStr">
-        <is>
-          <t>(0.9651904387334862, array([[2616, 1451],
-       [3257,  770],
-       [3914, 1389],
-       [3273, 2070]], dtype=int64))</t>
-        </is>
+      <c r="U126" t="n">
+        <v>0.9651904387334862</v>
       </c>
     </row>
     <row r="127">
@@ -9603,13 +8978,8 @@
       <c r="T127" t="n">
         <v>52.13469866666667</v>
       </c>
-      <c r="U127" t="inlineStr">
-        <is>
-          <t>(0.984326639799061, array([[2399, 2553],
-       [2837, 2299],
-       [3095, 2744],
-       [2657, 2998]], dtype=int64))</t>
-        </is>
+      <c r="U127" t="n">
+        <v>0.984326639799061</v>
       </c>
     </row>
     <row r="128">
@@ -9675,13 +9045,8 @@
       <c r="T128" t="n">
         <v>26.78416533333333</v>
       </c>
-      <c r="U128" t="inlineStr">
-        <is>
-          <t>(0.8101865125590416, array([[2635, 1410],
-       [3331, 1358],
-       [3396, 2217],
-       [2700, 2269]], dtype=int64))</t>
-        </is>
+      <c r="U128" t="n">
+        <v>0.8101865125590416</v>
       </c>
     </row>
     <row r="129">
@@ -9747,13 +9112,8 @@
       <c r="T129" t="n">
         <v>34.945792</v>
       </c>
-      <c r="U129" t="inlineStr">
-        <is>
-          <t>(0.7890837939401463, array([[2446, 3015],
-       [2842, 1725],
-       [3861, 2038],
-       [3464, 3328]], dtype=int64))</t>
-        </is>
+      <c r="U129" t="n">
+        <v>0.7892555963012582</v>
       </c>
     </row>
     <row r="130">
@@ -9819,13 +9179,8 @@
       <c r="T130" t="n">
         <v>57.03722666666667</v>
       </c>
-      <c r="U130" t="inlineStr">
-        <is>
-          <t>(0.9857988165680474, array([[2316, 1710],
-       [3161, 1710],
-       [3161, 2543],
-       [2316, 2543]], dtype=int64))</t>
-        </is>
+      <c r="U130" t="n">
+        <v>0.9857988165680474</v>
       </c>
     </row>
     <row r="131">
@@ -9891,13 +9246,8 @@
       <c r="T131" t="n">
         <v>41.244312</v>
       </c>
-      <c r="U131" t="inlineStr">
-        <is>
-          <t>(0.8439169642834791, array([[1904, 2862],
-       [2438, 1780],
-       [3720, 2413],
-       [3185, 3495]], dtype=int64))</t>
-        </is>
+      <c r="U131" t="n">
+        <v>0.8444465067573651</v>
       </c>
     </row>
     <row r="132">
@@ -9963,13 +9313,8 @@
       <c r="T132" t="n">
         <v>42.25391466666667</v>
       </c>
-      <c r="U132" t="inlineStr">
-        <is>
-          <t>(0.833792982828481, array([[2847, 2608],
-       [2919, 1525],
-       [3822, 1585],
-       [3750, 2668]], dtype=int64))</t>
-        </is>
+      <c r="U132" t="n">
+        <v>0.833792982828481</v>
       </c>
     </row>
     <row r="133">
@@ -10035,13 +9380,8 @@
       <c r="T133" t="n">
         <v>34.364488</v>
       </c>
-      <c r="U133" t="inlineStr">
-        <is>
-          <t>(0.7851095020508974, array([[2259, 2292],
-       [2529, 1426],
-       [3632, 1770],
-       [3362, 2636]], dtype=int64))</t>
-        </is>
+      <c r="U133" t="n">
+        <v>0.7851095020508974</v>
       </c>
     </row>
     <row r="134">
@@ -10107,13 +9447,8 @@
       <c r="T134" t="n">
         <v>40.901712</v>
       </c>
-      <c r="U134" t="inlineStr">
-        <is>
-          <t>(0.8377579189795478, array([[2361, 2034],
-       [3681, 1223],
-       [4361, 2329],
-       [3041, 3141]], dtype=int64))</t>
-        </is>
+      <c r="U134" t="n">
+        <v>0.8380411237264525</v>
       </c>
     </row>
     <row r="135">
@@ -10179,13 +9514,8 @@
       <c r="T135" t="n">
         <v>50.91778666666666</v>
       </c>
-      <c r="U135" t="inlineStr">
-        <is>
-          <t>(0.7158113180744468, array([[2691, 1557],
-       [3662, 1331],
-       [3824, 2026],
-       [2853, 2252]], dtype=int64))</t>
-        </is>
+      <c r="U135" t="n">
+        <v>0.7131733926440971</v>
       </c>
     </row>
     <row r="136">
@@ -10251,13 +9581,8 @@
       <c r="T136" t="n">
         <v>47.44738133333333</v>
       </c>
-      <c r="U136" t="inlineStr">
-        <is>
-          <t>(0.6738931125912325, array([[1977, 2345],
-       [3421, 1933],
-       [3699, 2906],
-       [2255, 3318]], dtype=int64))</t>
-        </is>
+      <c r="U136" t="n">
+        <v>0.6738931125912325</v>
       </c>
     </row>
     <row r="137">
@@ -10323,13 +9648,8 @@
       <c r="T137" t="n">
         <v>46.09085333333334</v>
       </c>
-      <c r="U137" t="inlineStr">
-        <is>
-          <t>(0.8241021792545831, array([[2198, 2005],
-       [3270, 1623],
-       [3733, 2924],
-       [2660, 3305]], dtype=int64))</t>
-        </is>
+      <c r="U137" t="n">
+        <v>0.8248651225923652</v>
       </c>
     </row>
     <row r="138">
@@ -10395,13 +9715,8 @@
       <c r="T138" t="n">
         <v>46.59665066666667</v>
       </c>
-      <c r="U138" t="inlineStr">
-        <is>
-          <t>(0.8882405077984863, array([[2279, 1952],
-       [3503, 1528],
-       [3979, 2905],
-       [2756, 3329]], dtype=int64))</t>
-        </is>
+      <c r="U138" t="n">
+        <v>0.8884398756371207</v>
       </c>
     </row>
     <row r="139">
@@ -10467,13 +9782,8 @@
       <c r="T139" t="n">
         <v>64.008912</v>
       </c>
-      <c r="U139" t="inlineStr">
-        <is>
-          <t>(0.8809670145039596, array([[2307, 2332],
-       [2445, 1882],
-       [2955, 2037],
-       [2818, 2488]], dtype=int64))</t>
-        </is>
+      <c r="U139" t="n">
+        <v>0.8830296207051465</v>
       </c>
     </row>
     <row r="140">
@@ -10539,13 +9849,8 @@
       <c r="T140" t="n">
         <v>30.77593866666667</v>
       </c>
-      <c r="U140" t="inlineStr">
-        <is>
-          <t>(0.7489459828139958, array([[1854, 2178],
-       [2151, 1050],
-       [3657, 1447],
-       [3360, 2575]], dtype=int64))</t>
-        </is>
+      <c r="U140" t="n">
+        <v>0.7489459828139958</v>
       </c>
     </row>
     <row r="141">
@@ -10611,13 +9916,8 @@
       <c r="T141" t="n">
         <v>43.42771466666667</v>
       </c>
-      <c r="U141" t="inlineStr">
-        <is>
-          <t>(0.6318293712569086, array([[2761, 2477],
-       [4442, 1667],
-       [4954, 2729],
-       [3273, 3539]], dtype=int64))</t>
-        </is>
+      <c r="U141" t="n">
+        <v>0.6601147507788785</v>
       </c>
     </row>
     <row r="142">
@@ -10683,13 +9983,8 @@
       <c r="T142" t="n">
         <v>44.43474133333333</v>
       </c>
-      <c r="U142" t="inlineStr">
-        <is>
-          <t>(0.8377066935147247, array([[2822, 1637],
-       [3899, 1178],
-       [4284, 2080],
-       [3207, 2539]], dtype=int64))</t>
-        </is>
+      <c r="U142" t="n">
+        <v>0.8377066935147247</v>
       </c>
     </row>
     <row r="143">
@@ -10755,13 +10050,8 @@
       <c r="T143" t="n">
         <v>46.012032</v>
       </c>
-      <c r="U143" t="inlineStr">
-        <is>
-          <t>(0.8331038403154448, array([[2017, 1916],
-       [2512,  963],
-       [3656, 1557],
-       [3161, 2510]], dtype=int64))</t>
-        </is>
+      <c r="U143" t="n">
+        <v>0.8331038403154448</v>
       </c>
     </row>
     <row r="144">
@@ -10827,13 +10117,8 @@
       <c r="T144" t="n">
         <v>43.71890933333334</v>
       </c>
-      <c r="U144" t="inlineStr">
-        <is>
-          <t>(0.6234405607903093, array([[2652, 1617],
-       [3590, 1300],
-       [3787, 1885],
-       [2850, 2202]], dtype=int64))</t>
-        </is>
+      <c r="U144" t="n">
+        <v>0.6240376183941498</v>
       </c>
     </row>
     <row r="145">
@@ -10899,13 +10184,8 @@
       <c r="T145" t="n">
         <v>51.56782933333334</v>
       </c>
-      <c r="U145" t="inlineStr">
-        <is>
-          <t>(0.9194253201681456, array([[2182, 2448],
-       [2444, 1344],
-       [3460, 1586],
-       [3197, 2690]], dtype=int64))</t>
-        </is>
+      <c r="U145" t="n">
+        <v>0.9196127625331444</v>
       </c>
     </row>
     <row r="146">
@@ -10971,13 +10251,8 @@
       <c r="T146" t="n">
         <v>49.76656</v>
       </c>
-      <c r="U146" t="inlineStr">
-        <is>
-          <t>(0.41505850167974323, array([[1667, 1589],
-       [1907, 1097],
-       [3092, 1676],
-       [2851, 2168]], dtype=int64))</t>
-        </is>
+      <c r="U146" t="n">
+        <v>0.4153414273250103</v>
       </c>
     </row>
     <row r="147">
@@ -11043,13 +10318,8 @@
       <c r="T147" t="n">
         <v>68.44891200000001</v>
       </c>
-      <c r="U147" t="inlineStr">
-        <is>
-          <t>(0.5152806090169156, array([[2414, 1642],
-       [3990, 1418],
-       [4106, 2230],
-       [2530, 2454]], dtype=int64))</t>
-        </is>
+      <c r="U147" t="n">
+        <v>0.5152806090169156</v>
       </c>
     </row>
     <row r="148">
@@ -11115,13 +10385,8 @@
       <c r="T148" t="n">
         <v>38.92284</v>
       </c>
-      <c r="U148" t="inlineStr">
-        <is>
-          <t>(0.6542946751968977, array([[2329, 1522],
-       [2914, 1265],
-       [3307, 2159],
-       [2722, 2416]], dtype=int64))</t>
-        </is>
+      <c r="U148" t="n">
+        <v>0.6542946751968977</v>
       </c>
     </row>
     <row r="149">
@@ -11187,13 +10452,8 @@
       <c r="T149" t="n">
         <v>42.766216</v>
       </c>
-      <c r="U149" t="inlineStr">
-        <is>
-          <t>(0.712482240190723, array([[2793, 2285],
-       [2814, 1652],
-       [3265, 1667],
-       [3244, 2300]], dtype=int64))</t>
-        </is>
+      <c r="U149" t="n">
+        <v>0.712482240190723</v>
       </c>
     </row>
     <row r="150">
@@ -11259,13 +10519,8 @@
       <c r="T150" t="n">
         <v>25.47427466666667</v>
       </c>
-      <c r="U150" t="inlineStr">
-        <is>
-          <t>(0.7738993253501172, array([[3718, 1998],
-       [4357, 1381],
-       [4834, 1876],
-       [4195, 2493]], dtype=int64))</t>
-        </is>
+      <c r="U150" t="n">
+        <v>0.7738993253501172</v>
       </c>
     </row>
     <row r="151">
@@ -11331,13 +10586,8 @@
       <c r="T151" t="n">
         <v>27.856768</v>
       </c>
-      <c r="U151" t="inlineStr">
-        <is>
-          <t>(0.9138271008846776, array([[2575, 1296],
-       [3670,  248],
-       [4816, 1446],
-       [3721, 2493]], dtype=int64))</t>
-        </is>
+      <c r="U151" t="n">
+        <v>0.9142255057134479</v>
       </c>
     </row>
     <row r="152">
@@ -11403,13 +10653,8 @@
       <c r="T152" t="n">
         <v>27.19453333333333</v>
       </c>
-      <c r="U152" t="inlineStr">
-        <is>
-          <t>(0.6941425774048618, array([[2684, 1744],
-       [2921, 1226],
-       [3666, 1567],
-       [3429, 2084]], dtype=int64))</t>
-        </is>
+      <c r="U152" t="n">
+        <v>0.6928992512955047</v>
       </c>
     </row>
     <row r="153">
@@ -11475,13 +10720,8 @@
       <c r="T153" t="n">
         <v>57.44512533333333</v>
       </c>
-      <c r="U153" t="inlineStr">
-        <is>
-          <t>(0.9518004837020029, array([[1293, 1013],
-       [3406,  441],
-       [3951, 2452],
-       [1838, 3024]], dtype=int64))</t>
-        </is>
+      <c r="U153" t="n">
+        <v>0.9518004837020029</v>
       </c>
     </row>
     <row r="154">
@@ -11547,13 +10787,8 @@
       <c r="T154" t="n">
         <v>86.539536</v>
       </c>
-      <c r="U154" t="inlineStr">
-        <is>
-          <t>(0.4429407957906277, array([[2190,  867],
-       [3386,  696],
-       [3773, 3396],
-       [2577, 3567]], dtype=int64))</t>
-        </is>
+      <c r="U154" t="n">
+        <v>0.4426008601266778</v>
       </c>
     </row>
     <row r="155">
@@ -11619,13 +10854,8 @@
       <c r="T155" t="n">
         <v>68.219168</v>
       </c>
-      <c r="U155" t="inlineStr">
-        <is>
-          <t>(0.5005852361946254, array([[2041, 2580],
-       [3830, -245],
-       [5245,  650],
-       [3456, 3476]], dtype=int64))</t>
-        </is>
+      <c r="U155" t="n">
+        <v>0.5007117191972243</v>
       </c>
     </row>
     <row r="156">
@@ -11691,13 +10921,8 @@
       <c r="T156" t="n">
         <v>54.56769066666666</v>
       </c>
-      <c r="U156" t="inlineStr">
-        <is>
-          <t>(0.6255612752874432, array([[2357, 2343],
-       [2458,  981],
-       [3311, 1045],
-       [3209, 2407]], dtype=int64))</t>
-        </is>
+      <c r="U156" t="n">
+        <v>0.6249564285724051</v>
       </c>
     </row>
     <row r="157">
@@ -11763,13 +10988,8 @@
       <c r="T157" t="n">
         <v>52.26304</v>
       </c>
-      <c r="U157" t="inlineStr">
-        <is>
-          <t>(0.9583789139810158, array([[2263, 2684],
-       [2419, 1697],
-       [3365, 1846],
-       [3209, 2833]], dtype=int64))</t>
-        </is>
+      <c r="U157" t="n">
+        <v>0.9583789139810158</v>
       </c>
     </row>
     <row r="158">
@@ -11835,13 +11055,8 @@
       <c r="T158" t="n">
         <v>60.53091733333333</v>
       </c>
-      <c r="U158" t="inlineStr">
-        <is>
-          <t>(0.8842448086589791, array([[2332,  926],
-       [3432,  735],
-       [3648, 1979],
-       [2548, 2170]], dtype=int64))</t>
-        </is>
+      <c r="U158" t="n">
+        <v>0.8842448086589791</v>
       </c>
     </row>
     <row r="159">
@@ -11907,13 +11122,8 @@
       <c r="T159" t="n">
         <v>48.30657066666667</v>
       </c>
-      <c r="U159" t="inlineStr">
-        <is>
-          <t>(0.7943055594319675, array([[2371, 1482],
-       [3645, 1255],
-       [3825, 2267],
-       [2551, 2494]], dtype=int64))</t>
-        </is>
+      <c r="U159" t="n">
+        <v>0.7943055594319675</v>
       </c>
     </row>
     <row r="160">
@@ -11979,13 +11189,8 @@
       <c r="T160" t="n">
         <v>40.06544</v>
       </c>
-      <c r="U160" t="inlineStr">
-        <is>
-          <t>(0.8764027528892024, array([[2401, 1478],
-       [3695, 1104],
-       [4023, 2238],
-       [2729, 2612]], dtype=int64))</t>
-        </is>
+      <c r="U160" t="n">
+        <v>0.8764027528892024</v>
       </c>
     </row>
     <row r="161">
@@ -12051,13 +11256,8 @@
       <c r="T161" t="n">
         <v>46.52319466666667</v>
       </c>
-      <c r="U161" t="inlineStr">
-        <is>
-          <t>(0.8304540805794198, array([[2524, 1283],
-       [3366,  923],
-       [3799, 1935],
-       [2958, 2296]], dtype=int64))</t>
-        </is>
+      <c r="U161" t="n">
+        <v>0.8314445792673752</v>
       </c>
     </row>
     <row r="162">
@@ -12123,13 +11323,8 @@
       <c r="T162" t="n">
         <v>71.22851733333333</v>
       </c>
-      <c r="U162" t="inlineStr">
-        <is>
-          <t>(0.6847912262994035, array([[2511, 2660],
-       [2833, 2003],
-       [3284, 2224],
-       [2961, 2881]], dtype=int64))</t>
-        </is>
+      <c r="U162" t="n">
+        <v>0.6852036400470782</v>
       </c>
     </row>
     <row r="163">
@@ -12195,13 +11390,8 @@
       <c r="T163" t="n">
         <v>41.84029066666667</v>
       </c>
-      <c r="U163" t="inlineStr">
-        <is>
-          <t>(0.6549766339356375, array([[1786, 3342],
-       [1926, 2760],
-       [2815, 2972],
-       [2675, 3554]], dtype=int64))</t>
-        </is>
+      <c r="U163" t="n">
+        <v>0.6549766339356375</v>
       </c>
     </row>
     <row r="164">
@@ -12267,13 +11457,8 @@
       <c r="T164" t="n">
         <v>85.18154133333333</v>
       </c>
-      <c r="U164" t="inlineStr">
-        <is>
-          <t>(0.9848032652034218, array([[2731, 2299],
-       [2965, 1824],
-       [3433, 2054],
-       [3199, 2529]], dtype=int64))</t>
-        </is>
+      <c r="U164" t="n">
+        <v>0.9848032652034218</v>
       </c>
     </row>
     <row r="165">
@@ -12339,13 +11524,8 @@
       <c r="T165" t="n">
         <v>37.164144</v>
       </c>
-      <c r="U165" t="inlineStr">
-        <is>
-          <t>(0.714390386402238, array([[2420, 1313],
-       [3273, 1216],
-       [3409, 2409],
-       [2556, 2507]], dtype=int64))</t>
-        </is>
+      <c r="U165" t="n">
+        <v>0.7149815258267617</v>
       </c>
     </row>
     <row r="166">
@@ -12411,13 +11591,8 @@
       <c r="T166" t="n">
         <v>23.17853866666667</v>
       </c>
-      <c r="U166" t="inlineStr">
-        <is>
-          <t>(0.773535702346509, array([[2440, 1555],
-       [3116, 1371],
-       [3258, 1894],
-       [2582, 2078]], dtype=int64))</t>
-        </is>
+      <c r="U166" t="n">
+        <v>0.773535702346509</v>
       </c>
     </row>
     <row r="167">
@@ -12483,13 +11658,8 @@
       <c r="T167" t="n">
         <v>39.646144</v>
       </c>
-      <c r="U167" t="inlineStr">
-        <is>
-          <t>(0.9441263227228803, array([[2216, 1894],
-       [2570, 1194],
-       [3231, 1528],
-       [2877, 2228]], dtype=int64))</t>
-        </is>
+      <c r="U167" t="n">
+        <v>0.9441263227228803</v>
       </c>
     </row>
     <row r="168">
@@ -12555,13 +11725,8 @@
       <c r="T168" t="n">
         <v>30.24366666666667</v>
       </c>
-      <c r="U168" t="inlineStr">
-        <is>
-          <t>(0.5444398519567942, array([[2277, 1630],
-       [2384,  982],
-       [3573, 1178],
-       [3467, 1826]], dtype=int64))</t>
-        </is>
+      <c r="U168" t="n">
+        <v>0.5499187707013042</v>
       </c>
     </row>
     <row r="169">
@@ -12627,13 +11792,8 @@
       <c r="T169" t="n">
         <v>70.681504</v>
       </c>
-      <c r="U169" t="inlineStr">
-        <is>
-          <t>(0.7057316737201017, array([[1758, 1668],
-       [2766,  940],
-       [3281, 1651],
-       [2273, 2380]], dtype=int64))</t>
-        </is>
+      <c r="U169" t="n">
+        <v>0.7060641371707909</v>
       </c>
     </row>
     <row r="170">
@@ -12699,13 +11859,8 @@
       <c r="T170" t="n">
         <v>24.110872</v>
       </c>
-      <c r="U170" t="inlineStr">
-        <is>
-          <t>(0.9167652684028362, array([[2261,  697],
-       [3098,  342],
-       [3484, 1254],
-       [2648, 1609]], dtype=int64))</t>
-        </is>
+      <c r="U170" t="n">
+        <v>0.9173007764570755</v>
       </c>
     </row>
     <row r="171">
@@ -12771,13 +11926,8 @@
       <c r="T171" t="n">
         <v>52.28736</v>
       </c>
-      <c r="U171" t="inlineStr">
-        <is>
-          <t>(0.7260908657670215, array([[3087, 1681],
-       [3406, 1631],
-       [3475, 2068],
-       [3157, 2119]], dtype=int64))</t>
-        </is>
+      <c r="U171" t="n">
+        <v>0.7262468541405268</v>
       </c>
     </row>
     <row r="172">
@@ -12843,13 +11993,8 @@
       <c r="T172" t="n">
         <v>43.55556</v>
       </c>
-      <c r="U172" t="inlineStr">
-        <is>
-          <t>(0.8630946107646352, array([[2608, 2000],
-       [3207, 1887],
-       [3338, 2581],
-       [2739, 2694]], dtype=int64))</t>
-        </is>
+      <c r="U172" t="n">
+        <v>0.8644860268587721</v>
       </c>
     </row>
     <row r="173">
@@ -12915,13 +12060,8 @@
       <c r="T173" t="n">
         <v>29.25066933333333</v>
       </c>
-      <c r="U173" t="inlineStr">
-        <is>
-          <t>(0.7441840548535965, array([[2758, 2148],
-       [2784, 1476],
-       [3687, 1511],
-       [3660, 2183]], dtype=int64))</t>
-        </is>
+      <c r="U173" t="n">
+        <v>0.7450078529465168</v>
       </c>
     </row>
     <row r="174">
@@ -12987,13 +12127,8 @@
       <c r="T174" t="n">
         <v>68.85675733333333</v>
       </c>
-      <c r="U174" t="inlineStr">
-        <is>
-          <t>(0.8072356692661349, array([[1974,  918],
-       [3116,  578],
-       [3390, 1500],
-       [2248, 1840]], dtype=int64))</t>
-        </is>
+      <c r="U174" t="n">
+        <v>0.8072356692661349</v>
       </c>
     </row>
     <row r="175">
@@ -13059,13 +12194,8 @@
       <c r="T175" t="n">
         <v>33.77013066666667</v>
       </c>
-      <c r="U175" t="inlineStr">
-        <is>
-          <t>(0.9173938526295233, array([[2044, 2115],
-       [2929, 1755],
-       [3259, 2567],
-       [2374, 2927]], dtype=int64))</t>
-        </is>
+      <c r="U175" t="n">
+        <v>0.9177843215466389</v>
       </c>
     </row>
     <row r="176">
@@ -13131,13 +12261,8 @@
       <c r="T176" t="n">
         <v>37.67774133333333</v>
       </c>
-      <c r="U176" t="inlineStr">
-        <is>
-          <t>(0.9473722018580473, array([[2611, 2372],
-       [2818, 1739],
-       [3486, 1958],
-       [3278, 2591]], dtype=int64))</t>
-        </is>
+      <c r="U176" t="n">
+        <v>0.9486544242227209</v>
       </c>
     </row>
     <row r="177">
@@ -13203,13 +12328,8 @@
       <c r="T177" t="n">
         <v>38.171568</v>
       </c>
-      <c r="U177" t="inlineStr">
-        <is>
-          <t>(0.7780096022807969, array([[2733, 1923],
-       [2809, 1324],
-       [3579, 1421],
-       [3503, 2020]], dtype=int64))</t>
-        </is>
+      <c r="U177" t="n">
+        <v>0.7780096022807969</v>
       </c>
     </row>
     <row r="178">
@@ -13275,13 +12395,8 @@
       <c r="T178" t="n">
         <v>41.965352</v>
       </c>
-      <c r="U178" t="inlineStr">
-        <is>
-          <t>(0.7850522946858017, array([[3039, 2174],
-       [3434, 1448],
-       [4004, 1758],
-       [3610, 2484]], dtype=int64))</t>
-        </is>
+      <c r="U178" t="n">
+        <v>0.7855060660539027</v>
       </c>
     </row>
     <row r="179">
@@ -13347,13 +12462,8 @@
       <c r="T179" t="n">
         <v>48.27762666666667</v>
       </c>
-      <c r="U179" t="inlineStr">
-        <is>
-          <t>(0.826074585224947, array([[2586, 1567],
-       [3328, 1454],
-       [3421, 2068],
-       [2679, 2180]], dtype=int64))</t>
-        </is>
+      <c r="U179" t="n">
+        <v>0.8262396052732985</v>
       </c>
     </row>
     <row r="180">
@@ -13419,13 +12529,8 @@
       <c r="T180" t="n">
         <v>62.02737066666667</v>
       </c>
-      <c r="U180" t="inlineStr">
-        <is>
-          <t>(0.5832182886765894, array([[2556, 1834],
-       [2885, 1802],
-       [2941, 2366],
-       [2612, 2398]], dtype=int64))</t>
-        </is>
+      <c r="U180" t="n">
+        <v>0.5832182886765894</v>
       </c>
     </row>
     <row r="181">
@@ -13491,13 +12596,8 @@
       <c r="T181" t="n">
         <v>31.31382933333333</v>
       </c>
-      <c r="U181" t="inlineStr">
-        <is>
-          <t>(0.925026554254775, array([[2348, 2022],
-       [2513, 1317],
-       [3166, 1469],
-       [3002, 2175]], dtype=int64))</t>
-        </is>
+      <c r="U181" t="n">
+        <v>0.9259806437496146</v>
       </c>
     </row>
     <row r="182">
@@ -13563,13 +12663,8 @@
       <c r="T182" t="n">
         <v>48.81990933333334</v>
       </c>
-      <c r="U182" t="inlineStr">
-        <is>
-          <t>(0.9875964546357379, array([[2747, 1683],
-       [3258, 1158],
-       [3790, 1675],
-       [3279, 2200]], dtype=int64))</t>
-        </is>
+      <c r="U182" t="n">
+        <v>0.9875964546357379</v>
       </c>
     </row>
     <row r="183">
@@ -13635,13 +12730,8 @@
       <c r="T183" t="n">
         <v>57.62716266666666</v>
       </c>
-      <c r="U183" t="inlineStr">
-        <is>
-          <t>(0.8092699503871142, array([[1888, 2547],
-       [2452, 2334],
-       [2715, 3031],
-       [2151, 3244]], dtype=int64))</t>
-        </is>
+      <c r="U183" t="n">
+        <v>0.8092699503871142</v>
       </c>
     </row>
     <row r="184">
@@ -13707,13 +12797,8 @@
       <c r="T184" t="n">
         <v>37.43929333333333</v>
       </c>
-      <c r="U184" t="inlineStr">
-        <is>
-          <t>(0.8446601941747572, array([[2704, 1944],
-       [3487, 1944],
-       [3487, 2871],
-       [2704, 2871]], dtype=int64))</t>
-        </is>
+      <c r="U184" t="n">
+        <v>0.8446601941747572</v>
       </c>
     </row>
     <row r="185">
@@ -13779,13 +12864,8 @@
       <c r="T185" t="n">
         <v>56.48178666666666</v>
       </c>
-      <c r="U185" t="inlineStr">
-        <is>
-          <t>(0.7123814922785041, array([[2937, 2083],
-       [3830, 1772],
-       [4052, 2408],
-       [3159, 2719]], dtype=int64))</t>
-        </is>
+      <c r="U185" t="n">
+        <v>0.7109612586445162</v>
       </c>
     </row>
     <row r="186">
@@ -13851,13 +12931,8 @@
       <c r="T186" t="n">
         <v>29.07110133333333</v>
       </c>
-      <c r="U186" t="inlineStr">
-        <is>
-          <t>(0.8891428571428571, array([[2766, 2629],
-       [2766, 1851],
-       [3641, 1851],
-       [3641, 2629]], dtype=int64))</t>
-        </is>
+      <c r="U186" t="n">
+        <v>0.9011328527291452</v>
       </c>
     </row>
     <row r="187">
@@ -13923,13 +12998,8 @@
       <c r="T187" t="n">
         <v>52.09096</v>
       </c>
-      <c r="U187" t="inlineStr">
-        <is>
-          <t>(0.43957043342297414, array([[2600, 1444],
-       [2998, 1385],
-       [3131, 2288],
-       [2734, 2346]], dtype=int64))</t>
-        </is>
+      <c r="U187" t="n">
+        <v>0.4399767462665262</v>
       </c>
     </row>
     <row r="188">
@@ -13995,13 +13065,8 @@
       <c r="T188" t="n">
         <v>58.010464</v>
       </c>
-      <c r="U188" t="inlineStr">
-        <is>
-          <t>(0.9302709416562868, array([[2167, 2115],
-       [2756, 1643],
-       [3195, 2192],
-       [2606, 2663]], dtype=int64))</t>
-        </is>
+      <c r="U188" t="n">
+        <v>0.9310418108280122</v>
       </c>
     </row>
     <row r="189">
@@ -14067,13 +13132,8 @@
       <c r="T189" t="n">
         <v>35.38577066666667</v>
       </c>
-      <c r="U189" t="inlineStr">
-        <is>
-          <t>(0.6031764488452556, array([[2660, 2458],
-       [3296, 1380],
-       [3946, 1764],
-       [3310, 2842]], dtype=int64))</t>
-        </is>
+      <c r="U189" t="n">
+        <v>0.6031764488452556</v>
       </c>
     </row>
     <row r="190">
@@ -14139,13 +13199,8 @@
       <c r="T190" t="n">
         <v>54.20159466666667</v>
       </c>
-      <c r="U190" t="inlineStr">
-        <is>
-          <t>(0.9525636972960276, array([[2634, 1814],
-       [3436, 1565],
-       [3674, 2329],
-       [2872, 2579]], dtype=int64))</t>
-        </is>
+      <c r="U190" t="n">
+        <v>0.9529006526703171</v>
       </c>
     </row>
     <row r="191">
@@ -14211,13 +13266,8 @@
       <c r="T191" t="n">
         <v>28.12924</v>
       </c>
-      <c r="U191" t="inlineStr">
-        <is>
-          <t>(0.9114084686987906, array([[2630, 2360],
-       [2706, 1547],
-       [3447, 1616],
-       [3371, 2429]], dtype=int64))</t>
-        </is>
+      <c r="U191" t="n">
+        <v>0.9114084686987906</v>
       </c>
     </row>
     <row r="192">
@@ -14283,13 +13333,8 @@
       <c r="T192" t="n">
         <v>30.16310666666667</v>
       </c>
-      <c r="U192" t="inlineStr">
-        <is>
-          <t>(0.9456297119162951, array([[2405, 2203],
-       [2424, 1265],
-       [3311, 1283],
-       [3292, 2221]], dtype=int64))</t>
-        </is>
+      <c r="U192" t="n">
+        <v>0.9456297119162951</v>
       </c>
     </row>
     <row r="193">
@@ -14355,13 +13400,8 @@
       <c r="T193" t="n">
         <v>47.546496</v>
       </c>
-      <c r="U193" t="inlineStr">
-        <is>
-          <t>(0.9699565174047596, array([[3016, 2423],
-       [3077, 1657],
-       [3820, 1716],
-       [3760, 2482]], dtype=int64))</t>
-        </is>
+      <c r="U193" t="n">
+        <v>0.9700559139768462</v>
       </c>
     </row>
     <row r="194">
@@ -14427,13 +13467,8 @@
       <c r="T194" t="n">
         <v>46.636784</v>
       </c>
-      <c r="U194" t="inlineStr">
-        <is>
-          <t>(0.6566659103480385, array([[2834, 1698],
-       [3343, 1594],
-       [3502, 2369],
-       [2993, 2473]], dtype=int64))</t>
-        </is>
+      <c r="U194" t="n">
+        <v>0.6566659103480385</v>
       </c>
     </row>
     <row r="195">
@@ -14499,13 +13534,8 @@
       <c r="T195" t="n">
         <v>50.02877866666667</v>
       </c>
-      <c r="U195" t="inlineStr">
-        <is>
-          <t>(0.6853988690210843, array([[2348, 2398],
-       [2901, 1616],
-       [3437, 1996],
-       [2884, 2777]], dtype=int64))</t>
-        </is>
+      <c r="U195" t="n">
+        <v>0.6859835254948921</v>
       </c>
     </row>
     <row r="196">
@@ -14571,13 +13601,8 @@
       <c r="T196" t="n">
         <v>75.35854933333333</v>
       </c>
-      <c r="U196" t="inlineStr">
-        <is>
-          <t>(0.7485529746548677, array([[2423, 1957],
-       [3199, 1732],
-       [3367, 2313],
-       [2592, 2538]], dtype=int64))</t>
-        </is>
+      <c r="U196" t="n">
+        <v>0.7498272545217946</v>
       </c>
     </row>
     <row r="197">
@@ -14643,13 +13668,8 @@
       <c r="T197" t="n">
         <v>35.9966</v>
       </c>
-      <c r="U197" t="inlineStr">
-        <is>
-          <t>(0.7576549661376324, array([[2086, 2531],
-       [2711, 1609],
-       [3410, 2083],
-       [2785, 3006]], dtype=int64))</t>
-        </is>
+      <c r="U197" t="n">
+        <v>0.7582180933981779</v>
       </c>
     </row>
     <row r="198">
@@ -14715,13 +13735,8 @@
       <c r="T198" t="n">
         <v>45.155856</v>
       </c>
-      <c r="U198" t="inlineStr">
-        <is>
-          <t>(0.9572619587969877, array([[2473, 1243],
-       [3366,  664],
-       [3920, 1519],
-       [3027, 2098]], dtype=int64))</t>
-        </is>
+      <c r="U198" t="n">
+        <v>0.9572619587969877</v>
       </c>
     </row>
     <row r="199">
@@ -14787,13 +13802,8 @@
       <c r="T199" t="n">
         <v>36.771824</v>
       </c>
-      <c r="U199" t="inlineStr">
-        <is>
-          <t>(0.8960848695914926, array([[2471, 2060],
-       [2680, 1049],
-       [3586, 1236],
-       [3377, 2247]], dtype=int64))</t>
-        </is>
+      <c r="U199" t="n">
+        <v>0.8960848695914926</v>
       </c>
     </row>
     <row r="200">
@@ -14859,13 +13869,8 @@
       <c r="T200" t="n">
         <v>32.858576</v>
       </c>
-      <c r="U200" t="inlineStr">
-        <is>
-          <t>(0.7367579989400834, array([[2144, 2834],
-       [2277, 1861],
-       [2994, 1959],
-       [2861, 2931]], dtype=int64))</t>
-        </is>
+      <c r="U200" t="n">
+        <v>0.7375020567354351</v>
       </c>
     </row>
     <row r="201">
@@ -14931,13 +13936,8 @@
       <c r="T201" t="n">
         <v>91.003136</v>
       </c>
-      <c r="U201" t="inlineStr">
-        <is>
-          <t>(0.951931112670104, array([[2755, 1432],
-       [3281,  816],
-       [3868, 1316],
-       [3342, 1932]], dtype=int64))</t>
-        </is>
+      <c r="U201" t="n">
+        <v>0.951931112670104</v>
       </c>
     </row>
     <row r="202">
@@ -15003,13 +14003,8 @@
       <c r="T202" t="n">
         <v>44.71149333333334</v>
       </c>
-      <c r="U202" t="inlineStr">
-        <is>
-          <t>(0.8125979905151278, array([[2473, 2407],
-       [3125, 1896],
-       [3540, 2427],
-       [2888, 2937]], dtype=int64))</t>
-        </is>
+      <c r="U202" t="n">
+        <v>0.8132031779593987</v>
       </c>
     </row>
     <row r="203">
@@ -15075,13 +14070,8 @@
       <c r="T203" t="n">
         <v>55.48130133333333</v>
       </c>
-      <c r="U203" t="inlineStr">
-        <is>
-          <t>(0.7284767528434594, array([[2504, 2409],
-       [2645, 1904],
-       [3337, 2097],
-       [3197, 2602]], dtype=int64))</t>
-        </is>
+      <c r="U203" t="n">
+        <v>0.7294535392558241</v>
       </c>
     </row>
     <row r="204">
@@ -15147,13 +14137,8 @@
       <c r="T204" t="n">
         <v>58.03114666666666</v>
       </c>
-      <c r="U204" t="inlineStr">
-        <is>
-          <t>(0.7324973534983009, array([[2351, 2173],
-       [2469, 1661],
-       [3167, 1821],
-       [3050, 2334]], dtype=int64))</t>
-        </is>
+      <c r="U204" t="n">
+        <v>0.7337233367338828</v>
       </c>
     </row>
     <row r="205">
@@ -15219,13 +14204,8 @@
       <c r="T205" t="n">
         <v>55.16712</v>
       </c>
-      <c r="U205" t="inlineStr">
-        <is>
-          <t>(0.8199067084661141, array([[2812, 2209],
-       [3595, 2132],
-       [3658, 2774],
-       [2875, 2851]], dtype=int64))</t>
-        </is>
+      <c r="U205" t="n">
+        <v>0.8199067084661141</v>
       </c>
     </row>
     <row r="206">
@@ -15291,13 +14271,8 @@
       <c r="T206" t="n">
         <v>53.950112</v>
       </c>
-      <c r="U206" t="inlineStr">
-        <is>
-          <t>(0.942993739943042, array([[2850, 2165],
-       [3656, 1951],
-       [3858, 2712],
-       [3052, 2925]], dtype=int64))</t>
-        </is>
+      <c r="U206" t="n">
+        <v>0.9432833756285637</v>
       </c>
     </row>
     <row r="207">
@@ -15363,13 +14338,8 @@
       <c r="T207" t="n">
         <v>70.958544</v>
       </c>
-      <c r="U207" t="inlineStr">
-        <is>
-          <t>(0.9456322704215387, array([[2292, 1835],
-       [2769, 1557],
-       [3032, 2009],
-       [2555, 2286]], dtype=int64))</t>
-        </is>
+      <c r="U207" t="n">
+        <v>0.9401916069692146</v>
       </c>
     </row>
     <row r="208">
@@ -15435,13 +14405,8 @@
       <c r="T208" t="n">
         <v>48.02062933333333</v>
       </c>
-      <c r="U208" t="inlineStr">
-        <is>
-          <t>(0.9325383615555682, array([[2490, 2262],
-       [2681, 1722],
-       [3260, 1927],
-       [3069, 2467]], dtype=int64))</t>
-        </is>
+      <c r="U208" t="n">
+        <v>0.9325383615555682</v>
       </c>
     </row>
     <row r="209">
@@ -15507,13 +14472,8 @@
       <c r="T209" t="n">
         <v>45.95682133333333</v>
       </c>
-      <c r="U209" t="inlineStr">
-        <is>
-          <t>(0.7379563731652221, array([[2920, 2604],
-       [3169, 1784],
-       [4280, 2122],
-       [4031, 2942]], dtype=int64))</t>
-        </is>
+      <c r="U209" t="n">
+        <v>0.7385648081997001</v>
       </c>
     </row>
     <row r="210">
@@ -15579,13 +14539,8 @@
       <c r="T210" t="n">
         <v>34.39473066666667</v>
       </c>
-      <c r="U210" t="inlineStr">
-        <is>
-          <t>(0.8097869185447385, array([[1633, 1755],
-       [2127,  983],
-       [3081, 1592],
-       [2586, 2365]], dtype=int64))</t>
-        </is>
+      <c r="U210" t="n">
+        <v>0.8100044670323809</v>
       </c>
     </row>
     <row r="211">
@@ -15651,13 +14606,8 @@
       <c r="T211" t="n">
         <v>30.97504</v>
       </c>
-      <c r="U211" t="inlineStr">
-        <is>
-          <t>(0.5041880900003409, array([[2242, 1640],
-       [2525, 1225],
-       [3347, 1787],
-       [3063, 2201]], dtype=int64))</t>
-        </is>
+      <c r="U211" t="n">
+        <v>0.50489281484977</v>
       </c>
     </row>
     <row r="212">
@@ -15723,13 +14673,8 @@
       <c r="T212" t="n">
         <v>29.485512</v>
       </c>
-      <c r="U212" t="inlineStr">
-        <is>
-          <t>(0.7880457523379308, array([[1847, 2209],
-       [2588, 1541],
-       [3436, 2481],
-       [2695, 3149]], dtype=int64))</t>
-        </is>
+      <c r="U212" t="n">
+        <v>0.7880457523379308</v>
       </c>
     </row>
     <row r="213">
@@ -15795,13 +14740,8 @@
       <c r="T213" t="n">
         <v>29.324936</v>
       </c>
-      <c r="U213" t="inlineStr">
-        <is>
-          <t>(0.7603952973716022, array([[2897, 2352],
-       [2991, 1129],
-       [3921, 1200],
-       [3827, 2423]], dtype=int64))</t>
-        </is>
+      <c r="U213" t="n">
+        <v>0.7603952973716022</v>
       </c>
     </row>
     <row r="214">
@@ -15867,13 +14807,8 @@
       <c r="T214" t="n">
         <v>29.151352</v>
       </c>
-      <c r="U214" t="inlineStr">
-        <is>
-          <t>(0.6668461665024835, array([[1928, 2385],
-       [1995, 1408],
-       [3460, 1509],
-       [3393, 2487]], dtype=int64))</t>
-        </is>
+      <c r="U214" t="n">
+        <v>0.6668775532938958</v>
       </c>
     </row>
     <row r="215">
@@ -15939,13 +14874,8 @@
       <c r="T215" t="n">
         <v>39.71856</v>
       </c>
-      <c r="U215" t="inlineStr">
-        <is>
-          <t>(0.5553279462851484, array([[1921, 2205],
-       [1936, 1391],
-       [3400, 1418],
-       [3385, 2231]], dtype=int64))</t>
-        </is>
+      <c r="U215" t="n">
+        <v>0.5553348102272287</v>
       </c>
     </row>
     <row r="216">
@@ -16011,13 +14941,8 @@
       <c r="T216" t="n">
         <v>34.41254933333333</v>
       </c>
-      <c r="U216" t="inlineStr">
-        <is>
-          <t>(0.7788116008994862, array([[3336, 2210],
-       [4240, 1696],
-       [4641, 2401],
-       [3736, 2915]], dtype=int64))</t>
-        </is>
+      <c r="U216" t="n">
+        <v>0.7794627317747885</v>
       </c>
     </row>
     <row r="217">
@@ -16083,13 +15008,8 @@
       <c r="T217" t="n">
         <v>58.01289066666666</v>
       </c>
-      <c r="U217" t="inlineStr">
-        <is>
-          <t>(0.6806373964371867, array([[2208, 1924],
-       [2890, 1664],
-       [3272, 2666],
-       [2589, 2926]], dtype=int64))</t>
-        </is>
+      <c r="U217" t="n">
+        <v>0.6808633170661057</v>
       </c>
     </row>
     <row r="218">
@@ -16155,13 +15075,8 @@
       <c r="T218" t="n">
         <v>58.71042133333334</v>
       </c>
-      <c r="U218" t="inlineStr">
-        <is>
-          <t>(0.46034994430642273, array([[3334, 2498],
-       [3570, 1849],
-       [3869, 1957],
-       [3633, 2606]], dtype=int64))</t>
-        </is>
+      <c r="U218" t="n">
+        <v>0.4633155920328848</v>
       </c>
     </row>
     <row r="219">
@@ -16227,13 +15142,8 @@
       <c r="T219" t="n">
         <v>50.23104</v>
       </c>
-      <c r="U219" t="inlineStr">
-        <is>
-          <t>(0.5630585898709036, array([[2592, 1880],
-       [3159, 1880],
-       [3159, 2887],
-       [2592, 2887]], dtype=int64))</t>
-        </is>
+      <c r="U219" t="n">
+        <v>0.5630585898709036</v>
       </c>
     </row>
     <row r="220">
@@ -16299,13 +15209,8 @@
       <c r="T220" t="n">
         <v>39.15983733333334</v>
       </c>
-      <c r="U220" t="inlineStr">
-        <is>
-          <t>(0.5315922763799609, array([[2978, 1727],
-       [3088, 1356],
-       [3784, 1563],
-       [3674, 1933]], dtype=int64))</t>
-        </is>
+      <c r="U220" t="n">
+        <v>0.53180059351749</v>
       </c>
     </row>
     <row r="221">
@@ -16371,13 +15276,8 @@
       <c r="T221" t="n">
         <v>30.98941866666667</v>
       </c>
-      <c r="U221" t="inlineStr">
-        <is>
-          <t>(0.30956349195717153, array([[3330,  858],
-       [3672,  755],
-       [4004, 1860],
-       [3662, 1963]], dtype=int64))</t>
-        </is>
+      <c r="U221" t="n">
+        <v>0.3095634919571715</v>
       </c>
     </row>
     <row r="222">
@@ -16443,13 +15343,8 @@
       <c r="T222" t="n">
         <v>32.23806133333333</v>
       </c>
-      <c r="U222" t="inlineStr">
-        <is>
-          <t>(0.8979031180182171, array([[2968, 2100],
-       [3412, 1355],
-       [4242, 1849],
-       [3798, 2594]], dtype=int64))</t>
-        </is>
+      <c r="U222" t="n">
+        <v>0.8979031180182171</v>
       </c>
     </row>
     <row r="223">
@@ -16515,13 +15410,8 @@
       <c r="T223" t="n">
         <v>31.89033066666667</v>
       </c>
-      <c r="U223" t="inlineStr">
-        <is>
-          <t>(0.9090791868361587, array([[2775, 2160],
-       [2884, 1290],
-       [3841, 1410],
-       [3732, 2280]], dtype=int64))</t>
-        </is>
+      <c r="U223" t="n">
+        <v>0.9090791868361587</v>
       </c>
     </row>
     <row r="224">
@@ -16587,13 +15477,8 @@
       <c r="T224" t="n">
         <v>43.03270133333334</v>
       </c>
-      <c r="U224" t="inlineStr">
-        <is>
-          <t>(0.553048345425141, array([[2607, 2261],
-       [2793, 1994],
-       [3276, 2330],
-       [3090, 2597]], dtype=int64))</t>
-        </is>
+      <c r="U224" t="n">
+        <v>0.553048345425141</v>
       </c>
     </row>
     <row r="225">
@@ -16659,13 +15544,8 @@
       <c r="T225" t="n">
         <v>33.92915466666667</v>
       </c>
-      <c r="U225" t="inlineStr">
-        <is>
-          <t>(0.4676848444784646, array([[2860, 1718],
-       [3367, 1648],
-       [3515, 2732],
-       [3008, 2801]], dtype=int64))</t>
-        </is>
+      <c r="U225" t="n">
+        <v>0.4681087731168927</v>
       </c>
     </row>
     <row r="226">
@@ -16731,13 +15611,8 @@
       <c r="T226" t="n">
         <v>46.395168</v>
       </c>
-      <c r="U226" t="inlineStr">
-        <is>
-          <t>(0.8262506207517989, array([[2681, 1759],
-       [2992, 1265],
-       [3589, 1640],
-       [3279, 2134]], dtype=int64))</t>
-        </is>
+      <c r="U226" t="n">
+        <v>0.8272432859722905</v>
       </c>
     </row>
     <row r="227">
@@ -16803,13 +15678,8 @@
       <c r="T227" t="n">
         <v>73.214032</v>
       </c>
-      <c r="U227" t="inlineStr">
-        <is>
-          <t>(0.9322789803668677, array([[2199, 2064],
-       [2948, 1101],
-       [3846, 1799],
-       [3097, 2762]], dtype=int64))</t>
-        </is>
+      <c r="U227" t="n">
+        <v>0.9322789803668677</v>
       </c>
     </row>
     <row r="228">
@@ -16875,13 +15745,8 @@
       <c r="T228" t="n">
         <v>42.71416</v>
       </c>
-      <c r="U228" t="inlineStr">
-        <is>
-          <t>(0.4572781122886502, array([[1767, 2167],
-       [1864, 1647],
-       [2999, 1859],
-       [2902, 2378]], dtype=int64))</t>
-        </is>
+      <c r="U228" t="n">
+        <v>0.4573506742381376</v>
       </c>
     </row>
     <row r="229">
@@ -16947,13 +15812,8 @@
       <c r="T229" t="n">
         <v>74.78309333333333</v>
       </c>
-      <c r="U229" t="inlineStr">
-        <is>
-          <t>(0.5970262565193875, array([[1600, 2036],
-       [1856, 1658],
-       [2488, 2086],
-       [2232, 2463]], dtype=int64))</t>
-        </is>
+      <c r="U229" t="n">
+        <v>0.5574018508665284</v>
       </c>
     </row>
     <row r="230">
@@ -17019,13 +15879,8 @@
       <c r="T230" t="n">
         <v>61.71795733333333</v>
       </c>
-      <c r="U230" t="inlineStr">
-        <is>
-          <t>(0.41760943776586446, array([[2239, 1918],
-       [2367, 1438],
-       [3516, 1746],
-       [3387, 2226]], dtype=int64))</t>
-        </is>
+      <c r="U230" t="n">
+        <v>0.4179487925954684</v>
       </c>
     </row>
     <row r="231">
@@ -17091,13 +15946,8 @@
       <c r="T231" t="n">
         <v>60.57999466666666</v>
       </c>
-      <c r="U231" t="inlineStr">
-        <is>
-          <t>(0.48234703813057295, array([[2028, 2019],
-       [2202, 1440],
-       [3402, 1802],
-       [3227, 2381]], dtype=int64))</t>
-        </is>
+      <c r="U231" t="n">
+        <v>0.4824652074786217</v>
       </c>
     </row>
     <row r="232">
@@ -17163,13 +16013,8 @@
       <c r="T232" t="n">
         <v>48.22080533333333</v>
       </c>
-      <c r="U232" t="inlineStr">
-        <is>
-          <t>(0.54363429041721, array([[1561, 2754],
-       [1803, 1216],
-       [4631, 1660],
-       [4390, 3198]], dtype=int64))</t>
-        </is>
+      <c r="U232" t="n">
+        <v>0.5438218995496763</v>
       </c>
     </row>
     <row r="233">
@@ -17235,13 +16080,8 @@
       <c r="T233" t="n">
         <v>49.7144</v>
       </c>
-      <c r="U233" t="inlineStr">
-        <is>
-          <t>(0.7927664542342664, array([[1204, 2442],
-       [3562,  265],
-       [5289, 2135],
-       [2930, 4312]], dtype=int64))</t>
-        </is>
+      <c r="U233" t="n">
+        <v>0.7929479705141201</v>
       </c>
     </row>
     <row r="234">
@@ -17307,13 +16147,8 @@
       <c r="T234" t="n">
         <v>36.58720059998172</v>
       </c>
-      <c r="U234" t="inlineStr">
-        <is>
-          <t>(0.6164190614013437, array([[2111,  843],
-       [2511,  614],
-       [2882, 1261],
-       [2483, 1490]], dtype=int64))</t>
-        </is>
+      <c r="U234" t="n">
+        <v>0.6168306088384395</v>
       </c>
     </row>
     <row r="235">
@@ -17379,13 +16214,8 @@
       <c r="T235" t="n">
         <v>85.77860800000001</v>
       </c>
-      <c r="U235" t="inlineStr">
-        <is>
-          <t>(0.7884718711488758, array([[1828, 2364],
-       [3351, 1647],
-       [3916, 2848],
-       [2393, 3565]], dtype=int64))</t>
-        </is>
+      <c r="U235" t="n">
+        <v>0.7925184513534747</v>
       </c>
     </row>
     <row r="236">
@@ -17451,13 +16281,8 @@
       <c r="T236" t="n">
         <v>41.569992</v>
       </c>
-      <c r="U236" t="inlineStr">
-        <is>
-          <t>(0.6370612206189764, array([[2141, 1210],
-       [2622,  615],
-       [3556, 1370],
-       [3075, 1965]], dtype=int64))</t>
-        </is>
+      <c r="U236" t="n">
+        <v>0.6370612206189764</v>
       </c>
     </row>
     <row r="237">
@@ -17523,13 +16348,8 @@
       <c r="T237" t="n">
         <v>69.109792</v>
       </c>
-      <c r="U237" t="inlineStr">
-        <is>
-          <t>(0.5224742523173281, array([[2468, 2525],
-       [2489, 1886],
-       [3712, 1927],
-       [3691, 2566]], dtype=int64))</t>
-        </is>
+      <c r="U237" t="n">
+        <v>0.5224742523173281</v>
       </c>
     </row>
     <row r="238">
@@ -17595,13 +16415,8 @@
       <c r="T238" t="n">
         <v>45.32157866666667</v>
       </c>
-      <c r="U238" t="inlineStr">
-        <is>
-          <t>(0.9900737702402014, array([[2117, 2682],
-       [2655, 1503],
-       [3846, 2046],
-       [3308, 3225]], dtype=int64))</t>
-        </is>
+      <c r="U238" t="n">
+        <v>0.9900737702402014</v>
       </c>
     </row>
     <row r="239">
@@ -17667,13 +16482,8 @@
       <c r="T239" t="n">
         <v>23.66088266666667</v>
       </c>
-      <c r="U239" t="inlineStr">
-        <is>
-          <t>(0.9169483807664355, array([[2612, 1898],
-       [3345, 1429],
-       [3856, 2228],
-       [3123, 2696]], dtype=int64))</t>
-        </is>
+      <c r="U239" t="n">
+        <v>0.9177634354937267</v>
       </c>
     </row>
     <row r="240">
@@ -17739,13 +16549,8 @@
       <c r="T240" t="n">
         <v>22.210764</v>
       </c>
-      <c r="U240" t="inlineStr">
-        <is>
-          <t>(0.9473559954612275, array([[2768, 1697],
-       [3292, 1413],
-       [3592, 1965],
-       [3068, 2250]], dtype=int64))</t>
-        </is>
+      <c r="U240" t="n">
+        <v>0.9486811615761119</v>
       </c>
     </row>
     <row r="241">
@@ -17811,13 +16616,8 @@
       <c r="T241" t="n">
         <v>52.74612266666666</v>
       </c>
-      <c r="U241" t="inlineStr">
-        <is>
-          <t>(0.9820059273730166, array([[2476, 2670],
-       [2497, 1796],
-       [3387, 1818],
-       [3365, 2692]], dtype=int64))</t>
-        </is>
+      <c r="U241" t="n">
+        <v>0.9831098702787999</v>
       </c>
     </row>
     <row r="242">
@@ -17883,13 +16683,8 @@
       <c r="T242" t="n">
         <v>38.15652266666667</v>
       </c>
-      <c r="U242" t="inlineStr">
-        <is>
-          <t>(0.5646371958117212, array([[1411,  913],
-       [2049,  318],
-       [3102, 1447],
-       [2464, 2041]], dtype=int64))</t>
-        </is>
+      <c r="U242" t="n">
+        <v>0.5649047264810314</v>
       </c>
     </row>
     <row r="243">
@@ -17955,13 +16750,8 @@
       <c r="T243" t="n">
         <v>48.133952</v>
       </c>
-      <c r="U243" t="inlineStr">
-        <is>
-          <t>(0.9181202316439604, array([[1690, 1651],
-       [2485,  626],
-       [3426, 1356],
-       [2632, 2381]], dtype=int64))</t>
-        </is>
+      <c r="U243" t="n">
+        <v>0.9185540494712814</v>
       </c>
     </row>
     <row r="244">
@@ -18027,13 +16817,8 @@
       <c r="T244" t="n">
         <v>44.373016</v>
       </c>
-      <c r="U244" t="inlineStr">
-        <is>
-          <t>(0.8172874921962638, array([[2435, 1592],
-       [3419, 1225],
-       [3868, 2429],
-       [2884, 2796]], dtype=int64))</t>
-        </is>
+      <c r="U244" t="n">
+        <v>0.8172874921962638</v>
       </c>
     </row>
     <row r="245">
@@ -18099,13 +16884,8 @@
       <c r="T245" t="n">
         <v>70.29410133333333</v>
       </c>
-      <c r="U245" t="inlineStr">
-        <is>
-          <t>(0.8346311082716826, array([[1601, 2962],
-       [2531, 1807],
-       [3496, 2583],
-       [2566, 3739]], dtype=int64))</t>
-        </is>
+      <c r="U245" t="n">
+        <v>0.8725527405345409</v>
       </c>
     </row>
     <row r="246">
@@ -18171,13 +16951,8 @@
       <c r="T246" t="n">
         <v>60.22644266666666</v>
       </c>
-      <c r="U246" t="inlineStr">
-        <is>
-          <t>(0.7725426482534524, array([[1224, 1720],
-       [2455, 1720],
-       [2455, 2671],
-       [1224, 2671]], dtype=int64))</t>
-        </is>
+      <c r="U246" t="n">
+        <v>0.7725426482534524</v>
       </c>
     </row>
     <row r="247">
@@ -18243,13 +17018,8 @@
       <c r="T247" t="n">
         <v>58.68736</v>
       </c>
-      <c r="U247" t="inlineStr">
-        <is>
-          <t>(0.9309140140134954, array([[2004, 1678],
-       [2850,  947],
-       [3635, 1856],
-       [2789, 2587]], dtype=int64))</t>
-        </is>
+      <c r="U247" t="n">
+        <v>0.9309140140134954</v>
       </c>
     </row>
     <row r="248">
@@ -18315,13 +17085,8 @@
       <c r="T248" t="n">
         <v>45.04216533333334</v>
       </c>
-      <c r="U248" t="inlineStr">
-        <is>
-          <t>(0.6097637200121846, array([[2120, 2329],
-       [2206, 1426],
-       [3687, 1566],
-       [3601, 2469]], dtype=int64))</t>
-        </is>
+      <c r="U248" t="n">
+        <v>0.6097637200121846</v>
       </c>
     </row>
     <row r="249">
@@ -18387,13 +17152,8 @@
       <c r="T249" t="n">
         <v>42.05477866666666</v>
       </c>
-      <c r="U249" t="inlineStr">
-        <is>
-          <t>(0.7998331943286072, array([[2024,  792],
-       [3223,  792],
-       [3223, 1751],
-       [2024, 1751]], dtype=int64))</t>
-        </is>
+      <c r="U249" t="n">
+        <v>0.7998331943286072</v>
       </c>
     </row>
     <row r="250">
@@ -18459,13 +17219,8 @@
       <c r="T250" t="n">
         <v>56.77508266666667</v>
       </c>
-      <c r="U250" t="inlineStr">
-        <is>
-          <t>(0.6349674006940695, array([[2717, 1718],
-       [3598, 1577],
-       [3820, 2962],
-       [2940, 3104]], dtype=int64))</t>
-        </is>
+      <c r="U250" t="n">
+        <v>0.6354861331063454</v>
       </c>
     </row>
   </sheetData>

</xml_diff>